<commit_message>
Table now contains abstracts from all 3 of our best models. Abstracts common to all three retrievings have been marked in gray and their evaluation boxes closed. This way we must only evaluate those abstracts that differ among the models. Moreover a formula has been put in place to check that marks have been given coherently when 2 out of 3 abstracts are the same
</commit_message>
<xml_diff>
--- a/project/evaluation/qualitative_evaluation/qualitative_evaluation_table.xlsx
+++ b/project/evaluation/qualitative_evaluation/qualitative_evaluation_table.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteom/shared-folder/nlpt_group/project/evaluation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteom/shared-folder/nlpt_group/project/evaluation/qualitative_evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A4EA54-8FC0-AD4B-B6BF-13817DE1BFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7119FCC3-8251-E84F-AF41-AD9733DDD04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{BFF5F178-14AB-6B4F-B81C-3E61E0B93405}"/>
+    <workbookView xWindow="28800" yWindow="-5940" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{BFF5F178-14AB-6B4F-B81C-3E61E0B93405}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Correct retrieval" sheetId="1" r:id="rId1"/>
+    <sheet name="Subjective scores" sheetId="2" r:id="rId2"/>
+    <sheet name="Cumulative scores" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="93">
   <si>
     <t>Comparison queries:</t>
   </si>
@@ -171,12 +172,6 @@
     <t>3)</t>
   </si>
   <si>
-    <t>model 2</t>
-  </si>
-  <si>
-    <t>model 3</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -280,13 +275,55 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>The aim of this study was to assess the cognitive and behavioral development of preterm and low birth weight newborns living in a disadvantageous socioeconomic environment at school age This crosssectional study included children aged 67 from a historical birth cohort of preterm gestational age 37 weeks and low birth weight 2500 g infants The Wechsler Intelligence Scale for Children III WISCIII was administered by a psychologist while the parents completed the Child Behavior Checklist The results were compared to the tests reference The perinatal information and followup data were collected from the hospital files The demographic data were collected from the parents The current performance was compared with the results from the Denver II and Bayley II tests which were administered during the first years of life The total intelligence quotient varied from 70 to 140 mean 987158 The borderline intelligence quotient was observed in 93 of the children The Child Behavior Checklist indicated a predominance of social competence problems 278 CI 192 to 379 compared with behavioral problems 155 CI 89 to 242 Both the Child Behavior Checklist domains such as schooling social and attention problems and the cognitive scores were significantly associated with maternal education and family income The results of the Denver and Bayley tests were associated with the cognitive performance p0001 and the Child Behavior Checklist social profile including aggressive and externalizing behavior p0001 Our data suggest that even lowrisk preterm newborns are at risk for developing disturbances in early school age such as mild cognitive deficits and behavioral disorders This risk might increase under unfavorable socioeconomic conditions</t>
+  </si>
+  <si>
+    <t>Cognitive impairment is common among individuals diagnosed with autism spectrum disorder ASD and attentiondeficit hyperactivity disorder ADHD It has been suggested that some aspects of intelligence are preserved or even superior in people with ASD compared with controls but consistent evidence is lacking Few studies have examined the genetic overlap between cognitive ability and ASDADHD The aim of this study was to examine the polygenic overlap between ASDADHD and cognitive ability in individuals from the general population Polygenic risk for ADHD and ASD was calculated from genomewide association studies of ASD and ADHD conducted by the Psychiatric Genetics Consortium Risk scores were created in three independent cohorts Generation Scotland Scottish Family Health Study GSSFHS n9863 the Lothian Birth Cohorts 1936 and 1921 n1522 and the Brisbane Adolescent Twin Sample BATS n921 We report that polygenic risk for ASD is positively correlated with general cognitive ability beta007 P6 107 r20003 logical memory and verbal intelligence in GSSFHS This was replicated in BATS as a positive association with fullscale intelligent quotient IQ beta007 P003 r20005 We did not find consistent evidence that polygenic risk for ADHD was associated with cognitive function however a negative correlation with IQ at age 11 years beta008 Z33 P0001 was observed in the Lothian Birth Cohorts These findings are in individuals from the general population suggesting that the relationship between genetic risk for ASD and intelligence is partly independent of clinical state These data suggest that common genetic variation relevant for ASD influences general cognitive ability</t>
+  </si>
+  <si>
+    <t>A metaanalysis of published randomized controlled trials investigating the longterm effect of dexamethasone on the nervous system of preterm infants Online literature retrieval was conducted using The Cochrane Library from January 1993 to June 2013 EMBASE from January 1980 to June 2013 MEDLINE from January 1963 to June 2013 OVID from January 1993 to June 2013 Springer from January 1994 to June 2013 and Chinese Academic Journal Fulltext Database from January 1994 to June 2013 Key words were preterm infants and dexamethasone in English and Chinese Selected studies were randomized controlled trials assessing the effect of intravenous dexamethasone in preterm infants The quality of the included papers was evaluated and those without the development of the nervous system and animal experiments were excluded Quality assessment was performed through bias risk evaluation in accordance with Cochrane Handbook 510 software in the Cochrane Collaboration The homogeneous studies were analyzed and compared using Revman 526 software and then effect model was selected and analyzed Those papers failed to be included in the metaanalysis were subjected to descriptive analysis Nervous system injury in preterm infants Ten randomized controlled trials were screened involving 1038 subjects Among them 512 cases received dexamethasone treatment while 526 cases served as placebo control group and blank control group Metaanalysis results showed that the incidence of cerebral palsy visual impairment and hearing loss in preterm infants after dexamethasone treatment within 7 days after birth was similar to that in the control group RR 147 95CI 097221 RR 146 95CI 097220 RR 080 95CI 054118 P 005 but intelligence quotient was significantly decreased compared with the control group MD 355 95CI 659 to 051 P 002 Preterm infants treated with dexamethasone 7 days after birth demonstrated an incidence of cerebral palsy and visual impairment and changes in intelligence quotient similar to those in the control group RR 126 95CI 089179 RR 137 95CI 073259 RR 053 95CI 032089 RR...</t>
+  </si>
+  <si>
+    <t>Although there is growing evidence on the role of preconception nutrition for birth outcomes very few studies have evaluated the longterm effects of nutrition interventions during the preconception period on offspring cognitive outcomes We evaluate the impact of preconception weekly multiple micronutrients MMs or iron and folic acid IFA supplementation compared with folic acid FA alone on offspring intellectual functioning at age 67 y We followed 1599 offspring born to women who participated in a doubleblinded randomized controlled trial of preconception supplementation in Vietnam Women received weekly supplements containing either 2800 μg FA only 60 mg iron and 2800 μg FA or MMs 15 micronutrients including IFA from baseline until conception followed by daily prenatal IFA supplements until delivery We used the Wechsler Intelligence Scale for Children to measure fullscale IQ FSIQ and 4 related domains of intellectual functioning Verbal Comprehension Index VCI Perceptual Reasoning Index PRI Working Memory Index WMI and Processing Speed Index PSI scores at 67 y Group comparisons were done using ANOVA tests for all children and the subgroup born to women who consumed the supplements 26 wk before conception perprotocol analyses The final sample with data at 67 y n 1321 was similar for baseline maternal and offspring birth characteristics and age at followup by treatment group Compared with the offspring in the FA group those in the MM group had higher FSIQ β 17 95 CI 01 33 WMI β 17 95 CI 02 32 and PSI β 25 95 CI 09 41 Similar findings were observed in the perprotocol analyses There were no significant differences by treatment group for VCI and PRI Preconception supplementation with MMs improved certain domains of intellectual functioning at age 67 y compared with FA These findings suggest the potential for preconception micronutrient interventions to have longterm benefits for offspring cognition</t>
+  </si>
+  <si>
+    <t>Research has shown that cognitive flexibility plays a critical role in students learning and academic achievement However the unique contribution of cognitive flexibility to academic achievement across schooling is not fully understood Thus this study tested whether cognitive flexibility explained a significant amount of variance in academic achievement ie literacy and mathematics outcomes across Grades 2 4 and 6 above and beyond fluid intelligence inhibitory control working memory attention and planning The sample included 243 second graders 284 fourth graders and 203 sixth graders For Grades 4 and 6 we found that better performance on the flexibility score was associated with better academic outcomes after controlling for fluid intelligence attention inhibitory control working memory and planning This effect was not observed for Grade 2 Our findings showed that cognitive flexibility is a key component for school achievement particularly for older students</t>
+  </si>
+  <si>
+    <t>In this article existing research investigating how school performance relates to cognitive selfawareness language and personality processes is reviewed We outline the architecture of the mind involving a general factor igi that underlies distinct mental processes ie executive reasoning language cognizance and personality processes From preschool to adolescence igi shifts from executive to reasoning and cognizance processes personality also changes consolidating in adolescence There are three major trends in the existing literature a All processes are highly predictive of school achievement if measured alone each accounting for 20 of its variance b when measured together cognitive processes executive functions and representational awareness in preschool and fluid intelligence after late primary school dominate as predictors over 50 drastically absorbing selfconcepts and personality dispositions that drop to 35 and c predictive power changes according to the processes forming g at successive levels attention control and representational awareness in preschool 85 fluid intelligence language and working memory in primary school 53 fluid intelligence language selfevaluation and schoolspecific selfconcepts in secondary school 70 Stability and plasticity of personality emerge as predictors in secondary school A theory of educational priorities is proposed arguing that a executive and awareness processes b information management and c reasoning selfevaluation and flexibility in knowledge building must dominate in preschool primary and secondary school respectively PsycInfo Database Record c 2023 APA all rights reserved</t>
+  </si>
+  <si>
+    <t>Anecdotal and biographical reports have long suggested that bipolar disorder is more common in people with exceptional cognitive or creative ability Epidemiological evidence for such a link is sparse We investigated the relationship between intelligence and subsequent risk of hospitalisation for bipolar disorder in a prospective cohort study of 1049607 Swedish men Intelligence was measured on conscription for military service at a mean age of 183 years and data on psychiatric hospital admissions over a mean followup period of 226 years was obtained from national records Risk of hospitalisation with any form of bipolar disorder fell in a stepwise manner as intelligence increased P for linear trend 00001 However when we restricted analyses to men with no psychiatric comorbidity there was a reversedJ shaped association men with the lowest intelligence had the greatest risk of being admitted with pure bipolar disorder but risk was also elevated among men with the highest intelligence P for quadratic trend003 primarily in those with the highest verbal P for quadratic trend0009 or technical ability P for quadratic trend 00001 At least in men high intelligence may indeed be a risk factor for bipolar disorder but only in the minority of cases who have the disorder in a pure form with no psychiatric comorbidity</t>
+  </si>
+  <si>
+    <t>Compared to their termborn peers children born very preterm are at risk for poorer cognitive academic and behavioral outcomes however this finding may have been confounded by lower parental education level in the very preterm children Studies that compare very preterm and termborn children with comparable high parental education level are needed to assess the true effect of very preterm birth on outcomes To compare cognitive academic and behavioral functioning in very preterm and termborn children of highly educated parents To examine whether outcomes differ for children of whom one or both parents are highly educated Crosssectional study with a termborn comparison group 113 very preterm children and 38 termborn children aged 812 years old with highly educated parents Cognitive functioning Intelligence Quotient academic functioning arithmetic facts and reading and parent and teacher rated behavioral functioning attention executive function hyperactivity and emotional conduct and peer problems Parental education was considered high when children had two highly educated parents or one highly and one middle educated parent Very preterm children had significantly poorer cognitive difference of 10 IQ points and behavioral functioning than their termborn peers but did not differ on academic functioning Children with one highly educated parent performed poorer than children with two highly educated parents on most outcome measures Performance of very preterm children should be compared to termborn peers with parents having comparable educational levels for accurate assessment of outcomes The number of highly educated parents also impacts outcomes</t>
+  </si>
+  <si>
+    <t>Two themes are emerging regarding the molecular genetic aetiology of intelligence The first is that intelligence is influenced by many variants and those that are tagged by common single nucleotide polymorphisms account for around 30 of the phenotypic variation The second in line with other polygenic traits such as height and schizophrenia is that these variants are not randomly distributed across the genome but cluster in genes that work together Less clear is whether the very low range of cognitive ability intellectual disability is simply one end of the normal distribution describing individual differences in cognitive ability across a population Here we examined 40 genes with a known association with nonsyndromic autosomal recessive intellectual disability NSARID to determine if they are enriched for common variants associated with the normal range of intelligence differences The current study used the 3511 individuals of the Cognitive Ageing Genetics in England and Scotland CAGES consortium In addition a text mining analysis was used to identify gene sets biologically related to the NSARID set Genebased tests indicated that genes implicated in NSARID were not significantly enriched for quantitative trait loci QTL associated with intelligence These findings suggest that genes in which mutations can have a large and deleterious effect on intelligence are not associated with variation across the range of intelligence differences</t>
+  </si>
+  <si>
+    <t>Multiple Micronutrient MMN supplementation during pregnancy can decrease the proportion of infants born low birth weight and small for gestational age Supplementation could also enhance childrens cognitive function by improving access to key nutrients during fetal brain development and increasing birth weight especially in areas where undernutrition is common We tested the hypothesis that children whose mothers received MMN supplementation during pregnancy would have higher intelligence in early adolescence compared with those receiving Iron and Folic Acid IFA only We followed up children in Nepal whose mothers took part in a doubleblind Randomised Controlled Trial RCT that compared the effects on birth weight and gestational duration of antenatal MMN versus IFA supplementation We assessed childrens Full Scale Intelligence Quotient FSIQ using the Universal Nonverbal Intelligence Test UNIT and their executive function using the counting Stroop test The parent trial was registered as ISRCTN88625934 We identified 813 76 of the 1069 children whose mothers took part in the parent trial We found no differences in FSIQ at 12 years between MMN and IFA groups absolute difference in means diff 125 95 CI 057 to 306 Similarly there were no differences in mean UNIT memory diff 141 95 CI 048 to 330 reasoning diff 117 95 CI 072 to 306 symbolic diff 097 95 CI 067 to 260 or nonsymbolic quotients diff 139 95 CI 060 to 338 Our followup of a doubleblind RCT in Nepal found no evidence of benefit from antenatal MMN compared with IFA for childrens overall intelligence and executive function at 12 years</t>
+  </si>
+  <si>
+    <t>Maternal perinatal depression has been shown to have long lasting effects on childrens development Studies have described the relationship of perinatal depression on childrens cognition especially negative effects on intelligence quotient IQ However a recent examination of the current studies to discern the patterns and strength of associations between perinatal depression and child IQ is not available The purpose of this systematic review is to discern the effects of perinatal depression prenatally and within the first 12 months of the postpartum period on the IQ of the child aged 018 years old We searched the electronic databases PubMed and CINAHL We identified 1633 studies and included 17 studies in the final review based on predetermined criteria After the data was extracted we assessed the strength of the study using the national heart lung and blood institute quality assessment tool for observational cohort and crosssectional studies This systematic review had a total sample of 10757 participants Across the studies we identified a relationship between limited maternal responsiveness due to postpartum depression and a decrease in full IQ scores in younger children Male children were found to be more sensitive to the postpartum depression resulting in a decrease in IQs in comparison to female children Policies should be implemented to identify women suffering from perinatal depression to mitigate the effects of the disorder for both the mother and her child</t>
+  </si>
+  <si>
+    <t>Education mode regular vs special kindergartenschool was significantly correlated with nonverbal IQ at the second assessment time point The results despite the small sample size clearly suggest that children with CIs can achieve intellectual abilities comparable to those of their normalhearing peers by around the third year after initial CI fitting and they continue to improve over the following 2 years We recommend further research focusing on verbal IQ assessed around the age of school entrance to be used as a predictor for further development and for the establishment of an individual educational program...</t>
+  </si>
+  <si>
+    <t>with outcome but they were inconsistent Sex and ethnicity also had predictive effects on measures of educational attainment undergraduate and postgraduate performance Women performed better in assessments but were less likely to be on the Specialist Register Nonwhite participants generally underperformed in undergraduate and postgraduate assessments but were equally likely to be on the Specialist Register There was a suggestion of smaller ethnicity effects in earlier studies The existence of the Academic Backbone concept is strongly supported with attainment at secondary school predicting performance in undergraduate and postgraduate medical assessments and the effects spanning many years The Academic Backbone is conceptualized in terms of the development of more sophisticated underlying structures of knowledge cognitive capital and medical capital The Academic Backbone provides strong support for using measures of educational attainment particularly Alevels in student selection...</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -302,8 +339,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,8 +391,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DDCD"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFE0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -503,11 +572,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,8 +673,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -579,14 +691,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -597,48 +715,64 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -964,7 +1098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53D78E8-53DE-5744-88FC-D2EE8D7F5B8B}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1138,30 +1272,30 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
     </row>
     <row r="26" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
     </row>
     <row r="27" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C27" s="15" t="s">
@@ -1190,7 +1324,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="37" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="5">
@@ -1206,7 +1340,7 @@
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="35"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="9">
         <v>2</v>
       </c>
@@ -1220,7 +1354,7 @@
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="35"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="9">
         <v>3</v>
       </c>
@@ -1234,7 +1368,7 @@
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="35"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="9">
         <v>4</v>
       </c>
@@ -1248,7 +1382,7 @@
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="35"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="9">
         <v>5</v>
       </c>
@@ -1262,7 +1396,7 @@
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="35"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="9">
         <v>6</v>
       </c>
@@ -1276,7 +1410,7 @@
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="35"/>
+      <c r="A34" s="37"/>
       <c r="B34" s="9">
         <v>7</v>
       </c>
@@ -1290,7 +1424,7 @@
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="35"/>
+      <c r="A35" s="37"/>
       <c r="B35" s="9">
         <v>8</v>
       </c>
@@ -1304,7 +1438,7 @@
       <c r="J35" s="4"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="35"/>
+      <c r="A36" s="37"/>
       <c r="B36" s="9">
         <v>9</v>
       </c>
@@ -1318,7 +1452,7 @@
       <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="10">
         <v>10</v>
       </c>
@@ -1350,11 +1484,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03816060-24A7-D946-9AB1-F7E07293AE02}">
-  <dimension ref="A1:N249"/>
+  <dimension ref="A1:O249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
+      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1372,165 +1506,212 @@
     <col min="11" max="11" width="3" style="23" customWidth="1"/>
     <col min="12" max="13" width="3" style="24" customWidth="1"/>
     <col min="14" max="14" width="2.83203125" style="24" customWidth="1"/>
+    <col min="15" max="15" width="54.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C1" s="45" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="F1" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>48</v>
-      </c>
       <c r="I2" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="26" t="s">
-        <v>48</v>
-      </c>
       <c r="L2" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="56"/>
-    </row>
-    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="40"/>
+    </row>
+    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-    </row>
-    <row r="5" spans="1:14" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="28"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="N4" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="O4" t="str">
+        <f>IF(OR( AND(C5=D5,OR(F4&lt;&gt;G4, I4&lt;&gt;J4,L4&lt;&gt;M4)),  AND(D5=E5,OR(G4&lt;&gt;H4,J4&lt;&gt;K4,M4&lt;&gt;N4)), AND(C5=E5, OR(F4&lt;&gt;H4,I4&lt;&gt;K4,L4&lt;&gt;N4) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="32"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-    </row>
-    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C5" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="47"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="55"/>
+    </row>
+    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="38"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="30"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-    </row>
-    <row r="7" spans="1:14" ht="372" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L6" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="N6" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="O6" t="str">
+        <f>IF(OR( AND(C7=D7,OR(F6&lt;&gt;G6, I6&lt;&gt;J6,L6&lt;&gt;M6)),  AND(D7=E7,OR(G6&lt;&gt;H6,J6&lt;&gt;K6,M6&lt;&gt;N6)), AND(C7=E7, OR(F6&lt;&gt;H6,I6&lt;&gt;K6,L6&lt;&gt;N6) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="372" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="32"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-    </row>
-    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C7" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="47"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="55"/>
+    </row>
+    <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="37" t="s">
-        <v>52</v>
-      </c>
+      <c r="C8" s="28"/>
       <c r="D8" s="29"/>
       <c r="E8" s="30"/>
       <c r="F8" s="25"/>
@@ -1542,354 +1723,573 @@
       <c r="L8" s="27"/>
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
-    </row>
-    <row r="9" spans="1:14" ht="255" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O8" t="str">
+        <f>IF(OR( AND(C9=D9,OR(F8&lt;&gt;G8, I8&lt;&gt;J8,L8&lt;&gt;M8)),  AND(D9=E9,OR(G8&lt;&gt;H8,J8&lt;&gt;K8,M8&lt;&gt;N8)), AND(C9=E9, OR(F8&lt;&gt;H8,I8&lt;&gt;K8,L8&lt;&gt;N8) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="255" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="32"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C9" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="47"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="55"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="56"/>
-    </row>
-    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="40"/>
+    </row>
+    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="37" t="s">
-        <v>53</v>
-      </c>
+      <c r="C11" s="28"/>
       <c r="D11" s="29"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-    </row>
-    <row r="12" spans="1:14" ht="404" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="33"/>
+      <c r="F11" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M11" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O11" t="str">
+        <f>IF(OR( AND(C12=D12,OR(F11&lt;&gt;G11, I11&lt;&gt;J11,L11&lt;&gt;M11)),  AND(D12=E12,OR(G11&lt;&gt;H11,J11&lt;&gt;K11,M11&lt;&gt;N11)), AND(C12=E12, OR(F11&lt;&gt;H11,I11&lt;&gt;K11,L11&lt;&gt;N11) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="404" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="32"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-    </row>
-    <row r="13" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="47"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="55"/>
+    </row>
+    <row r="13" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-    </row>
-    <row r="14" spans="1:14" ht="344" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="28"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L13" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M13" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N13" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O13" t="str">
+        <f>IF(OR( AND(C14=D14,OR(F13&lt;&gt;G13, I13&lt;&gt;J13,L13&lt;&gt;M13)),  AND(D14=E14,OR(G13&lt;&gt;H13,J13&lt;&gt;K13,M13&lt;&gt;N13)), AND(C14=E14, OR(F13&lt;&gt;H13,I13&lt;&gt;K13,L13&lt;&gt;N13) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="344" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="32"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-    </row>
-    <row r="15" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="55"/>
+    </row>
+    <row r="15" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-    </row>
-    <row r="16" spans="1:14" ht="340" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M15" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N15" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O15" t="str">
+        <f>IF(OR( AND(C16=D16,OR(F15&lt;&gt;G15, I15&lt;&gt;J15,L15&lt;&gt;M15)),  AND(D16=E16,OR(G15&lt;&gt;H15,J15&lt;&gt;K15,M15&lt;&gt;N15)), AND(C16=E16, OR(F15&lt;&gt;H15,I15&lt;&gt;K15,L15&lt;&gt;N15) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="340" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="32"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C16" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="47"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="55"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>3</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="56"/>
-    </row>
-    <row r="18" spans="1:14" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="40"/>
+    </row>
+    <row r="18" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-    </row>
-    <row r="19" spans="1:14" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K18" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M18" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N18" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O18" t="str">
+        <f>IF(OR( AND(C19=D19,OR(F18&lt;&gt;G18, I18&lt;&gt;J18,L18&lt;&gt;M18)),  AND(D19=E19,OR(G18&lt;&gt;H18,J18&lt;&gt;K18,M18&lt;&gt;N18)), AND(C19=E19, OR(F18&lt;&gt;H18,I18&lt;&gt;K18,L18&lt;&gt;N18) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="32"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-    </row>
-    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C19" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="47"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="55"/>
+    </row>
+    <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-    </row>
-    <row r="21" spans="1:14" ht="404" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="28"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K20" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L20" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M20" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N20" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O20" t="str">
+        <f>IF(OR( AND(C21=D21,OR(F20&lt;&gt;G20, I20&lt;&gt;J20,L20&lt;&gt;M20)),  AND(D21=E21,OR(G20&lt;&gt;H20,J20&lt;&gt;K20,M20&lt;&gt;N20)), AND(C21=E21, OR(F20&lt;&gt;H20,I20&lt;&gt;K20,L20&lt;&gt;N20) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="404" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="32"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-    </row>
-    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C21" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="47"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="55"/>
+    </row>
+    <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-    </row>
-    <row r="23" spans="1:14" ht="372" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K22" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L22" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M22" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N22" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O22" t="str">
+        <f>IF(OR( AND(C23=D23,OR(F22&lt;&gt;G22, I22&lt;&gt;J22,L22&lt;&gt;M22)),  AND(D23=E23,OR(G22&lt;&gt;H22,J22&lt;&gt;K22,M22&lt;&gt;N22)), AND(C23=E23, OR(F22&lt;&gt;H22,I22&lt;&gt;K22,L22&lt;&gt;N22) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="372" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="32"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C23" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="64" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="47"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="55"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>4</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="56"/>
-    </row>
-    <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="40"/>
+    </row>
+    <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B25" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="30"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-    </row>
-    <row r="26" spans="1:14" ht="272" x14ac:dyDescent="0.2">
+      <c r="F25" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H25" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L25" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M25" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N25" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O25" t="str">
+        <f>IF(OR( AND(C26=D26,OR(F25&lt;&gt;G25, I25&lt;&gt;J25,L25&lt;&gt;M25)),  AND(D26=E26,OR(G25&lt;&gt;H25,J25&lt;&gt;K25,M25&lt;&gt;N25)), AND(C26=E26, OR(F25&lt;&gt;H25,I25&lt;&gt;K25,L25&lt;&gt;N25) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="272" x14ac:dyDescent="0.2">
       <c r="B26" s="32"/>
-      <c r="C26" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="52"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
-    </row>
-    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C26" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="55"/>
+    </row>
+    <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-    </row>
-    <row r="28" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="C27" s="66"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I27" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J27" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K27" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L27" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M27" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N27" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O27" t="str">
+        <f>IF(OR( AND(C28=D28,OR(F27&lt;&gt;G27, I27&lt;&gt;J27,L27&lt;&gt;M27)),  AND(D28=E28,OR(G27&lt;&gt;H27,J27&lt;&gt;K27,M27&lt;&gt;N27)), AND(C28=E28, OR(F27&lt;&gt;H27,I27&lt;&gt;K27,L27&lt;&gt;N27) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B28" s="32"/>
-      <c r="C28" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-    </row>
-    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C28" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="47"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="54"/>
+      <c r="N28" s="55"/>
+    </row>
+    <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="32" t="s">
         <v>43</v>
       </c>
@@ -1904,111 +2304,171 @@
       <c r="L29" s="27"/>
       <c r="M29" s="27"/>
       <c r="N29" s="27"/>
-    </row>
-    <row r="30" spans="1:14" ht="255" x14ac:dyDescent="0.2">
+      <c r="O29" t="str">
+        <f>IF(OR( AND(C30=D30,OR(F29&lt;&gt;G29, I29&lt;&gt;J29,L29&lt;&gt;M29)),  AND(D30=E30,OR(G29&lt;&gt;H29,J29&lt;&gt;K29,M29&lt;&gt;N29)), AND(C30=E30, OR(F29&lt;&gt;H29,I29&lt;&gt;K29,L29&lt;&gt;N29) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="404" x14ac:dyDescent="0.2">
       <c r="B30" s="32"/>
       <c r="C30" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="47"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="54"/>
+      <c r="N30" s="55"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>5</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="56"/>
-    </row>
-    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="40"/>
+    </row>
+    <row r="32" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="32" t="s">
         <v>41</v>
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="30"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-    </row>
-    <row r="33" spans="1:14" ht="289" x14ac:dyDescent="0.2">
+      <c r="F32" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H32" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J32" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K32" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L32" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M32" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N32" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O32" t="str">
+        <f>IF(OR( AND(C33=D33,OR(F32&lt;&gt;G32, I32&lt;&gt;J32,L32&lt;&gt;M32)),  AND(D33=E33,OR(G32&lt;&gt;H32,J32&lt;&gt;K32,M32&lt;&gt;N32)), AND(C33=E33, OR(F32&lt;&gt;H32,I32&lt;&gt;K32,L32&lt;&gt;N32) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="289" x14ac:dyDescent="0.2">
       <c r="B33" s="32"/>
-      <c r="C33" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="29"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-    </row>
-    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C33" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="47"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="53"/>
+      <c r="M33" s="54"/>
+      <c r="N33" s="55"/>
+    </row>
+    <row r="34" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" s="32" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="30"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="27"/>
-      <c r="M34" s="27"/>
-      <c r="N34" s="27"/>
-    </row>
-    <row r="35" spans="1:14" ht="306" x14ac:dyDescent="0.2">
+      <c r="F34" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G34" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H34" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J34" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K34" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L34" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M34" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N34" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O34" t="str">
+        <f>IF(OR( AND(C35=D35,OR(F34&lt;&gt;G34, I34&lt;&gt;J34,L34&lt;&gt;M34)),  AND(D35=E35,OR(G34&lt;&gt;H34,J34&lt;&gt;K34,M34&lt;&gt;N34)), AND(C35=E35, OR(F34&lt;&gt;H34,I34&lt;&gt;K34,L34&lt;&gt;N34) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="306" x14ac:dyDescent="0.2">
       <c r="B35" s="32"/>
-      <c r="C35" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="27"/>
-      <c r="M35" s="27"/>
-      <c r="N35" s="27"/>
-    </row>
-    <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C35" s="56" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="47"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="54"/>
+      <c r="N35" s="55"/>
+    </row>
+    <row r="36" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" s="32" t="s">
         <v>43</v>
       </c>
@@ -2023,45 +2483,53 @@
       <c r="L36" s="27"/>
       <c r="M36" s="27"/>
       <c r="N36" s="27"/>
-    </row>
-    <row r="37" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="O36" t="str">
+        <f>IF(OR( AND(C37=D37,OR(F36&lt;&gt;G36, I36&lt;&gt;J36,L36&lt;&gt;M36)),  AND(D37=E37,OR(G36&lt;&gt;H36,J36&lt;&gt;K36,M36&lt;&gt;N36)), AND(C37=E37, OR(F36&lt;&gt;H36,I36&lt;&gt;K36,L36&lt;&gt;N36) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="32"/>
       <c r="C37" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="29"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="27"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F37" s="47"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="54"/>
+      <c r="N37" s="55"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>6</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="43"/>
-      <c r="L38" s="43"/>
-      <c r="M38" s="43"/>
-      <c r="N38" s="56"/>
-    </row>
-    <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="40"/>
+    </row>
+    <row r="39" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B39" s="32" t="s">
         <v>41</v>
       </c>
@@ -2076,58 +2544,92 @@
       <c r="L39" s="27"/>
       <c r="M39" s="27"/>
       <c r="N39" s="27"/>
-    </row>
-    <row r="40" spans="1:14" ht="323" x14ac:dyDescent="0.2">
+      <c r="O39" t="str">
+        <f>IF(OR( AND(C40=D40,OR(F39&lt;&gt;G39, I39&lt;&gt;J39,L39&lt;&gt;M39)),  AND(D40=E40,OR(G39&lt;&gt;H39,J39&lt;&gt;K39,M39&lt;&gt;N39)), AND(C40=E40, OR(F39&lt;&gt;H39,I39&lt;&gt;K39,L39&lt;&gt;N39) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="323" x14ac:dyDescent="0.2">
       <c r="B40" s="32"/>
       <c r="C40" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="D40" s="29"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="26"/>
-      <c r="K40" s="26"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-    </row>
-    <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" s="47"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="54"/>
+      <c r="N40" s="55"/>
+    </row>
+    <row r="41" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B41" s="32" t="s">
         <v>42</v>
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="30"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-    </row>
-    <row r="42" spans="1:14" ht="340" x14ac:dyDescent="0.2">
+      <c r="F41" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H41" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I41" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J41" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K41" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L41" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M41" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N41" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O41" t="str">
+        <f>IF(OR( AND(C42=D42,OR(F41&lt;&gt;G41, I41&lt;&gt;J41,L41&lt;&gt;M41)),  AND(D42=E42,OR(G41&lt;&gt;H41,J41&lt;&gt;K41,M41&lt;&gt;N41)), AND(C42=E42, OR(F41&lt;&gt;H41,I41&lt;&gt;K41,L41&lt;&gt;N41) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="340" x14ac:dyDescent="0.2">
       <c r="B42" s="32"/>
-      <c r="C42" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="29"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="26"/>
-      <c r="K42" s="26"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="27"/>
-      <c r="N42" s="27"/>
-    </row>
-    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C42" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="47"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="51"/>
+      <c r="K42" s="52"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="54"/>
+      <c r="N42" s="55"/>
+    </row>
+    <row r="43" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B43" s="32" t="s">
         <v>43</v>
       </c>
@@ -2142,111 +2644,171 @@
       <c r="L43" s="27"/>
       <c r="M43" s="27"/>
       <c r="N43" s="27"/>
-    </row>
-    <row r="44" spans="1:14" ht="340" x14ac:dyDescent="0.2">
+      <c r="O43" t="str">
+        <f>IF(OR( AND(C44=D44,OR(F43&lt;&gt;G43, I43&lt;&gt;J43,L43&lt;&gt;M43)),  AND(D44=E44,OR(G43&lt;&gt;H43,J43&lt;&gt;K43,M43&lt;&gt;N43)), AND(C44=E44, OR(F43&lt;&gt;H43,I43&lt;&gt;K43,L43&lt;&gt;N43) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B44" s="32"/>
       <c r="C44" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
-      <c r="K44" s="26"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="27"/>
-      <c r="N44" s="27"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F44" s="47"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="54"/>
+      <c r="N44" s="55"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>7</v>
       </c>
-      <c r="B45" s="43" t="s">
+      <c r="B45" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="43"/>
-      <c r="N45" s="56"/>
-    </row>
-    <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="39"/>
+      <c r="M45" s="39"/>
+      <c r="N45" s="40"/>
+    </row>
+    <row r="46" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B46" s="32" t="s">
         <v>41</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="30"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="27"/>
-      <c r="N46" s="27"/>
-    </row>
-    <row r="47" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="F46" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H46" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I46" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J46" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K46" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L46" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M46" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N46" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O46" t="str">
+        <f>IF(OR( AND(C47=D47,OR(F46&lt;&gt;G46, I46&lt;&gt;J46,L46&lt;&gt;M46)),  AND(D47=E47,OR(G46&lt;&gt;H46,J46&lt;&gt;K46,M46&lt;&gt;N46)), AND(C47=E47, OR(F46&lt;&gt;H46,I46&lt;&gt;K46,L46&lt;&gt;N46) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="32"/>
-      <c r="C47" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47" s="29"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="26"/>
-      <c r="L47" s="27"/>
-      <c r="M47" s="27"/>
-      <c r="N47" s="27"/>
-    </row>
-    <row r="48" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C47" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="F47" s="47"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="52"/>
+      <c r="L47" s="53"/>
+      <c r="M47" s="54"/>
+      <c r="N47" s="55"/>
+    </row>
+    <row r="48" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B48" s="32" t="s">
         <v>42</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="30"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
-      <c r="L48" s="27"/>
-      <c r="M48" s="27"/>
-      <c r="N48" s="27"/>
-    </row>
-    <row r="49" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="F48" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H48" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I48" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J48" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K48" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L48" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M48" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N48" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O48" t="str">
+        <f>IF(OR( AND(C49=D49,OR(F48&lt;&gt;G48, I48&lt;&gt;J48,L48&lt;&gt;M48)),  AND(D49=E49,OR(G48&lt;&gt;H48,J48&lt;&gt;K48,M48&lt;&gt;N48)), AND(C49=E49, OR(F48&lt;&gt;H48,I48&lt;&gt;K48,L48&lt;&gt;N48) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="32"/>
-      <c r="C49" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D49" s="29"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
-      <c r="L49" s="27"/>
-      <c r="M49" s="27"/>
-      <c r="N49" s="27"/>
-    </row>
-    <row r="50" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C49" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="E49" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="F49" s="47"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="49"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="51"/>
+      <c r="K49" s="52"/>
+      <c r="L49" s="53"/>
+      <c r="M49" s="54"/>
+      <c r="N49" s="55"/>
+    </row>
+    <row r="50" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B50" s="32" t="s">
         <v>43</v>
       </c>
@@ -2261,111 +2823,171 @@
       <c r="L50" s="27"/>
       <c r="M50" s="27"/>
       <c r="N50" s="27"/>
-    </row>
-    <row r="51" spans="1:14" ht="404" x14ac:dyDescent="0.2">
+      <c r="O50" t="str">
+        <f>IF(OR( AND(C51=D51,OR(F50&lt;&gt;G50, I50&lt;&gt;J50,L50&lt;&gt;M50)),  AND(D51=E51,OR(G50&lt;&gt;H50,J50&lt;&gt;K50,M50&lt;&gt;N50)), AND(C51=E51, OR(F50&lt;&gt;H50,I50&lt;&gt;K50,L50&lt;&gt;N50) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B51" s="32"/>
       <c r="C51" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="D51" s="29"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="26"/>
-      <c r="K51" s="26"/>
-      <c r="L51" s="27"/>
-      <c r="M51" s="27"/>
-      <c r="N51" s="27"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E51" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51" s="47"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="49"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="51"/>
+      <c r="K51" s="52"/>
+      <c r="L51" s="53"/>
+      <c r="M51" s="54"/>
+      <c r="N51" s="55"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>8</v>
       </c>
-      <c r="B52" s="43" t="s">
+      <c r="B52" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="43"/>
-      <c r="J52" s="43"/>
-      <c r="K52" s="43"/>
-      <c r="L52" s="43"/>
-      <c r="M52" s="43"/>
-      <c r="N52" s="56"/>
-    </row>
-    <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="39"/>
+      <c r="I52" s="39"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="39"/>
+      <c r="L52" s="39"/>
+      <c r="M52" s="39"/>
+      <c r="N52" s="40"/>
+    </row>
+    <row r="53" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B53" s="32" t="s">
         <v>41</v>
       </c>
       <c r="D53" s="29"/>
       <c r="E53" s="30"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="26"/>
-      <c r="J53" s="26"/>
-      <c r="K53" s="26"/>
-      <c r="L53" s="27"/>
-      <c r="M53" s="27"/>
-      <c r="N53" s="27"/>
-    </row>
-    <row r="54" spans="1:14" ht="340" x14ac:dyDescent="0.2">
+      <c r="F53" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H53" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I53" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J53" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K53" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L53" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M53" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N53" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O53" t="str">
+        <f>IF(OR( AND(C54=D54,OR(F53&lt;&gt;G53, I53&lt;&gt;J53,L53&lt;&gt;M53)),  AND(D54=E54,OR(G53&lt;&gt;H53,J53&lt;&gt;K53,M53&lt;&gt;N53)), AND(C54=E54, OR(F53&lt;&gt;H53,I53&lt;&gt;K53,L53&lt;&gt;N53) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="340" x14ac:dyDescent="0.2">
       <c r="B54" s="32"/>
-      <c r="C54" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D54" s="29"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="26"/>
-      <c r="J54" s="26"/>
-      <c r="K54" s="26"/>
-      <c r="L54" s="27"/>
-      <c r="M54" s="27"/>
-      <c r="N54" s="27"/>
-    </row>
-    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C54" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="F54" s="47"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="50"/>
+      <c r="J54" s="51"/>
+      <c r="K54" s="52"/>
+      <c r="L54" s="53"/>
+      <c r="M54" s="54"/>
+      <c r="N54" s="55"/>
+    </row>
+    <row r="55" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B55" s="32" t="s">
         <v>42</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="30"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="26"/>
-      <c r="K55" s="26"/>
-      <c r="L55" s="27"/>
-      <c r="M55" s="27"/>
-      <c r="N55" s="27"/>
-    </row>
-    <row r="56" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="F55" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H55" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I55" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J55" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K55" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L55" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M55" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N55" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O55" t="str">
+        <f>IF(OR( AND(C56=D56,OR(F55&lt;&gt;G55, I55&lt;&gt;J55,L55&lt;&gt;M55)),  AND(D56=E56,OR(G55&lt;&gt;H55,J55&lt;&gt;K55,M55&lt;&gt;N55)), AND(C56=E56, OR(F55&lt;&gt;H55,I55&lt;&gt;K55,L55&lt;&gt;N55) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B56" s="32"/>
-      <c r="C56" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D56" s="29"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
-      <c r="H56" s="25"/>
-      <c r="I56" s="26"/>
-      <c r="J56" s="26"/>
-      <c r="K56" s="26"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="27"/>
-      <c r="N56" s="27"/>
-    </row>
-    <row r="57" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C56" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="D56" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="F56" s="47"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="50"/>
+      <c r="J56" s="51"/>
+      <c r="K56" s="52"/>
+      <c r="L56" s="53"/>
+      <c r="M56" s="54"/>
+      <c r="N56" s="55"/>
+    </row>
+    <row r="57" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B57" s="32" t="s">
         <v>43</v>
       </c>
@@ -2380,78 +3002,112 @@
       <c r="L57" s="27"/>
       <c r="M57" s="27"/>
       <c r="N57" s="27"/>
-    </row>
-    <row r="58" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="O57" t="str">
+        <f>IF(OR( AND(C58=D58,OR(F57&lt;&gt;G57, I57&lt;&gt;J57,L57&lt;&gt;M57)),  AND(D58=E58,OR(G57&lt;&gt;H57,J57&lt;&gt;K57,M57&lt;&gt;N57)), AND(C58=E58, OR(F57&lt;&gt;H57,I57&lt;&gt;K57,L57&lt;&gt;N57) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B58" s="32"/>
       <c r="C58" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" s="29"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
-      <c r="I58" s="26"/>
-      <c r="J58" s="26"/>
-      <c r="K58" s="26"/>
-      <c r="L58" s="27"/>
-      <c r="M58" s="27"/>
-      <c r="N58" s="27"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F58" s="47"/>
+      <c r="G58" s="48"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="50"/>
+      <c r="J58" s="51"/>
+      <c r="K58" s="52"/>
+      <c r="L58" s="53"/>
+      <c r="M58" s="54"/>
+      <c r="N58" s="55"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>9</v>
       </c>
-      <c r="B59" s="43" t="s">
+      <c r="B59" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="43"/>
-      <c r="D59" s="43"/>
-      <c r="E59" s="43"/>
-      <c r="F59" s="43"/>
-      <c r="G59" s="43"/>
-      <c r="H59" s="43"/>
-      <c r="I59" s="43"/>
-      <c r="J59" s="43"/>
-      <c r="K59" s="43"/>
-      <c r="L59" s="43"/>
-      <c r="M59" s="43"/>
-      <c r="N59" s="56"/>
-    </row>
-    <row r="60" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C59" s="39"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="39"/>
+      <c r="I59" s="39"/>
+      <c r="J59" s="39"/>
+      <c r="K59" s="39"/>
+      <c r="L59" s="39"/>
+      <c r="M59" s="39"/>
+      <c r="N59" s="40"/>
+    </row>
+    <row r="60" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B60" s="32" t="s">
         <v>41</v>
       </c>
       <c r="D60" s="29"/>
       <c r="E60" s="30"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
-      <c r="I60" s="26"/>
-      <c r="J60" s="26"/>
-      <c r="K60" s="26"/>
-      <c r="L60" s="27"/>
-      <c r="M60" s="27"/>
-      <c r="N60" s="27"/>
-    </row>
-    <row r="61" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="F60" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G60" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H60" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I60" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J60" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K60" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L60" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M60" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N60" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O60" t="str">
+        <f>IF(OR( AND(C61=D61,OR(F60&lt;&gt;G60, I60&lt;&gt;J60,L60&lt;&gt;M60)),  AND(D61=E61,OR(G60&lt;&gt;H60,J60&lt;&gt;K60,M60&lt;&gt;N60)), AND(C61=E61, OR(F60&lt;&gt;H60,I60&lt;&gt;K60,L60&lt;&gt;N60) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="32"/>
-      <c r="C61" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="D61" s="29"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="26"/>
-      <c r="K61" s="26"/>
-      <c r="L61" s="27"/>
-      <c r="M61" s="27"/>
-      <c r="N61" s="27"/>
-    </row>
-    <row r="62" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C61" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D61" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="E61" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="F61" s="47"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="50"/>
+      <c r="J61" s="51"/>
+      <c r="K61" s="52"/>
+      <c r="L61" s="53"/>
+      <c r="M61" s="54"/>
+      <c r="N61" s="55"/>
+    </row>
+    <row r="62" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B62" s="32" t="s">
         <v>42</v>
       </c>
@@ -2466,25 +3122,34 @@
       <c r="L62" s="27"/>
       <c r="M62" s="27"/>
       <c r="N62" s="27"/>
-    </row>
-    <row r="63" spans="1:14" ht="306" x14ac:dyDescent="0.2">
+      <c r="O62" t="str">
+        <f>IF(OR( AND(C63=D63,OR(F62&lt;&gt;G62, I62&lt;&gt;J62,L62&lt;&gt;M62)),  AND(D63=E63,OR(G62&lt;&gt;H62,J62&lt;&gt;K62,M62&lt;&gt;N62)), AND(C63=E63, OR(F62&lt;&gt;H62,I62&lt;&gt;K62,L62&lt;&gt;N62) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="306" x14ac:dyDescent="0.2">
       <c r="B63" s="32"/>
       <c r="C63" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D63" s="29"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="25"/>
-      <c r="H63" s="25"/>
-      <c r="I63" s="26"/>
-      <c r="J63" s="26"/>
-      <c r="K63" s="26"/>
-      <c r="L63" s="27"/>
-      <c r="M63" s="27"/>
-      <c r="N63" s="27"/>
-    </row>
-    <row r="64" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="D63" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E63" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="F63" s="47"/>
+      <c r="G63" s="48"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="50"/>
+      <c r="J63" s="51"/>
+      <c r="K63" s="52"/>
+      <c r="L63" s="53"/>
+      <c r="M63" s="54"/>
+      <c r="N63" s="55"/>
+      <c r="O63" s="1"/>
+    </row>
+    <row r="64" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B64" s="32" t="s">
         <v>43</v>
       </c>
@@ -2499,144 +3164,232 @@
       <c r="L64" s="27"/>
       <c r="M64" s="27"/>
       <c r="N64" s="27"/>
-    </row>
-    <row r="65" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+      <c r="O64" t="str">
+        <f>IF(OR( AND(C65=D65,OR(F64&lt;&gt;G64, I64&lt;&gt;J64,L64&lt;&gt;M64)),  AND(D65=E65,OR(G64&lt;&gt;H64,J64&lt;&gt;K64,M64&lt;&gt;N64)), AND(C65=E65, OR(F64&lt;&gt;H64,I64&lt;&gt;K64,L64&lt;&gt;N64) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="388" x14ac:dyDescent="0.2">
       <c r="B65" s="32"/>
       <c r="C65" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D65" s="29"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="25"/>
-      <c r="I65" s="26"/>
-      <c r="J65" s="26"/>
-      <c r="K65" s="26"/>
-      <c r="L65" s="27"/>
-      <c r="M65" s="27"/>
-      <c r="N65" s="27"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="D65" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E65" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="F65" s="47"/>
+      <c r="G65" s="48"/>
+      <c r="H65" s="49"/>
+      <c r="I65" s="50"/>
+      <c r="J65" s="51"/>
+      <c r="K65" s="52"/>
+      <c r="L65" s="53"/>
+      <c r="M65" s="54"/>
+      <c r="N65" s="55"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>10</v>
       </c>
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="43"/>
-      <c r="I66" s="43"/>
-      <c r="J66" s="43"/>
-      <c r="K66" s="43"/>
-      <c r="L66" s="43"/>
-      <c r="M66" s="43"/>
-      <c r="N66" s="56"/>
-    </row>
-    <row r="67" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="39"/>
+      <c r="F66" s="39"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="39"/>
+      <c r="I66" s="39"/>
+      <c r="J66" s="39"/>
+      <c r="K66" s="39"/>
+      <c r="L66" s="39"/>
+      <c r="M66" s="39"/>
+      <c r="N66" s="40"/>
+    </row>
+    <row r="67" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B67" s="32" t="s">
         <v>41</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="30"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="25"/>
-      <c r="H67" s="25"/>
-      <c r="I67" s="26"/>
-      <c r="J67" s="26"/>
-      <c r="K67" s="26"/>
-      <c r="L67" s="27"/>
-      <c r="M67" s="27"/>
-      <c r="N67" s="27"/>
-    </row>
-    <row r="68" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="F67" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G67" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H67" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I67" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J67" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K67" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L67" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M67" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N67" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O67" t="str">
+        <f>IF(OR( AND(C68=D68,OR(F67&lt;&gt;G67, I67&lt;&gt;J67,L67&lt;&gt;M67)),  AND(D68=E68,OR(G67&lt;&gt;H67,J67&lt;&gt;K67,M67&lt;&gt;N67)), AND(C68=E68, OR(F67&lt;&gt;H67,I67&lt;&gt;K67,L67&lt;&gt;N67) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="32"/>
-      <c r="C68" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="D68" s="29"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="25"/>
-      <c r="H68" s="25"/>
-      <c r="I68" s="26"/>
-      <c r="J68" s="26"/>
-      <c r="K68" s="26"/>
-      <c r="L68" s="27"/>
-      <c r="M68" s="27"/>
-      <c r="N68" s="27"/>
-    </row>
-    <row r="69" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C68" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="D68" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="E68" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="F68" s="47"/>
+      <c r="G68" s="48"/>
+      <c r="H68" s="49"/>
+      <c r="I68" s="50"/>
+      <c r="J68" s="51"/>
+      <c r="K68" s="52"/>
+      <c r="L68" s="53"/>
+      <c r="M68" s="54"/>
+      <c r="N68" s="55"/>
+    </row>
+    <row r="69" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D69" s="29"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="25"/>
-      <c r="H69" s="25"/>
-      <c r="I69" s="26"/>
-      <c r="J69" s="26"/>
-      <c r="K69" s="26"/>
-      <c r="L69" s="27"/>
-      <c r="M69" s="27"/>
-      <c r="N69" s="27"/>
-    </row>
-    <row r="70" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="C69" s="66"/>
+      <c r="D69" s="57"/>
+      <c r="E69" s="58"/>
+      <c r="F69" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G69" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H69" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I69" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J69" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K69" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L69" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M69" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N69" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O69" t="str">
+        <f>IF(OR( AND(C70=D70,OR(F69&lt;&gt;G69, I69&lt;&gt;J69,L69&lt;&gt;M69)),  AND(D70=E70,OR(G69&lt;&gt;H69,J69&lt;&gt;K69,M69&lt;&gt;N69)), AND(C70=E70, OR(F69&lt;&gt;H69,I69&lt;&gt;K69,L69&lt;&gt;N69) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="32"/>
-      <c r="C70" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D70" s="29"/>
-      <c r="E70" s="30"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="25"/>
-      <c r="H70" s="25"/>
-      <c r="I70" s="26"/>
-      <c r="J70" s="26"/>
-      <c r="K70" s="26"/>
-      <c r="L70" s="27"/>
-      <c r="M70" s="27"/>
-      <c r="N70" s="27"/>
-    </row>
-    <row r="71" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="C70" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="D70" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="E70" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="F70" s="47"/>
+      <c r="G70" s="48"/>
+      <c r="H70" s="49"/>
+      <c r="I70" s="50"/>
+      <c r="J70" s="51"/>
+      <c r="K70" s="52"/>
+      <c r="L70" s="53"/>
+      <c r="M70" s="54"/>
+      <c r="N70" s="55"/>
+    </row>
+    <row r="71" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="D71" s="29"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="25"/>
-      <c r="H71" s="25"/>
-      <c r="I71" s="26"/>
-      <c r="J71" s="26"/>
-      <c r="K71" s="26"/>
-      <c r="L71" s="27"/>
-      <c r="M71" s="27"/>
-      <c r="N71" s="27"/>
-    </row>
-    <row r="72" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="C71" s="56"/>
+      <c r="D71" s="57"/>
+      <c r="E71" s="58"/>
+      <c r="F71" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="G71" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="H71" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="I71" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="J71" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="K71" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="L71" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="M71" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="N71" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O71" t="str">
+        <f>IF(OR( AND(C72=D72,OR(F71&lt;&gt;G71, I71&lt;&gt;J71,L71&lt;&gt;M71)),  AND(D72=E72,OR(G71&lt;&gt;H71,J71&lt;&gt;K71,M71&lt;&gt;N71)), AND(C72=E72, OR(F71&lt;&gt;H71,I71&lt;&gt;K71,L71&lt;&gt;N71) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="32"/>
-      <c r="C72" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="D72" s="29"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="53"/>
-      <c r="G72" s="53"/>
-      <c r="H72" s="53"/>
-      <c r="I72" s="54"/>
-      <c r="J72" s="54"/>
-      <c r="K72" s="54"/>
-      <c r="L72" s="55"/>
-      <c r="M72" s="55"/>
+      <c r="C72" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="D72" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="E72" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="F72" s="47"/>
+      <c r="G72" s="48"/>
+      <c r="H72" s="49"/>
+      <c r="I72" s="50"/>
+      <c r="J72" s="51"/>
+      <c r="K72" s="52"/>
+      <c r="L72" s="53"/>
+      <c r="M72" s="54"/>
       <c r="N72" s="55"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C73"/>
       <c r="D73"/>
       <c r="E73"/>
@@ -2650,7 +3403,7 @@
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C74"/>
       <c r="D74"/>
       <c r="E74"/>
@@ -2664,7 +3417,7 @@
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C75"/>
       <c r="D75"/>
       <c r="E75"/>
@@ -2678,7 +3431,7 @@
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C76"/>
       <c r="D76"/>
       <c r="E76"/>
@@ -2692,7 +3445,7 @@
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C77"/>
       <c r="D77"/>
       <c r="E77"/>
@@ -2706,7 +3459,7 @@
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C78"/>
       <c r="D78"/>
       <c r="E78"/>
@@ -2720,7 +3473,7 @@
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C79"/>
       <c r="D79"/>
       <c r="E79"/>
@@ -2734,7 +3487,7 @@
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C80"/>
       <c r="D80"/>
       <c r="E80"/>
@@ -4961,8 +5714,106 @@
       <c r="M249" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="C22:C23"/>
+  <mergeCells count="106">
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="L21:N21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="L37:N37"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="L44:N44"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="L47:N47"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="L51:N51"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="L49:N49"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="L72:N72"/>
+    <mergeCell ref="I72:K72"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="L58:N58"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="I61:K61"/>
+    <mergeCell ref="L61:N61"/>
+    <mergeCell ref="L63:N63"/>
+    <mergeCell ref="I63:K63"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="L65:N65"/>
+    <mergeCell ref="I65:K65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="L68:N68"/>
+    <mergeCell ref="I68:K68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="L70:N70"/>
+    <mergeCell ref="I70:K70"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="B17:N17"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B10:N10"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="B66:N66"/>
     <mergeCell ref="B59:N59"/>
     <mergeCell ref="B52:N52"/>
@@ -4970,35 +5821,19 @@
     <mergeCell ref="B38:N38"/>
     <mergeCell ref="B31:N31"/>
     <mergeCell ref="B24:N24"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B10:N10"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B17:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1AA851-AA00-BA45-955A-1248E058A2EC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added cross-sheet point retrieval
</commit_message>
<xml_diff>
--- a/project/evaluation/qualitative_evaluation/qualitative_evaluation_table.xlsx
+++ b/project/evaluation/qualitative_evaluation/qualitative_evaluation_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteom/shared-folder/nlpt_group/project/evaluation/qualitative_evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7119FCC3-8251-E84F-AF41-AD9733DDD04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFB62E7-BE06-5245-87AE-7F69DF20A1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-5940" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{BFF5F178-14AB-6B4F-B81C-3E61E0B93405}"/>
+    <workbookView xWindow="28800" yWindow="-5940" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{BFF5F178-14AB-6B4F-B81C-3E61E0B93405}"/>
   </bookViews>
   <sheets>
     <sheet name="Correct retrieval" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="98">
   <si>
     <t>Comparison queries:</t>
   </si>
@@ -317,6 +317,21 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Averaged scores</t>
+  </si>
+  <si>
+    <t>Qualitative scores</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>mrr</t>
+  </si>
+  <si>
+    <t>ndcg</t>
   </si>
 </sst>
 </file>
@@ -613,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -675,6 +690,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -773,6 +797,25 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1272,30 +1315,30 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
     </row>
     <row r="26" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
     </row>
     <row r="27" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C27" s="15" t="s">
@@ -1324,7 +1367,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="5">
@@ -1340,7 +1383,7 @@
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="37"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="9">
         <v>2</v>
       </c>
@@ -1354,7 +1397,7 @@
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="37"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="9">
         <v>3</v>
       </c>
@@ -1368,7 +1411,7 @@
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="37"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="9">
         <v>4</v>
       </c>
@@ -1382,7 +1425,7 @@
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="37"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="9">
         <v>5</v>
       </c>
@@ -1396,7 +1439,7 @@
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="37"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="9">
         <v>6</v>
       </c>
@@ -1410,7 +1453,7 @@
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="37"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="9">
         <v>7</v>
       </c>
@@ -1424,7 +1467,7 @@
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="37"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="9">
         <v>8</v>
       </c>
@@ -1438,7 +1481,7 @@
       <c r="J35" s="4"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="37"/>
+      <c r="A36" s="40"/>
       <c r="B36" s="9">
         <v>9</v>
       </c>
@@ -1452,7 +1495,7 @@
       <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="37"/>
+      <c r="A37" s="40"/>
       <c r="B37" s="10">
         <v>10</v>
       </c>
@@ -1486,9 +1529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03816060-24A7-D946-9AB1-F7E07293AE02}">
   <dimension ref="A1:O249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1510,35 +1553,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="46" t="s">
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="25" t="s">
         <v>44</v>
       </c>
@@ -1571,21 +1614,21 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="40"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="43"/>
     </row>
     <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
@@ -1628,24 +1671,24 @@
     </row>
     <row r="5" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="32"/>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="47"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="55"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="58"/>
     </row>
     <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="32" t="s">
@@ -1688,24 +1731,24 @@
     </row>
     <row r="7" spans="1:15" ht="372" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="32"/>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="57" t="s">
+      <c r="D7" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="55"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="58"/>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="32" t="s">
@@ -1739,35 +1782,35 @@
       <c r="E9" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="47"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="55"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="58"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="40"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="43"/>
     </row>
     <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="32" t="s">
@@ -1776,31 +1819,31 @@
       <c r="C11" s="28"/>
       <c r="D11" s="29"/>
       <c r="E11" s="33"/>
-      <c r="F11" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H11" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I11" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K11" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L11" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M11" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N11" s="63" t="s">
+      <c r="F11" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M11" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O11" t="str">
@@ -1810,24 +1853,24 @@
     </row>
     <row r="12" spans="1:15" ht="404" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="32"/>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="57" t="s">
+      <c r="D12" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="47"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="55"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="58"/>
     </row>
     <row r="13" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="32" t="s">
@@ -1836,31 +1879,31 @@
       <c r="C13" s="28"/>
       <c r="D13" s="29"/>
       <c r="E13" s="33"/>
-      <c r="F13" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H13" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J13" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K13" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L13" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M13" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N13" s="63" t="s">
+      <c r="F13" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L13" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M13" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N13" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O13" t="str">
@@ -1870,24 +1913,24 @@
     </row>
     <row r="14" spans="1:15" ht="344" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="32"/>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="57" t="s">
+      <c r="D14" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="47"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="55"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="58"/>
     </row>
     <row r="15" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="32" t="s">
@@ -1896,31 +1939,31 @@
       <c r="C15" s="28"/>
       <c r="D15" s="29"/>
       <c r="E15" s="33"/>
-      <c r="F15" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H15" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I15" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J15" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K15" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L15" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M15" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N15" s="63" t="s">
+      <c r="F15" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M15" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N15" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O15" t="str">
@@ -1930,44 +1973,44 @@
     </row>
     <row r="16" spans="1:15" ht="340" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="32"/>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="57" t="s">
+      <c r="D16" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="47"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="55"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="58"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>3</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="40"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="43"/>
     </row>
     <row r="18" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="32" t="s">
@@ -1976,31 +2019,31 @@
       <c r="C18" s="28"/>
       <c r="D18" s="29"/>
       <c r="E18" s="33"/>
-      <c r="F18" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G18" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I18" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K18" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L18" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M18" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N18" s="63" t="s">
+      <c r="F18" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K18" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M18" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N18" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O18" t="str">
@@ -2010,24 +2053,24 @@
     </row>
     <row r="19" spans="1:15" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="32"/>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="57" t="s">
+      <c r="D19" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="59" t="s">
+      <c r="E19" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="55"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="58"/>
     </row>
     <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="32" t="s">
@@ -2036,31 +2079,31 @@
       <c r="C20" s="28"/>
       <c r="D20" s="29"/>
       <c r="E20" s="33"/>
-      <c r="F20" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H20" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I20" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J20" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K20" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L20" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M20" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N20" s="63" t="s">
+      <c r="F20" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K20" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L20" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M20" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N20" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O20" t="str">
@@ -2070,24 +2113,24 @@
     </row>
     <row r="21" spans="1:15" ht="404" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="32"/>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="57" t="s">
+      <c r="D21" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="59" t="s">
+      <c r="E21" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="55"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="58"/>
     </row>
     <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="32" t="s">
@@ -2095,32 +2138,32 @@
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="29"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G22" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J22" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K22" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L22" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M22" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N22" s="63" t="s">
+      <c r="E22" s="37"/>
+      <c r="F22" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K22" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L22" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M22" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N22" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O22" t="str">
@@ -2130,77 +2173,77 @@
     </row>
     <row r="23" spans="1:15" ht="372" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="32"/>
-      <c r="C23" s="56" t="s">
+      <c r="C23" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="57" t="s">
+      <c r="D23" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="64" t="s">
+      <c r="E23" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="47"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="55"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="57"/>
+      <c r="N23" s="58"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>4</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="40"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="43"/>
     </row>
     <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B25" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="35"/>
+      <c r="C25" s="38"/>
       <c r="D25" s="29"/>
       <c r="E25" s="30"/>
-      <c r="F25" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H25" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J25" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K25" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L25" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M25" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N25" s="63" t="s">
+      <c r="F25" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H25" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L25" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M25" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N25" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O25" t="str">
@@ -2210,57 +2253,57 @@
     </row>
     <row r="26" spans="1:15" ht="272" x14ac:dyDescent="0.2">
       <c r="B26" s="32"/>
-      <c r="C26" s="65" t="s">
+      <c r="C26" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="57" t="s">
+      <c r="D26" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="58" t="s">
+      <c r="E26" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="54"/>
-      <c r="N26" s="55"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="58"/>
     </row>
     <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H27" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I27" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J27" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K27" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L27" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M27" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N27" s="63" t="s">
+      <c r="C27" s="69"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I27" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J27" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K27" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L27" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M27" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N27" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O27" t="str">
@@ -2270,24 +2313,24 @@
     </row>
     <row r="28" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B28" s="32"/>
-      <c r="C28" s="65" t="s">
+      <c r="C28" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="57" t="s">
+      <c r="D28" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="58" t="s">
+      <c r="E28" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="F28" s="47"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="54"/>
-      <c r="N28" s="55"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="58"/>
     </row>
     <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="32" t="s">
@@ -2320,35 +2363,35 @@
       <c r="E30" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="47"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="52"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="55"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="58"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>5</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="40"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="43"/>
     </row>
     <row r="32" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="32" t="s">
@@ -2356,31 +2399,31 @@
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="30"/>
-      <c r="F32" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G32" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H32" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I32" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J32" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K32" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L32" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M32" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N32" s="63" t="s">
+      <c r="F32" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H32" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J32" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K32" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L32" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M32" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N32" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O32" t="str">
@@ -2390,24 +2433,24 @@
     </row>
     <row r="33" spans="1:15" ht="289" x14ac:dyDescent="0.2">
       <c r="B33" s="32"/>
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="57" t="s">
+      <c r="D33" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="58" t="s">
+      <c r="E33" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="47"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="53"/>
-      <c r="M33" s="54"/>
-      <c r="N33" s="55"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="57"/>
+      <c r="N33" s="58"/>
     </row>
     <row r="34" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" s="32" t="s">
@@ -2415,31 +2458,31 @@
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="30"/>
-      <c r="F34" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G34" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H34" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I34" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J34" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K34" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L34" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M34" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N34" s="63" t="s">
+      <c r="F34" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G34" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H34" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J34" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K34" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L34" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M34" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N34" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O34" t="str">
@@ -2449,24 +2492,24 @@
     </row>
     <row r="35" spans="1:15" ht="306" x14ac:dyDescent="0.2">
       <c r="B35" s="32"/>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="57" t="s">
+      <c r="D35" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="E35" s="58" t="s">
+      <c r="E35" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="F35" s="47"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="51"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="54"/>
-      <c r="N35" s="55"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="54"/>
+      <c r="K35" s="55"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="57"/>
+      <c r="N35" s="58"/>
     </row>
     <row r="36" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" s="32" t="s">
@@ -2499,35 +2542,35 @@
       <c r="E37" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="47"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="52"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="54"/>
-      <c r="N37" s="55"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="54"/>
+      <c r="K37" s="55"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="57"/>
+      <c r="N37" s="58"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>6</v>
       </c>
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39"/>
-      <c r="M38" s="39"/>
-      <c r="N38" s="40"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="42"/>
+      <c r="L38" s="42"/>
+      <c r="M38" s="42"/>
+      <c r="N38" s="43"/>
     </row>
     <row r="39" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B39" s="32" t="s">
@@ -2560,15 +2603,15 @@
       <c r="E40" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F40" s="47"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="49"/>
-      <c r="I40" s="50"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="52"/>
-      <c r="L40" s="53"/>
-      <c r="M40" s="54"/>
-      <c r="N40" s="55"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="54"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="56"/>
+      <c r="M40" s="57"/>
+      <c r="N40" s="58"/>
     </row>
     <row r="41" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B41" s="32" t="s">
@@ -2576,31 +2619,31 @@
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="30"/>
-      <c r="F41" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G41" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H41" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I41" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J41" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K41" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L41" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M41" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N41" s="63" t="s">
+      <c r="F41" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H41" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I41" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J41" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K41" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L41" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M41" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N41" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O41" t="str">
@@ -2610,24 +2653,24 @@
     </row>
     <row r="42" spans="1:15" ht="340" x14ac:dyDescent="0.2">
       <c r="B42" s="32"/>
-      <c r="C42" s="56" t="s">
+      <c r="C42" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="57" t="s">
+      <c r="D42" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="58" t="s">
+      <c r="E42" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="47"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="50"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="52"/>
-      <c r="L42" s="53"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="55"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="54"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="56"/>
+      <c r="M42" s="57"/>
+      <c r="N42" s="58"/>
     </row>
     <row r="43" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B43" s="32" t="s">
@@ -2660,35 +2703,35 @@
       <c r="E44" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F44" s="47"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="49"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="52"/>
-      <c r="L44" s="53"/>
-      <c r="M44" s="54"/>
-      <c r="N44" s="55"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="54"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="57"/>
+      <c r="N44" s="58"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>7</v>
       </c>
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
-      <c r="M45" s="39"/>
-      <c r="N45" s="40"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
+      <c r="J45" s="42"/>
+      <c r="K45" s="42"/>
+      <c r="L45" s="42"/>
+      <c r="M45" s="42"/>
+      <c r="N45" s="43"/>
     </row>
     <row r="46" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B46" s="32" t="s">
@@ -2696,31 +2739,31 @@
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="30"/>
-      <c r="F46" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G46" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H46" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I46" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J46" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K46" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L46" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M46" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N46" s="63" t="s">
+      <c r="F46" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H46" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I46" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J46" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K46" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L46" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M46" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N46" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O46" t="str">
@@ -2730,24 +2773,24 @@
     </row>
     <row r="47" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="32"/>
-      <c r="C47" s="56" t="s">
+      <c r="C47" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="D47" s="57" t="s">
+      <c r="D47" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="58" t="s">
+      <c r="E47" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="F47" s="47"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="49"/>
-      <c r="I47" s="50"/>
-      <c r="J47" s="51"/>
-      <c r="K47" s="52"/>
-      <c r="L47" s="53"/>
-      <c r="M47" s="54"/>
-      <c r="N47" s="55"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="52"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="54"/>
+      <c r="K47" s="55"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="57"/>
+      <c r="N47" s="58"/>
     </row>
     <row r="48" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B48" s="32" t="s">
@@ -2755,31 +2798,31 @@
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="30"/>
-      <c r="F48" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G48" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H48" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I48" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J48" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K48" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L48" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M48" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N48" s="63" t="s">
+      <c r="F48" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H48" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I48" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J48" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K48" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L48" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M48" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N48" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O48" t="str">
@@ -2789,24 +2832,24 @@
     </row>
     <row r="49" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="32"/>
-      <c r="C49" s="56" t="s">
+      <c r="C49" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="D49" s="57" t="s">
+      <c r="D49" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="E49" s="58" t="s">
+      <c r="E49" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="F49" s="47"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="49"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="51"/>
-      <c r="K49" s="52"/>
-      <c r="L49" s="53"/>
-      <c r="M49" s="54"/>
-      <c r="N49" s="55"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="54"/>
+      <c r="K49" s="55"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="57"/>
+      <c r="N49" s="58"/>
     </row>
     <row r="50" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B50" s="32" t="s">
@@ -2839,35 +2882,35 @@
       <c r="E51" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="F51" s="47"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="49"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="51"/>
-      <c r="K51" s="52"/>
-      <c r="L51" s="53"/>
-      <c r="M51" s="54"/>
-      <c r="N51" s="55"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="53"/>
+      <c r="J51" s="54"/>
+      <c r="K51" s="55"/>
+      <c r="L51" s="56"/>
+      <c r="M51" s="57"/>
+      <c r="N51" s="58"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>8</v>
       </c>
-      <c r="B52" s="39" t="s">
+      <c r="B52" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="39"/>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="39"/>
-      <c r="N52" s="40"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="42"/>
+      <c r="H52" s="42"/>
+      <c r="I52" s="42"/>
+      <c r="J52" s="42"/>
+      <c r="K52" s="42"/>
+      <c r="L52" s="42"/>
+      <c r="M52" s="42"/>
+      <c r="N52" s="43"/>
     </row>
     <row r="53" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B53" s="32" t="s">
@@ -2875,31 +2918,31 @@
       </c>
       <c r="D53" s="29"/>
       <c r="E53" s="30"/>
-      <c r="F53" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G53" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H53" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I53" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J53" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K53" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L53" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M53" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N53" s="63" t="s">
+      <c r="F53" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H53" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I53" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J53" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K53" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L53" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M53" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N53" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O53" t="str">
@@ -2909,24 +2952,24 @@
     </row>
     <row r="54" spans="1:15" ht="340" x14ac:dyDescent="0.2">
       <c r="B54" s="32"/>
-      <c r="C54" s="56" t="s">
+      <c r="C54" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="D54" s="57" t="s">
+      <c r="D54" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="E54" s="58" t="s">
+      <c r="E54" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="F54" s="47"/>
-      <c r="G54" s="48"/>
-      <c r="H54" s="49"/>
-      <c r="I54" s="50"/>
-      <c r="J54" s="51"/>
-      <c r="K54" s="52"/>
-      <c r="L54" s="53"/>
-      <c r="M54" s="54"/>
-      <c r="N54" s="55"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="51"/>
+      <c r="H54" s="52"/>
+      <c r="I54" s="53"/>
+      <c r="J54" s="54"/>
+      <c r="K54" s="55"/>
+      <c r="L54" s="56"/>
+      <c r="M54" s="57"/>
+      <c r="N54" s="58"/>
     </row>
     <row r="55" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B55" s="32" t="s">
@@ -2934,31 +2977,31 @@
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="30"/>
-      <c r="F55" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G55" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H55" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I55" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J55" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K55" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L55" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M55" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N55" s="63" t="s">
+      <c r="F55" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H55" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I55" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J55" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K55" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L55" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M55" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N55" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O55" t="str">
@@ -2968,24 +3011,24 @@
     </row>
     <row r="56" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B56" s="32"/>
-      <c r="C56" s="56" t="s">
+      <c r="C56" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="D56" s="57" t="s">
+      <c r="D56" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="E56" s="58" t="s">
+      <c r="E56" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="F56" s="47"/>
-      <c r="G56" s="48"/>
-      <c r="H56" s="49"/>
-      <c r="I56" s="50"/>
-      <c r="J56" s="51"/>
-      <c r="K56" s="52"/>
-      <c r="L56" s="53"/>
-      <c r="M56" s="54"/>
-      <c r="N56" s="55"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="53"/>
+      <c r="J56" s="54"/>
+      <c r="K56" s="55"/>
+      <c r="L56" s="56"/>
+      <c r="M56" s="57"/>
+      <c r="N56" s="58"/>
     </row>
     <row r="57" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B57" s="32" t="s">
@@ -3018,35 +3061,35 @@
       <c r="E58" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="F58" s="47"/>
-      <c r="G58" s="48"/>
-      <c r="H58" s="49"/>
-      <c r="I58" s="50"/>
-      <c r="J58" s="51"/>
-      <c r="K58" s="52"/>
-      <c r="L58" s="53"/>
-      <c r="M58" s="54"/>
-      <c r="N58" s="55"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="51"/>
+      <c r="H58" s="52"/>
+      <c r="I58" s="53"/>
+      <c r="J58" s="54"/>
+      <c r="K58" s="55"/>
+      <c r="L58" s="56"/>
+      <c r="M58" s="57"/>
+      <c r="N58" s="58"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>9</v>
       </c>
-      <c r="B59" s="39" t="s">
+      <c r="B59" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="39"/>
-      <c r="D59" s="39"/>
-      <c r="E59" s="39"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
-      <c r="I59" s="39"/>
-      <c r="J59" s="39"/>
-      <c r="K59" s="39"/>
-      <c r="L59" s="39"/>
-      <c r="M59" s="39"/>
-      <c r="N59" s="40"/>
+      <c r="C59" s="42"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="42"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="42"/>
+      <c r="H59" s="42"/>
+      <c r="I59" s="42"/>
+      <c r="J59" s="42"/>
+      <c r="K59" s="42"/>
+      <c r="L59" s="42"/>
+      <c r="M59" s="42"/>
+      <c r="N59" s="43"/>
     </row>
     <row r="60" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B60" s="32" t="s">
@@ -3054,31 +3097,31 @@
       </c>
       <c r="D60" s="29"/>
       <c r="E60" s="30"/>
-      <c r="F60" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G60" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H60" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I60" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J60" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K60" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L60" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M60" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N60" s="63" t="s">
+      <c r="F60" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G60" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H60" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I60" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J60" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K60" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L60" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M60" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N60" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O60" t="str">
@@ -3088,24 +3131,24 @@
     </row>
     <row r="61" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="32"/>
-      <c r="C61" s="56" t="s">
+      <c r="C61" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="D61" s="57" t="s">
+      <c r="D61" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="E61" s="58" t="s">
+      <c r="E61" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="F61" s="47"/>
-      <c r="G61" s="48"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="50"/>
-      <c r="J61" s="51"/>
-      <c r="K61" s="52"/>
-      <c r="L61" s="53"/>
-      <c r="M61" s="54"/>
-      <c r="N61" s="55"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="51"/>
+      <c r="H61" s="52"/>
+      <c r="I61" s="53"/>
+      <c r="J61" s="54"/>
+      <c r="K61" s="55"/>
+      <c r="L61" s="56"/>
+      <c r="M61" s="57"/>
+      <c r="N61" s="58"/>
     </row>
     <row r="62" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B62" s="32" t="s">
@@ -3138,15 +3181,15 @@
       <c r="E63" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="F63" s="47"/>
-      <c r="G63" s="48"/>
-      <c r="H63" s="49"/>
-      <c r="I63" s="50"/>
-      <c r="J63" s="51"/>
-      <c r="K63" s="52"/>
-      <c r="L63" s="53"/>
-      <c r="M63" s="54"/>
-      <c r="N63" s="55"/>
+      <c r="F63" s="50"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="53"/>
+      <c r="J63" s="54"/>
+      <c r="K63" s="55"/>
+      <c r="L63" s="56"/>
+      <c r="M63" s="57"/>
+      <c r="N63" s="58"/>
       <c r="O63" s="1"/>
     </row>
     <row r="64" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -3177,38 +3220,38 @@
       <c r="D65" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="E65" s="34" t="s">
+      <c r="E65" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="F65" s="47"/>
-      <c r="G65" s="48"/>
-      <c r="H65" s="49"/>
-      <c r="I65" s="50"/>
-      <c r="J65" s="51"/>
-      <c r="K65" s="52"/>
-      <c r="L65" s="53"/>
-      <c r="M65" s="54"/>
-      <c r="N65" s="55"/>
+      <c r="F65" s="50"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="52"/>
+      <c r="I65" s="53"/>
+      <c r="J65" s="54"/>
+      <c r="K65" s="55"/>
+      <c r="L65" s="56"/>
+      <c r="M65" s="57"/>
+      <c r="N65" s="58"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>10</v>
       </c>
-      <c r="B66" s="39" t="s">
+      <c r="B66" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="39"/>
-      <c r="D66" s="39"/>
-      <c r="E66" s="39"/>
-      <c r="F66" s="39"/>
-      <c r="G66" s="39"/>
-      <c r="H66" s="39"/>
-      <c r="I66" s="39"/>
-      <c r="J66" s="39"/>
-      <c r="K66" s="39"/>
-      <c r="L66" s="39"/>
-      <c r="M66" s="39"/>
-      <c r="N66" s="40"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="42"/>
+      <c r="I66" s="42"/>
+      <c r="J66" s="42"/>
+      <c r="K66" s="42"/>
+      <c r="L66" s="42"/>
+      <c r="M66" s="42"/>
+      <c r="N66" s="43"/>
     </row>
     <row r="67" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B67" s="32" t="s">
@@ -3216,31 +3259,31 @@
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="30"/>
-      <c r="F67" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G67" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H67" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I67" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J67" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K67" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L67" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M67" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N67" s="63" t="s">
+      <c r="F67" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G67" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H67" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I67" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J67" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K67" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L67" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M67" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N67" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O67" t="str">
@@ -3250,57 +3293,57 @@
     </row>
     <row r="68" spans="1:15" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="32"/>
-      <c r="C68" s="56" t="s">
+      <c r="C68" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="D68" s="57" t="s">
+      <c r="D68" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="E68" s="58" t="s">
+      <c r="E68" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="F68" s="47"/>
-      <c r="G68" s="48"/>
-      <c r="H68" s="49"/>
-      <c r="I68" s="50"/>
-      <c r="J68" s="51"/>
-      <c r="K68" s="52"/>
-      <c r="L68" s="53"/>
-      <c r="M68" s="54"/>
-      <c r="N68" s="55"/>
+      <c r="F68" s="50"/>
+      <c r="G68" s="51"/>
+      <c r="H68" s="52"/>
+      <c r="I68" s="53"/>
+      <c r="J68" s="54"/>
+      <c r="K68" s="55"/>
+      <c r="L68" s="56"/>
+      <c r="M68" s="57"/>
+      <c r="N68" s="58"/>
     </row>
     <row r="69" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C69" s="66"/>
-      <c r="D69" s="57"/>
-      <c r="E69" s="58"/>
-      <c r="F69" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G69" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H69" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I69" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J69" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K69" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L69" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M69" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N69" s="63" t="s">
+      <c r="C69" s="69"/>
+      <c r="D69" s="60"/>
+      <c r="E69" s="61"/>
+      <c r="F69" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G69" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H69" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I69" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J69" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K69" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L69" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M69" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N69" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O69" t="str">
@@ -3310,57 +3353,57 @@
     </row>
     <row r="70" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="32"/>
-      <c r="C70" s="56" t="s">
+      <c r="C70" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="D70" s="57" t="s">
+      <c r="D70" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="E70" s="58" t="s">
+      <c r="E70" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="F70" s="47"/>
-      <c r="G70" s="48"/>
-      <c r="H70" s="49"/>
-      <c r="I70" s="50"/>
-      <c r="J70" s="51"/>
-      <c r="K70" s="52"/>
-      <c r="L70" s="53"/>
-      <c r="M70" s="54"/>
-      <c r="N70" s="55"/>
+      <c r="F70" s="50"/>
+      <c r="G70" s="51"/>
+      <c r="H70" s="52"/>
+      <c r="I70" s="53"/>
+      <c r="J70" s="54"/>
+      <c r="K70" s="55"/>
+      <c r="L70" s="56"/>
+      <c r="M70" s="57"/>
+      <c r="N70" s="58"/>
     </row>
     <row r="71" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C71" s="56"/>
-      <c r="D71" s="57"/>
-      <c r="E71" s="58"/>
-      <c r="F71" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G71" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="H71" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="I71" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="J71" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="K71" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="L71" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M71" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="N71" s="63" t="s">
+      <c r="C71" s="59"/>
+      <c r="D71" s="60"/>
+      <c r="E71" s="61"/>
+      <c r="F71" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="G71" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="H71" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="I71" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="J71" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K71" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="L71" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="M71" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="N71" s="66" t="s">
         <v>92</v>
       </c>
       <c r="O71" t="str">
@@ -3370,24 +3413,24 @@
     </row>
     <row r="72" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="32"/>
-      <c r="C72" s="56" t="s">
+      <c r="C72" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="D72" s="57" t="s">
+      <c r="D72" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="E72" s="58" t="s">
+      <c r="E72" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="F72" s="47"/>
-      <c r="G72" s="48"/>
-      <c r="H72" s="49"/>
-      <c r="I72" s="50"/>
-      <c r="J72" s="51"/>
-      <c r="K72" s="52"/>
-      <c r="L72" s="53"/>
-      <c r="M72" s="54"/>
-      <c r="N72" s="55"/>
+      <c r="F72" s="50"/>
+      <c r="G72" s="51"/>
+      <c r="H72" s="52"/>
+      <c r="I72" s="53"/>
+      <c r="J72" s="54"/>
+      <c r="K72" s="55"/>
+      <c r="L72" s="56"/>
+      <c r="M72" s="57"/>
+      <c r="N72" s="58"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C73"/>
@@ -3404,9 +3447,11 @@
       <c r="N73" s="1"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C74"/>
-      <c r="D74"/>
-      <c r="E74"/>
+      <c r="C74" s="70" t="s">
+        <v>93</v>
+      </c>
+      <c r="D74" s="70"/>
+      <c r="E74" s="70"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
@@ -3418,9 +3463,18 @@
       <c r="N74" s="1"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C75"/>
-      <c r="D75"/>
-      <c r="E75"/>
+      <c r="C75" s="21" t="e">
+        <f>AVERAGE(AVERAGE(F4:F71),AVERAGE(G4:G74),AVERAGE(H4:H74))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D75" s="21" t="e">
+        <f>AVERAGE(AVERAGE(I4:I71),AVERAGE(J4:J74),AVERAGE(K4:K74))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E75" s="21" t="e">
+        <f>AVERAGE(AVERAGE(L4:L71),AVERAGE(M4:M74),AVERAGE(N4:N74))</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
@@ -3460,7 +3514,7 @@
       <c r="N77" s="1"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C78"/>
+      <c r="C78" s="71"/>
       <c r="D78"/>
       <c r="E78"/>
       <c r="F78" s="1"/>
@@ -5714,7 +5768,8 @@
       <c r="M249" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="106">
+  <mergeCells count="107">
+    <mergeCell ref="C74:E74"/>
     <mergeCell ref="F23:H23"/>
     <mergeCell ref="L21:N21"/>
     <mergeCell ref="I21:K21"/>
@@ -5828,12 +5883,82 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1AA851-AA00-BA45-955A-1248E058A2EC}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="C3" s="75" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="74"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+    </row>
+    <row r="4" spans="2:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="73" t="e">
+        <f>'Subjective scores'!C75</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+    </row>
+    <row r="5" spans="2:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="73" t="e">
+        <f>'Subjective scores'!D75</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+    </row>
+    <row r="6" spans="2:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="73" t="e">
+        <f>'Subjective scores'!E75</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add subjective ratings for queries 1-8
</commit_message>
<xml_diff>
--- a/project/evaluation/qualitative_evaluation/qualitative_evaluation_table.xlsx
+++ b/project/evaluation/qualitative_evaluation/qualitative_evaluation_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteom/shared-folder/nlpt_group/project/evaluation/qualitative_evaluation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandrafriebolin/Desktop/WS23-24/transformers/nlpt_group/project/evaluation/qualitative_evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFB62E7-BE06-5245-87AE-7F69DF20A1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC5F685-D06C-234D-B37A-048E54989C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-5940" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{BFF5F178-14AB-6B4F-B81C-3E61E0B93405}"/>
+    <workbookView xWindow="-4760" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{BFF5F178-14AB-6B4F-B81C-3E61E0B93405}"/>
   </bookViews>
   <sheets>
     <sheet name="Correct retrieval" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="136">
   <si>
     <t>Comparison queries:</t>
   </si>
@@ -332,13 +332,127 @@
   </si>
   <si>
     <t>ndcg</t>
+  </si>
+  <si>
+    <t>3 (relevant) [comment: directly addresses the impact of premorbid functioning and intelligence on occupational outcomes in bipolar disorder patients]</t>
+  </si>
+  <si>
+    <t>3 (relevant) [comment: same as model 1]</t>
+  </si>
+  <si>
+    <t>2 (neutral) [comment: focus is on how premorbid IQ moderates the relationship between clinical severity and executive functioning]</t>
+  </si>
+  <si>
+    <t>3 [comment: discusses association between premorbid intelligence, functioning, and illness severity in bipolar disorder]</t>
+  </si>
+  <si>
+    <t>3 [comment: same as model 1]</t>
+  </si>
+  <si>
+    <t>2 [comment: same as model 1]</t>
+  </si>
+  <si>
+    <t>1 (not relevant) [comment: focuses on the relationship between intelligence and risk of developing bipolar disorder, which diverges from query's interest in occupational outcomes]</t>
+  </si>
+  <si>
+    <t>1 [comment: same as model 1]</t>
+  </si>
+  <si>
+    <t>3 [comment: directly investigates association between bilateral hearing loss and nonverbal intelligence in US children aged 6 to 16 years]</t>
+  </si>
+  <si>
+    <t>3 [comment: although study was conducted in Nepal and includes young adults, it evaluates impact of hearing loss on nonverbal intelligence, making it relevant to the query]</t>
+  </si>
+  <si>
+    <t>1 [comment: study focuses on verbal intelligence outcomes in deaf children, rather than the specific association between bilateral hearing loss and nonverbal intelligence]</t>
+  </si>
+  <si>
+    <t>3 [comment: directly explores association between cognitive abilities in childhood and risk of suicide in adulthood]</t>
+  </si>
+  <si>
+    <t>3 [comment: examines relationship between cognitive ability in youth and  suicide/attempts]</t>
+  </si>
+  <si>
+    <t>2 [comment: also investigates cognitive abilities in children/adolescents who died by suicide, focusing more on improving reading/math skills]</t>
+  </si>
+  <si>
+    <t>1 [comment: focuses on parenting stress]</t>
+  </si>
+  <si>
+    <t>3 [comment: directly investigates association between early parenting behavior and child outcomes at 7]</t>
+  </si>
+  <si>
+    <t>1 [comment: no specifik linking of early parenting behaviours and later school outcomes]</t>
+  </si>
+  <si>
+    <t>1 [comment: focus is on socioeconomic factors and early life assessments without explicitly connecting them to parenting behaviors]</t>
+  </si>
+  <si>
+    <t>2 [comment: primarily focuses on impact of parental education levels rather than early parenting behavior]</t>
+  </si>
+  <si>
+    <t>3 [comment: directly investigates the association]</t>
+  </si>
+  <si>
+    <t>2 [comment: focus is a little broader, including cognitive ability in the normal range ]</t>
+  </si>
+  <si>
+    <t>2 [comment: direct relevance to cognitive impairment in intellectual disability in the context of homozygosity is less clear]</t>
+  </si>
+  <si>
+    <t>1 [comment:dDiscusses genetic basis of intelligence and intellectual disability broadly]</t>
+  </si>
+  <si>
+    <t>1 [comment: focuses on the genetic overlap between ASD/ADHD and cognitive ability]</t>
+  </si>
+  <si>
+    <t>1 [comment: not related to the query's focus on hydrocortisone treatment and neurodevelopment]</t>
+  </si>
+  <si>
+    <t>3 [comment: directly addresses the impact]</t>
+  </si>
+  <si>
+    <t>3 [comment: evaluates long-term neurocognitive outcomes of prophylactic hydrocortisone treatment]</t>
+  </si>
+  <si>
+    <t>2 [comment: related to the query but does not focus on the neonatal period or randomized trials]</t>
+  </si>
+  <si>
+    <t>3 [comment: presents a meta-analysis of trials]</t>
+  </si>
+  <si>
+    <t>3 [comment: directly investigates effects of prenatal micronutrient supplementation on intellectual development in children]</t>
+  </si>
+  <si>
+    <t>3 [comment: focuses on the long-term association of micronutrient supplementation with adolescents]</t>
+  </si>
+  <si>
+    <t>2 [comment: reviews effect of micronutrient interventions on cognitive performance in children, but not directly tied to prenatal micronutrient supplementation]</t>
+  </si>
+  <si>
+    <t>3 [comment: evaluates impact of prenatal micronutrient supplementation on children]</t>
+  </si>
+  <si>
+    <t>3 [comment: evaluates impact of prenatal micronutrient supplementation versus iron/folic acid on children's intelligence]</t>
+  </si>
+  <si>
+    <t>3 [comment: directly assesses association]</t>
+  </si>
+  <si>
+    <t>3 [comment: considers maternal stress/depression over time and its impact on child development]</t>
+  </si>
+  <si>
+    <t>3 [comment:  impact of maternal depression from pregnancy onwards, explores its association with children's cognitive development]</t>
+  </si>
+  <si>
+    <t>3 [comment: systematic review of effects of perinatal depression on IQ of children]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -362,6 +476,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -706,66 +828,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -798,10 +860,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -815,6 +873,72 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1315,30 +1439,30 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
     </row>
     <row r="26" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
     </row>
     <row r="27" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C27" s="15" t="s">
@@ -1367,7 +1491,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="56" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="5">
@@ -1383,7 +1507,7 @@
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="40"/>
+      <c r="A29" s="56"/>
       <c r="B29" s="9">
         <v>2</v>
       </c>
@@ -1397,7 +1521,7 @@
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="40"/>
+      <c r="A30" s="56"/>
       <c r="B30" s="9">
         <v>3</v>
       </c>
@@ -1411,7 +1535,7 @@
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="40"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="9">
         <v>4</v>
       </c>
@@ -1425,7 +1549,7 @@
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="40"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="9">
         <v>5</v>
       </c>
@@ -1439,7 +1563,7 @@
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="40"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="9">
         <v>6</v>
       </c>
@@ -1453,7 +1577,7 @@
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="40"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="9">
         <v>7</v>
       </c>
@@ -1467,7 +1591,7 @@
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="40"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="9">
         <v>8</v>
       </c>
@@ -1481,7 +1605,7 @@
       <c r="J35" s="4"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="40"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="9">
         <v>9</v>
       </c>
@@ -1495,7 +1619,7 @@
       <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="10">
         <v>10</v>
       </c>
@@ -1529,9 +1653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03816060-24A7-D946-9AB1-F7E07293AE02}">
   <dimension ref="A1:O249"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1553,35 +1677,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="48" t="s">
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="72" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="49" t="s">
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="75"/>
       <c r="F2" s="25" t="s">
         <v>44</v>
       </c>
@@ -1614,21 +1738,21 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="43"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="69"/>
     </row>
     <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
@@ -1641,7 +1765,7 @@
         <v>92</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H4" s="25" t="s">
         <v>92</v>
@@ -1650,7 +1774,7 @@
         <v>92</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="K4" s="26" t="s">
         <v>92</v>
@@ -1659,36 +1783,36 @@
         <v>92</v>
       </c>
       <c r="M4" s="27" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="N4" s="27" t="s">
         <v>92</v>
       </c>
       <c r="O4" t="str">
         <f>IF(OR( AND(C5=D5,OR(F4&lt;&gt;G4, I4&lt;&gt;J4,L4&lt;&gt;M4)),  AND(D5=E5,OR(G4&lt;&gt;H4,J4&lt;&gt;K4,M4&lt;&gt;N4)), AND(C5=E5, OR(F4&lt;&gt;H4,I4&lt;&gt;K4,L4&lt;&gt;N4) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="32"/>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="E5" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="50"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="58"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="64"/>
     </row>
     <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="32" t="s">
@@ -1701,7 +1825,7 @@
         <v>92</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="H6" s="25" t="s">
         <v>92</v>
@@ -1710,7 +1834,7 @@
         <v>92</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="K6" s="26" t="s">
         <v>92</v>
@@ -1719,36 +1843,36 @@
         <v>92</v>
       </c>
       <c r="M6" s="27" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="N6" s="27" t="s">
         <v>92</v>
       </c>
       <c r="O6" t="str">
         <f>IF(OR( AND(C7=D7,OR(F6&lt;&gt;G6, I6&lt;&gt;J6,L6&lt;&gt;M6)),  AND(D7=E7,OR(G6&lt;&gt;H6,J6&lt;&gt;K6,M6&lt;&gt;N6)), AND(C7=E7, OR(F6&lt;&gt;H6,I6&lt;&gt;K6,L6&lt;&gt;N6) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="372" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="32"/>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="61" t="s">
+      <c r="E7" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="50"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="57"/>
-      <c r="N7" s="58"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="64"/>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="32" t="s">
@@ -1757,18 +1881,36 @@
       <c r="C8" s="28"/>
       <c r="D8" s="29"/>
       <c r="E8" s="30"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
+      <c r="F8" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="N8" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="O8" t="str">
         <f>IF(OR( AND(C9=D9,OR(F8&lt;&gt;G8, I8&lt;&gt;J8,L8&lt;&gt;M8)),  AND(D9=E9,OR(G8&lt;&gt;H8,J8&lt;&gt;K8,M8&lt;&gt;N8)), AND(C9=E9, OR(F8&lt;&gt;H8,I8&lt;&gt;K8,L8&lt;&gt;N8) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="255" customHeight="1" x14ac:dyDescent="0.2">
@@ -1782,35 +1924,35 @@
       <c r="E9" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="50"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="57"/>
-      <c r="N9" s="58"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="64"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="43"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="69"/>
     </row>
     <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="32" t="s">
@@ -1819,58 +1961,58 @@
       <c r="C11" s="28"/>
       <c r="D11" s="29"/>
       <c r="E11" s="33"/>
-      <c r="F11" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H11" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I11" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K11" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L11" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M11" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N11" s="66" t="s">
+      <c r="F11" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M11" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="N11" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O11" t="str">
         <f>IF(OR( AND(C12=D12,OR(F11&lt;&gt;G11, I11&lt;&gt;J11,L11&lt;&gt;M11)),  AND(D12=E12,OR(G11&lt;&gt;H11,J11&lt;&gt;K11,M11&lt;&gt;N11)), AND(C12=E12, OR(F11&lt;&gt;H11,I11&lt;&gt;K11,L11&lt;&gt;N11) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="404" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="32"/>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="62" t="s">
+      <c r="E12" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="58"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="64"/>
     </row>
     <row r="13" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="32" t="s">
@@ -1879,58 +2021,58 @@
       <c r="C13" s="28"/>
       <c r="D13" s="29"/>
       <c r="E13" s="33"/>
-      <c r="F13" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G13" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H13" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J13" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K13" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L13" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M13" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N13" s="66" t="s">
+      <c r="F13" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="K13" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L13" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M13" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="N13" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O13" t="str">
         <f>IF(OR( AND(C14=D14,OR(F13&lt;&gt;G13, I13&lt;&gt;J13,L13&lt;&gt;M13)),  AND(D14=E14,OR(G13&lt;&gt;H13,J13&lt;&gt;K13,M13&lt;&gt;N13)), AND(C14=E14, OR(F13&lt;&gt;H13,I13&lt;&gt;K13,L13&lt;&gt;N13) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="344" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="32"/>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="62" t="s">
+      <c r="E14" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="58"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="64"/>
     </row>
     <row r="15" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="32" t="s">
@@ -1939,78 +2081,78 @@
       <c r="C15" s="28"/>
       <c r="D15" s="29"/>
       <c r="E15" s="33"/>
-      <c r="F15" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H15" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I15" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J15" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K15" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L15" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M15" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N15" s="66" t="s">
+      <c r="F15" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="K15" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M15" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="N15" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O15" t="str">
         <f>IF(OR( AND(C16=D16,OR(F15&lt;&gt;G15, I15&lt;&gt;J15,L15&lt;&gt;M15)),  AND(D16=E16,OR(G15&lt;&gt;H15,J15&lt;&gt;K15,M15&lt;&gt;N15)), AND(C16=E16, OR(F15&lt;&gt;H15,I15&lt;&gt;K15,L15&lt;&gt;N15) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="340" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="32"/>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="62" t="s">
+      <c r="E16" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="50"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="58"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="64"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>3</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="43"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="69"/>
     </row>
     <row r="18" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="32" t="s">
@@ -2019,58 +2161,58 @@
       <c r="C18" s="28"/>
       <c r="D18" s="29"/>
       <c r="E18" s="33"/>
-      <c r="F18" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G18" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I18" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K18" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L18" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M18" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N18" s="66" t="s">
+      <c r="F18" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="K18" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M18" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="N18" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O18" t="str">
         <f>IF(OR( AND(C19=D19,OR(F18&lt;&gt;G18, I18&lt;&gt;J18,L18&lt;&gt;M18)),  AND(D19=E19,OR(G18&lt;&gt;H18,J18&lt;&gt;K18,M18&lt;&gt;N18)), AND(C19=E19, OR(F18&lt;&gt;H18,I18&lt;&gt;K18,L18&lt;&gt;N18) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="32"/>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="62" t="s">
+      <c r="E19" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="55"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="58"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="64"/>
     </row>
     <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="32" t="s">
@@ -2079,58 +2221,58 @@
       <c r="C20" s="28"/>
       <c r="D20" s="29"/>
       <c r="E20" s="33"/>
-      <c r="F20" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H20" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I20" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J20" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K20" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L20" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M20" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N20" s="66" t="s">
+      <c r="F20" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L20" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M20" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="N20" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O20" t="str">
         <f>IF(OR( AND(C21=D21,OR(F20&lt;&gt;G20, I20&lt;&gt;J20,L20&lt;&gt;M20)),  AND(D21=E21,OR(G20&lt;&gt;H20,J20&lt;&gt;K20,M20&lt;&gt;N20)), AND(C21=E21, OR(F20&lt;&gt;H20,I20&lt;&gt;K20,L20&lt;&gt;N20) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="404" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="32"/>
-      <c r="C21" s="59" t="s">
+      <c r="C21" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="62" t="s">
+      <c r="E21" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="50"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="58"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="64"/>
     </row>
     <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="32" t="s">
@@ -2139,78 +2281,78 @@
       <c r="C22" s="28"/>
       <c r="D22" s="29"/>
       <c r="E22" s="37"/>
-      <c r="F22" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G22" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J22" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K22" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L22" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M22" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N22" s="66" t="s">
+      <c r="F22" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J22" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="K22" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L22" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M22" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="N22" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O22" t="str">
         <f>IF(OR( AND(C23=D23,OR(F22&lt;&gt;G22, I22&lt;&gt;J22,L22&lt;&gt;M22)),  AND(D23=E23,OR(G22&lt;&gt;H22,J22&lt;&gt;K22,M22&lt;&gt;N22)), AND(C23=E23, OR(F22&lt;&gt;H22,I22&lt;&gt;K22,L22&lt;&gt;N22) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="372" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="32"/>
-      <c r="C23" s="59" t="s">
+      <c r="C23" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="60" t="s">
+      <c r="D23" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="67" t="s">
+      <c r="E23" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="50"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="58"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="64"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>4</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="43"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="69"/>
     </row>
     <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B25" s="32" t="s">
@@ -2219,118 +2361,118 @@
       <c r="C25" s="38"/>
       <c r="D25" s="29"/>
       <c r="E25" s="30"/>
-      <c r="F25" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H25" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J25" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K25" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L25" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M25" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N25" s="66" t="s">
+      <c r="F25" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="K25" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L25" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M25" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="N25" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O25" t="str">
         <f>IF(OR( AND(C26=D26,OR(F25&lt;&gt;G25, I25&lt;&gt;J25,L25&lt;&gt;M25)),  AND(D26=E26,OR(G25&lt;&gt;H25,J25&lt;&gt;K25,M25&lt;&gt;N25)), AND(C26=E26, OR(F25&lt;&gt;H25,I25&lt;&gt;K25,L25&lt;&gt;N25) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="272" x14ac:dyDescent="0.2">
       <c r="B26" s="32"/>
-      <c r="C26" s="68" t="s">
+      <c r="C26" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="60" t="s">
+      <c r="D26" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="61" t="s">
+      <c r="E26" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="F26" s="50"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="58"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="66"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="64"/>
     </row>
     <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="69"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H27" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I27" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J27" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K27" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L27" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M27" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N27" s="66" t="s">
+      <c r="C27" s="49"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I27" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J27" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="K27" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L27" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M27" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="N27" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O27" t="str">
         <f>IF(OR( AND(C28=D28,OR(F27&lt;&gt;G27, I27&lt;&gt;J27,L27&lt;&gt;M27)),  AND(D28=E28,OR(G27&lt;&gt;H27,J27&lt;&gt;K27,M27&lt;&gt;N27)), AND(C28=E28, OR(F27&lt;&gt;H27,I27&lt;&gt;K27,L27&lt;&gt;N27) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B28" s="32"/>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="61" t="s">
+      <c r="E28" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="F28" s="50"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="54"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="58"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="64"/>
     </row>
     <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="32" t="s">
@@ -2338,15 +2480,33 @@
       </c>
       <c r="D29" s="29"/>
       <c r="E29" s="30"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
+      <c r="F29" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J29" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="K29" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L29" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="M29" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="N29" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="O29" t="str">
         <f>IF(OR( AND(C30=D30,OR(F29&lt;&gt;G29, I29&lt;&gt;J29,L29&lt;&gt;M29)),  AND(D30=E30,OR(G29&lt;&gt;H29,J29&lt;&gt;K29,M29&lt;&gt;N29)), AND(C30=E30, OR(F29&lt;&gt;H29,I29&lt;&gt;K29,L29&lt;&gt;N29) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -2363,35 +2523,35 @@
       <c r="E30" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="50"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="56"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="58"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="66"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="62"/>
+      <c r="M30" s="63"/>
+      <c r="N30" s="64"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>5</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="42"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="43"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="68"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="69"/>
     </row>
     <row r="32" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="32" t="s">
@@ -2399,58 +2559,58 @@
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="30"/>
-      <c r="F32" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G32" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H32" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I32" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J32" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K32" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L32" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M32" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N32" s="66" t="s">
+      <c r="F32" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="H32" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J32" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="K32" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L32" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M32" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="N32" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O32" t="str">
         <f>IF(OR( AND(C33=D33,OR(F32&lt;&gt;G32, I32&lt;&gt;J32,L32&lt;&gt;M32)),  AND(D33=E33,OR(G32&lt;&gt;H32,J32&lt;&gt;K32,M32&lt;&gt;N32)), AND(C33=E33, OR(F32&lt;&gt;H32,I32&lt;&gt;K32,L32&lt;&gt;N32) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="289" x14ac:dyDescent="0.2">
       <c r="B33" s="32"/>
-      <c r="C33" s="59" t="s">
+      <c r="C33" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="60" t="s">
+      <c r="D33" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="61" t="s">
+      <c r="E33" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="50"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="56"/>
-      <c r="M33" s="57"/>
-      <c r="N33" s="58"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="65"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="64"/>
     </row>
     <row r="34" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" s="32" t="s">
@@ -2458,58 +2618,58 @@
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="30"/>
-      <c r="F34" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G34" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H34" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I34" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J34" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K34" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L34" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M34" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N34" s="66" t="s">
+      <c r="F34" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G34" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="H34" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J34" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="K34" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L34" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M34" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="N34" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O34" t="str">
         <f>IF(OR( AND(C35=D35,OR(F34&lt;&gt;G34, I34&lt;&gt;J34,L34&lt;&gt;M34)),  AND(D35=E35,OR(G34&lt;&gt;H34,J34&lt;&gt;K34,M34&lt;&gt;N34)), AND(C35=E35, OR(F34&lt;&gt;H34,I34&lt;&gt;K34,L34&lt;&gt;N34) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="306" x14ac:dyDescent="0.2">
       <c r="B35" s="32"/>
-      <c r="C35" s="59" t="s">
+      <c r="C35" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="60" t="s">
+      <c r="D35" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E35" s="61" t="s">
+      <c r="E35" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="55"/>
-      <c r="L35" s="56"/>
-      <c r="M35" s="57"/>
-      <c r="N35" s="58"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="66"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="62"/>
+      <c r="M35" s="63"/>
+      <c r="N35" s="64"/>
     </row>
     <row r="36" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" s="32" t="s">
@@ -2517,15 +2677,33 @@
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="30"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
+      <c r="F36" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I36" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J36" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="K36" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L36" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="M36" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="N36" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="O36" t="str">
         <f>IF(OR( AND(C37=D37,OR(F36&lt;&gt;G36, I36&lt;&gt;J36,L36&lt;&gt;M36)),  AND(D37=E37,OR(G36&lt;&gt;H36,J36&lt;&gt;K36,M36&lt;&gt;N36)), AND(C37=E37, OR(F36&lt;&gt;H36,I36&lt;&gt;K36,L36&lt;&gt;N36) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -2542,35 +2720,35 @@
       <c r="E37" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="50"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="54"/>
-      <c r="K37" s="55"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="57"/>
-      <c r="N37" s="58"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="62"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="64"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>6</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="42"/>
-      <c r="L38" s="42"/>
-      <c r="M38" s="42"/>
-      <c r="N38" s="43"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="68"/>
+      <c r="K38" s="68"/>
+      <c r="L38" s="68"/>
+      <c r="M38" s="68"/>
+      <c r="N38" s="69"/>
     </row>
     <row r="39" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B39" s="32" t="s">
@@ -2578,15 +2756,33 @@
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="30"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
+      <c r="F39" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I39" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J39" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="K39" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L39" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="M39" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N39" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="O39" t="str">
         <f>IF(OR( AND(C40=D40,OR(F39&lt;&gt;G39, I39&lt;&gt;J39,L39&lt;&gt;M39)),  AND(D40=E40,OR(G39&lt;&gt;H39,J39&lt;&gt;K39,M39&lt;&gt;N39)), AND(C40=E40, OR(F39&lt;&gt;H39,I39&lt;&gt;K39,L39&lt;&gt;N39) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -2603,15 +2799,15 @@
       <c r="E40" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="F40" s="50"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="53"/>
-      <c r="J40" s="54"/>
-      <c r="K40" s="55"/>
-      <c r="L40" s="56"/>
-      <c r="M40" s="57"/>
-      <c r="N40" s="58"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="65"/>
+      <c r="J40" s="66"/>
+      <c r="K40" s="67"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="63"/>
+      <c r="N40" s="64"/>
     </row>
     <row r="41" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B41" s="32" t="s">
@@ -2619,58 +2815,58 @@
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="30"/>
-      <c r="F41" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G41" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H41" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I41" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J41" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K41" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L41" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M41" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N41" s="66" t="s">
+      <c r="F41" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="H41" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I41" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J41" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="K41" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L41" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M41" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="N41" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O41" t="str">
         <f>IF(OR( AND(C42=D42,OR(F41&lt;&gt;G41, I41&lt;&gt;J41,L41&lt;&gt;M41)),  AND(D42=E42,OR(G41&lt;&gt;H41,J41&lt;&gt;K41,M41&lt;&gt;N41)), AND(C42=E42, OR(F41&lt;&gt;H41,I41&lt;&gt;K41,L41&lt;&gt;N41) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="340" x14ac:dyDescent="0.2">
       <c r="B42" s="32"/>
-      <c r="C42" s="59" t="s">
+      <c r="C42" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="60" t="s">
+      <c r="D42" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="61" t="s">
+      <c r="E42" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="50"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="54"/>
-      <c r="K42" s="55"/>
-      <c r="L42" s="56"/>
-      <c r="M42" s="57"/>
-      <c r="N42" s="58"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="65"/>
+      <c r="J42" s="66"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="64"/>
     </row>
     <row r="43" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B43" s="32" t="s">
@@ -2678,21 +2874,39 @@
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="30"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
-      <c r="K43" s="26"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="27"/>
-      <c r="N43" s="27"/>
+      <c r="F43" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G43" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H43" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I43" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J43" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="K43" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L43" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="M43" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="N43" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="O43" t="str">
         <f>IF(OR( AND(C44=D44,OR(F43&lt;&gt;G43, I43&lt;&gt;J43,L43&lt;&gt;M43)),  AND(D44=E44,OR(G43&lt;&gt;H43,J43&lt;&gt;K43,M43&lt;&gt;N43)), AND(C44=E44, OR(F43&lt;&gt;H43,I43&lt;&gt;K43,L43&lt;&gt;N43) )), "error: different mark to same abstract","")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="409.5" x14ac:dyDescent="0.2">
       <c r="B44" s="32"/>
       <c r="C44" s="28" t="s">
         <v>65</v>
@@ -2703,35 +2917,35 @@
       <c r="E44" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F44" s="50"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="54"/>
-      <c r="K44" s="55"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="57"/>
-      <c r="N44" s="58"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="61"/>
+      <c r="I44" s="65"/>
+      <c r="J44" s="66"/>
+      <c r="K44" s="67"/>
+      <c r="L44" s="62"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="64"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>7</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
-      <c r="K45" s="42"/>
-      <c r="L45" s="42"/>
-      <c r="M45" s="42"/>
-      <c r="N45" s="43"/>
+      <c r="C45" s="68"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="68"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="68"/>
+      <c r="H45" s="68"/>
+      <c r="I45" s="68"/>
+      <c r="J45" s="68"/>
+      <c r="K45" s="68"/>
+      <c r="L45" s="68"/>
+      <c r="M45" s="68"/>
+      <c r="N45" s="69"/>
     </row>
     <row r="46" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B46" s="32" t="s">
@@ -2739,58 +2953,58 @@
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="30"/>
-      <c r="F46" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G46" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H46" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I46" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J46" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K46" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L46" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M46" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N46" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="O46" t="str">
-        <f>IF(OR( AND(C47=D47,OR(F46&lt;&gt;G46, I46&lt;&gt;J46,L46&lt;&gt;M46)),  AND(D47=E47,OR(G46&lt;&gt;H46,J46&lt;&gt;K46,M46&lt;&gt;N46)), AND(C47=E47, OR(F46&lt;&gt;H46,I46&lt;&gt;K46,L46&lt;&gt;N46) )), "error: different mark to same abstract","")</f>
-        <v/>
+      <c r="F46" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="H46" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I46" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J46" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="K46" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L46" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M46" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="N46" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="O46" t="e">
+        <f>IF(OR( AND(C47=D47,OR(F46&lt;&gt;G46, I46&lt;&gt;J46,L46&lt;&gt;#REF!)),  AND(D47=E47,OR(G46&lt;&gt;H46,J46&lt;&gt;K46,#REF!&lt;&gt;N46)), AND(C47=E47, OR(F46&lt;&gt;H46,I46&lt;&gt;K46,L46&lt;&gt;N46) )), "error: different mark to same abstract","")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="32"/>
-      <c r="C47" s="59" t="s">
+      <c r="C47" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D47" s="60" t="s">
+      <c r="D47" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="E47" s="61" t="s">
+      <c r="E47" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="F47" s="50"/>
-      <c r="G47" s="51"/>
-      <c r="H47" s="52"/>
-      <c r="I47" s="53"/>
-      <c r="J47" s="54"/>
-      <c r="K47" s="55"/>
-      <c r="L47" s="56"/>
-      <c r="M47" s="57"/>
-      <c r="N47" s="58"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="65"/>
+      <c r="J47" s="66"/>
+      <c r="K47" s="67"/>
+      <c r="L47" s="62"/>
+      <c r="M47" s="63"/>
+      <c r="N47" s="64"/>
     </row>
     <row r="48" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B48" s="32" t="s">
@@ -2798,58 +3012,58 @@
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="30"/>
-      <c r="F48" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G48" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H48" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I48" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J48" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K48" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L48" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M48" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N48" s="66" t="s">
+      <c r="F48" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="H48" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I48" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J48" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="K48" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L48" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M48" s="76" t="s">
+        <v>102</v>
+      </c>
+      <c r="N48" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O48" t="str">
         <f>IF(OR( AND(C49=D49,OR(F48&lt;&gt;G48, I48&lt;&gt;J48,L48&lt;&gt;M48)),  AND(D49=E49,OR(G48&lt;&gt;H48,J48&lt;&gt;K48,M48&lt;&gt;N48)), AND(C49=E49, OR(F48&lt;&gt;H48,I48&lt;&gt;K48,L48&lt;&gt;N48) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="32"/>
-      <c r="C49" s="59" t="s">
+      <c r="C49" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="D49" s="60" t="s">
+      <c r="D49" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="E49" s="61" t="s">
+      <c r="E49" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="F49" s="50"/>
-      <c r="G49" s="51"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="53"/>
-      <c r="J49" s="54"/>
-      <c r="K49" s="55"/>
-      <c r="L49" s="56"/>
-      <c r="M49" s="57"/>
-      <c r="N49" s="58"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="61"/>
+      <c r="I49" s="65"/>
+      <c r="J49" s="66"/>
+      <c r="K49" s="67"/>
+      <c r="L49" s="62"/>
+      <c r="M49" s="63"/>
+      <c r="N49" s="64"/>
     </row>
     <row r="50" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B50" s="32" t="s">
@@ -2857,15 +3071,33 @@
       </c>
       <c r="D50" s="29"/>
       <c r="E50" s="30"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="26"/>
-      <c r="K50" s="26"/>
-      <c r="L50" s="27"/>
-      <c r="M50" s="27"/>
-      <c r="N50" s="27"/>
+      <c r="F50" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G50" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="H50" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I50" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J50" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="K50" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L50" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="M50" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="N50" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="O50" t="str">
         <f>IF(OR( AND(C51=D51,OR(F50&lt;&gt;G50, I50&lt;&gt;J50,L50&lt;&gt;M50)),  AND(D51=E51,OR(G50&lt;&gt;H50,J50&lt;&gt;K50,M50&lt;&gt;N50)), AND(C51=E51, OR(F50&lt;&gt;H50,I50&lt;&gt;K50,L50&lt;&gt;N50) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -2882,35 +3114,35 @@
       <c r="E51" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="F51" s="50"/>
-      <c r="G51" s="51"/>
-      <c r="H51" s="52"/>
-      <c r="I51" s="53"/>
-      <c r="J51" s="54"/>
-      <c r="K51" s="55"/>
-      <c r="L51" s="56"/>
-      <c r="M51" s="57"/>
-      <c r="N51" s="58"/>
+      <c r="F51" s="59"/>
+      <c r="G51" s="60"/>
+      <c r="H51" s="61"/>
+      <c r="I51" s="65"/>
+      <c r="J51" s="66"/>
+      <c r="K51" s="67"/>
+      <c r="L51" s="62"/>
+      <c r="M51" s="63"/>
+      <c r="N51" s="64"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>8</v>
       </c>
-      <c r="B52" s="42" t="s">
+      <c r="B52" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="42"/>
-      <c r="J52" s="42"/>
-      <c r="K52" s="42"/>
-      <c r="L52" s="42"/>
-      <c r="M52" s="42"/>
-      <c r="N52" s="43"/>
+      <c r="C52" s="68"/>
+      <c r="D52" s="68"/>
+      <c r="E52" s="68"/>
+      <c r="F52" s="68"/>
+      <c r="G52" s="68"/>
+      <c r="H52" s="68"/>
+      <c r="I52" s="68"/>
+      <c r="J52" s="68"/>
+      <c r="K52" s="68"/>
+      <c r="L52" s="68"/>
+      <c r="M52" s="68"/>
+      <c r="N52" s="69"/>
     </row>
     <row r="53" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B53" s="32" t="s">
@@ -2918,58 +3150,58 @@
       </c>
       <c r="D53" s="29"/>
       <c r="E53" s="30"/>
-      <c r="F53" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G53" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H53" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I53" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J53" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K53" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L53" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M53" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N53" s="66" t="s">
+      <c r="F53" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="H53" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I53" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J53" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="K53" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L53" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M53" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N53" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O53" t="str">
-        <f>IF(OR( AND(C54=D54,OR(F53&lt;&gt;G53, I53&lt;&gt;J53,L53&lt;&gt;M53)),  AND(D54=E54,OR(G53&lt;&gt;H53,J53&lt;&gt;K53,M53&lt;&gt;N53)), AND(C54=E54, OR(F53&lt;&gt;H53,I53&lt;&gt;K53,L53&lt;&gt;N53) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <f>IF(OR( AND(C54=D54,OR(F53&lt;&gt;G53, I53&lt;&gt;J53,L53&lt;&gt;M46)),  AND(D54=E54,OR(G53&lt;&gt;H53,J53&lt;&gt;K53,M46&lt;&gt;N53)), AND(C54=E54, OR(F53&lt;&gt;H53,I53&lt;&gt;K53,L53&lt;&gt;N53) )), "error: different mark to same abstract","")</f>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="340" x14ac:dyDescent="0.2">
       <c r="B54" s="32"/>
-      <c r="C54" s="59" t="s">
+      <c r="C54" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="D54" s="60" t="s">
+      <c r="D54" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E54" s="61" t="s">
+      <c r="E54" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="F54" s="50"/>
-      <c r="G54" s="51"/>
-      <c r="H54" s="52"/>
-      <c r="I54" s="53"/>
-      <c r="J54" s="54"/>
-      <c r="K54" s="55"/>
-      <c r="L54" s="56"/>
-      <c r="M54" s="57"/>
-      <c r="N54" s="58"/>
+      <c r="F54" s="59"/>
+      <c r="G54" s="60"/>
+      <c r="H54" s="61"/>
+      <c r="I54" s="65"/>
+      <c r="J54" s="66"/>
+      <c r="K54" s="67"/>
+      <c r="L54" s="62"/>
+      <c r="M54" s="63"/>
+      <c r="N54" s="64"/>
     </row>
     <row r="55" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B55" s="32" t="s">
@@ -2977,58 +3209,58 @@
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="30"/>
-      <c r="F55" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G55" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H55" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I55" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J55" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K55" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L55" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M55" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N55" s="66" t="s">
+      <c r="F55" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G55" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H55" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I55" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J55" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="K55" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L55" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M55" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="N55" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O55" t="str">
         <f>IF(OR( AND(C56=D56,OR(F55&lt;&gt;G55, I55&lt;&gt;J55,L55&lt;&gt;M55)),  AND(D56=E56,OR(G55&lt;&gt;H55,J55&lt;&gt;K55,M55&lt;&gt;N55)), AND(C56=E56, OR(F55&lt;&gt;H55,I55&lt;&gt;K55,L55&lt;&gt;N55) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B56" s="32"/>
-      <c r="C56" s="59" t="s">
+      <c r="C56" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="D56" s="60" t="s">
+      <c r="D56" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="E56" s="61" t="s">
+      <c r="E56" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="F56" s="50"/>
-      <c r="G56" s="51"/>
-      <c r="H56" s="52"/>
-      <c r="I56" s="53"/>
-      <c r="J56" s="54"/>
-      <c r="K56" s="55"/>
-      <c r="L56" s="56"/>
-      <c r="M56" s="57"/>
-      <c r="N56" s="58"/>
+      <c r="F56" s="59"/>
+      <c r="G56" s="60"/>
+      <c r="H56" s="61"/>
+      <c r="I56" s="65"/>
+      <c r="J56" s="66"/>
+      <c r="K56" s="67"/>
+      <c r="L56" s="62"/>
+      <c r="M56" s="63"/>
+      <c r="N56" s="64"/>
     </row>
     <row r="57" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B57" s="32" t="s">
@@ -3036,18 +3268,36 @@
       </c>
       <c r="D57" s="29"/>
       <c r="E57" s="30"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="25"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="26"/>
-      <c r="K57" s="26"/>
-      <c r="L57" s="27"/>
-      <c r="M57" s="27"/>
-      <c r="N57" s="27"/>
+      <c r="F57" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G57" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="H57" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I57" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J57" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="K57" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L57" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="M57" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="N57" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="O57" t="str">
         <f>IF(OR( AND(C58=D58,OR(F57&lt;&gt;G57, I57&lt;&gt;J57,L57&lt;&gt;M57)),  AND(D58=E58,OR(G57&lt;&gt;H57,J57&lt;&gt;K57,M57&lt;&gt;N57)), AND(C58=E58, OR(F57&lt;&gt;H57,I57&lt;&gt;K57,L57&lt;&gt;N57) )), "error: different mark to same abstract","")</f>
-        <v/>
+        <v>error: different mark to same abstract</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
@@ -3061,35 +3311,35 @@
       <c r="E58" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="F58" s="50"/>
-      <c r="G58" s="51"/>
-      <c r="H58" s="52"/>
-      <c r="I58" s="53"/>
-      <c r="J58" s="54"/>
-      <c r="K58" s="55"/>
-      <c r="L58" s="56"/>
-      <c r="M58" s="57"/>
-      <c r="N58" s="58"/>
+      <c r="F58" s="59"/>
+      <c r="G58" s="60"/>
+      <c r="H58" s="61"/>
+      <c r="I58" s="65"/>
+      <c r="J58" s="66"/>
+      <c r="K58" s="67"/>
+      <c r="L58" s="62"/>
+      <c r="M58" s="63"/>
+      <c r="N58" s="64"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>9</v>
       </c>
-      <c r="B59" s="42" t="s">
+      <c r="B59" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="42"/>
-      <c r="D59" s="42"/>
-      <c r="E59" s="42"/>
-      <c r="F59" s="42"/>
-      <c r="G59" s="42"/>
-      <c r="H59" s="42"/>
-      <c r="I59" s="42"/>
-      <c r="J59" s="42"/>
-      <c r="K59" s="42"/>
-      <c r="L59" s="42"/>
-      <c r="M59" s="42"/>
-      <c r="N59" s="43"/>
+      <c r="C59" s="68"/>
+      <c r="D59" s="68"/>
+      <c r="E59" s="68"/>
+      <c r="F59" s="68"/>
+      <c r="G59" s="68"/>
+      <c r="H59" s="68"/>
+      <c r="I59" s="68"/>
+      <c r="J59" s="68"/>
+      <c r="K59" s="68"/>
+      <c r="L59" s="68"/>
+      <c r="M59" s="68"/>
+      <c r="N59" s="69"/>
     </row>
     <row r="60" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B60" s="32" t="s">
@@ -3097,31 +3347,31 @@
       </c>
       <c r="D60" s="29"/>
       <c r="E60" s="30"/>
-      <c r="F60" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G60" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H60" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I60" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J60" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K60" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L60" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M60" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N60" s="66" t="s">
+      <c r="F60" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G60" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="H60" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I60" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J60" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="K60" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L60" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M60" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="N60" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O60" t="str">
@@ -3131,24 +3381,24 @@
     </row>
     <row r="61" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="32"/>
-      <c r="C61" s="59" t="s">
+      <c r="C61" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="D61" s="60" t="s">
+      <c r="D61" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="E61" s="61" t="s">
+      <c r="E61" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="F61" s="50"/>
-      <c r="G61" s="51"/>
-      <c r="H61" s="52"/>
-      <c r="I61" s="53"/>
-      <c r="J61" s="54"/>
-      <c r="K61" s="55"/>
-      <c r="L61" s="56"/>
-      <c r="M61" s="57"/>
-      <c r="N61" s="58"/>
+      <c r="F61" s="59"/>
+      <c r="G61" s="60"/>
+      <c r="H61" s="61"/>
+      <c r="I61" s="65"/>
+      <c r="J61" s="66"/>
+      <c r="K61" s="67"/>
+      <c r="L61" s="62"/>
+      <c r="M61" s="63"/>
+      <c r="N61" s="64"/>
     </row>
     <row r="62" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B62" s="32" t="s">
@@ -3156,15 +3406,33 @@
       </c>
       <c r="D62" s="29"/>
       <c r="E62" s="30"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
-      <c r="I62" s="26"/>
-      <c r="J62" s="26"/>
-      <c r="K62" s="26"/>
-      <c r="L62" s="27"/>
-      <c r="M62" s="27"/>
-      <c r="N62" s="27"/>
+      <c r="F62" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G62" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H62" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I62" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J62" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="K62" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L62" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="M62" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="N62" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="O62" t="str">
         <f>IF(OR( AND(C63=D63,OR(F62&lt;&gt;G62, I62&lt;&gt;J62,L62&lt;&gt;M62)),  AND(D63=E63,OR(G62&lt;&gt;H62,J62&lt;&gt;K62,M62&lt;&gt;N62)), AND(C63=E63, OR(F62&lt;&gt;H62,I62&lt;&gt;K62,L62&lt;&gt;N62) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -3181,15 +3449,15 @@
       <c r="E63" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="F63" s="50"/>
-      <c r="G63" s="51"/>
-      <c r="H63" s="52"/>
-      <c r="I63" s="53"/>
-      <c r="J63" s="54"/>
-      <c r="K63" s="55"/>
-      <c r="L63" s="56"/>
-      <c r="M63" s="57"/>
-      <c r="N63" s="58"/>
+      <c r="F63" s="59"/>
+      <c r="G63" s="60"/>
+      <c r="H63" s="61"/>
+      <c r="I63" s="65"/>
+      <c r="J63" s="66"/>
+      <c r="K63" s="67"/>
+      <c r="L63" s="62"/>
+      <c r="M63" s="63"/>
+      <c r="N63" s="64"/>
       <c r="O63" s="1"/>
     </row>
     <row r="64" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -3198,15 +3466,33 @@
       </c>
       <c r="D64" s="29"/>
       <c r="E64" s="30"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
-      <c r="I64" s="26"/>
-      <c r="J64" s="26"/>
-      <c r="K64" s="26"/>
-      <c r="L64" s="27"/>
-      <c r="M64" s="27"/>
-      <c r="N64" s="27"/>
+      <c r="F64" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G64" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H64" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I64" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J64" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="K64" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="L64" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="M64" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="N64" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="O64" t="str">
         <f>IF(OR( AND(C65=D65,OR(F64&lt;&gt;G64, I64&lt;&gt;J64,L64&lt;&gt;M64)),  AND(D65=E65,OR(G64&lt;&gt;H64,J64&lt;&gt;K64,M64&lt;&gt;N64)), AND(C65=E65, OR(F64&lt;&gt;H64,I64&lt;&gt;K64,L64&lt;&gt;N64) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -3223,35 +3509,35 @@
       <c r="E65" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="F65" s="50"/>
-      <c r="G65" s="51"/>
-      <c r="H65" s="52"/>
-      <c r="I65" s="53"/>
-      <c r="J65" s="54"/>
-      <c r="K65" s="55"/>
-      <c r="L65" s="56"/>
-      <c r="M65" s="57"/>
-      <c r="N65" s="58"/>
+      <c r="F65" s="59"/>
+      <c r="G65" s="60"/>
+      <c r="H65" s="61"/>
+      <c r="I65" s="65"/>
+      <c r="J65" s="66"/>
+      <c r="K65" s="67"/>
+      <c r="L65" s="62"/>
+      <c r="M65" s="63"/>
+      <c r="N65" s="64"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>10</v>
       </c>
-      <c r="B66" s="42" t="s">
+      <c r="B66" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="42"/>
-      <c r="D66" s="42"/>
-      <c r="E66" s="42"/>
-      <c r="F66" s="42"/>
-      <c r="G66" s="42"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="42"/>
-      <c r="J66" s="42"/>
-      <c r="K66" s="42"/>
-      <c r="L66" s="42"/>
-      <c r="M66" s="42"/>
-      <c r="N66" s="43"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="68"/>
+      <c r="H66" s="68"/>
+      <c r="I66" s="68"/>
+      <c r="J66" s="68"/>
+      <c r="K66" s="68"/>
+      <c r="L66" s="68"/>
+      <c r="M66" s="68"/>
+      <c r="N66" s="69"/>
     </row>
     <row r="67" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B67" s="32" t="s">
@@ -3259,31 +3545,31 @@
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="30"/>
-      <c r="F67" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G67" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H67" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I67" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J67" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K67" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L67" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M67" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N67" s="66" t="s">
+      <c r="F67" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G67" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="H67" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I67" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J67" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="K67" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L67" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M67" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="N67" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O67" t="str">
@@ -3293,57 +3579,57 @@
     </row>
     <row r="68" spans="1:15" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="32"/>
-      <c r="C68" s="59" t="s">
+      <c r="C68" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="D68" s="60" t="s">
+      <c r="D68" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="E68" s="61" t="s">
+      <c r="E68" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="F68" s="50"/>
-      <c r="G68" s="51"/>
-      <c r="H68" s="52"/>
-      <c r="I68" s="53"/>
-      <c r="J68" s="54"/>
-      <c r="K68" s="55"/>
-      <c r="L68" s="56"/>
-      <c r="M68" s="57"/>
-      <c r="N68" s="58"/>
+      <c r="F68" s="59"/>
+      <c r="G68" s="60"/>
+      <c r="H68" s="61"/>
+      <c r="I68" s="65"/>
+      <c r="J68" s="66"/>
+      <c r="K68" s="67"/>
+      <c r="L68" s="62"/>
+      <c r="M68" s="63"/>
+      <c r="N68" s="64"/>
     </row>
     <row r="69" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C69" s="69"/>
-      <c r="D69" s="60"/>
-      <c r="E69" s="61"/>
-      <c r="F69" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G69" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H69" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I69" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J69" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K69" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L69" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M69" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N69" s="66" t="s">
+      <c r="C69" s="49"/>
+      <c r="D69" s="40"/>
+      <c r="E69" s="41"/>
+      <c r="F69" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G69" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="H69" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I69" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J69" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="K69" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L69" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M69" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="N69" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O69" t="str">
@@ -3353,57 +3639,57 @@
     </row>
     <row r="70" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="32"/>
-      <c r="C70" s="59" t="s">
+      <c r="C70" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="D70" s="60" t="s">
+      <c r="D70" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E70" s="61" t="s">
+      <c r="E70" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="F70" s="50"/>
-      <c r="G70" s="51"/>
-      <c r="H70" s="52"/>
-      <c r="I70" s="53"/>
-      <c r="J70" s="54"/>
-      <c r="K70" s="55"/>
-      <c r="L70" s="56"/>
-      <c r="M70" s="57"/>
-      <c r="N70" s="58"/>
+      <c r="F70" s="59"/>
+      <c r="G70" s="60"/>
+      <c r="H70" s="61"/>
+      <c r="I70" s="65"/>
+      <c r="J70" s="66"/>
+      <c r="K70" s="67"/>
+      <c r="L70" s="62"/>
+      <c r="M70" s="63"/>
+      <c r="N70" s="64"/>
     </row>
     <row r="71" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C71" s="59"/>
-      <c r="D71" s="60"/>
-      <c r="E71" s="61"/>
-      <c r="F71" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="G71" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="H71" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="I71" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="J71" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="K71" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="L71" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="M71" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="N71" s="66" t="s">
+      <c r="C71" s="39"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="41"/>
+      <c r="F71" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="G71" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="H71" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="I71" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J71" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="K71" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L71" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="M71" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="N71" s="46" t="s">
         <v>92</v>
       </c>
       <c r="O71" t="str">
@@ -3413,24 +3699,24 @@
     </row>
     <row r="72" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="32"/>
-      <c r="C72" s="59" t="s">
+      <c r="C72" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="D72" s="60" t="s">
+      <c r="D72" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E72" s="61" t="s">
+      <c r="E72" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="F72" s="50"/>
-      <c r="G72" s="51"/>
-      <c r="H72" s="52"/>
-      <c r="I72" s="53"/>
-      <c r="J72" s="54"/>
-      <c r="K72" s="55"/>
-      <c r="L72" s="56"/>
-      <c r="M72" s="57"/>
-      <c r="N72" s="58"/>
+      <c r="F72" s="59"/>
+      <c r="G72" s="60"/>
+      <c r="H72" s="61"/>
+      <c r="I72" s="65"/>
+      <c r="J72" s="66"/>
+      <c r="K72" s="67"/>
+      <c r="L72" s="62"/>
+      <c r="M72" s="63"/>
+      <c r="N72" s="64"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C73"/>
@@ -3447,11 +3733,11 @@
       <c r="N73" s="1"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C74" s="70" t="s">
+      <c r="C74" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="D74" s="70"/>
-      <c r="E74" s="70"/>
+      <c r="D74" s="58"/>
+      <c r="E74" s="58"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
@@ -3514,7 +3800,7 @@
       <c r="N77" s="1"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C78" s="71"/>
+      <c r="C78"/>
       <c r="D78"/>
       <c r="E78"/>
       <c r="F78" s="1"/>
@@ -5769,6 +6055,89 @@
     </row>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="B10:N10"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L70:N70"/>
+    <mergeCell ref="I70:K70"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="B17:N17"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="B66:N66"/>
+    <mergeCell ref="B59:N59"/>
+    <mergeCell ref="B52:N52"/>
+    <mergeCell ref="B45:N45"/>
+    <mergeCell ref="B38:N38"/>
+    <mergeCell ref="B31:N31"/>
+    <mergeCell ref="B24:N24"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="L72:N72"/>
+    <mergeCell ref="I72:K72"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="L58:N58"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="I61:K61"/>
+    <mergeCell ref="L61:N61"/>
+    <mergeCell ref="L63:N63"/>
+    <mergeCell ref="I63:K63"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="L65:N65"/>
+    <mergeCell ref="I65:K65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="L68:N68"/>
+    <mergeCell ref="I68:K68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="L47:N47"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="L51:N51"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="L49:N49"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="L44:N44"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="F44:H44"/>
     <mergeCell ref="C74:E74"/>
     <mergeCell ref="F23:H23"/>
     <mergeCell ref="L21:N21"/>
@@ -5793,89 +6162,6 @@
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="L37:N37"/>
     <mergeCell ref="I37:K37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="L44:N44"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="L47:N47"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="L51:N51"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="L49:N49"/>
-    <mergeCell ref="I49:K49"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="L56:N56"/>
-    <mergeCell ref="I56:K56"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="L72:N72"/>
-    <mergeCell ref="I72:K72"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="L58:N58"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="I61:K61"/>
-    <mergeCell ref="L61:N61"/>
-    <mergeCell ref="L63:N63"/>
-    <mergeCell ref="I63:K63"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="L65:N65"/>
-    <mergeCell ref="I65:K65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="L68:N68"/>
-    <mergeCell ref="I68:K68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="L70:N70"/>
-    <mergeCell ref="I70:K70"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="B17:N17"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B10:N10"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="B66:N66"/>
-    <mergeCell ref="B59:N59"/>
-    <mergeCell ref="B52:N52"/>
-    <mergeCell ref="B45:N45"/>
-    <mergeCell ref="B38:N38"/>
-    <mergeCell ref="B31:N31"/>
-    <mergeCell ref="B24:N24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5885,7 +6171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1AA851-AA00-BA45-955A-1248E058A2EC}">
   <dimension ref="B3:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -5895,68 +6181,68 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
     </row>
     <row r="4" spans="2:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="73" t="e">
+      <c r="C4" s="51" t="e">
         <f>'Subjective scores'!C75</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
     </row>
     <row r="5" spans="2:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="73" t="e">
+      <c r="C5" s="51" t="e">
         <f>'Subjective scores'!D75</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
     </row>
     <row r="6" spans="2:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="73" t="e">
+      <c r="C6" s="51" t="e">
         <f>'Subjective scores'!E75</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Matteo] Filled in with my votes
</commit_message>
<xml_diff>
--- a/project/evaluation/qualitative_evaluation/qualitative_evaluation_table.xlsx
+++ b/project/evaluation/qualitative_evaluation/qualitative_evaluation_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteom/shared-folder/nlpt_group/project/evaluation/qualitative_evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB793C72-91C7-8F43-8352-7AF49A985885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C27056F-2193-9542-AC01-25F6A00113DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{BFF5F178-14AB-6B4F-B81C-3E61E0B93405}"/>
+    <workbookView xWindow="28800" yWindow="-5940" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{BFF5F178-14AB-6B4F-B81C-3E61E0B93405}"/>
   </bookViews>
   <sheets>
     <sheet name="Correct retrieval" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="92">
   <si>
     <t>Comparison queries:</t>
   </si>
@@ -185,24 +185,9 @@
     <t xml:space="preserve">Score </t>
   </si>
   <si>
-    <t>Bipolar disorder BD over the long term can manifest a variety of outcomes depending on a number of different conditions There is a need for further knowledge regarding preventive factors as well as predictors of the disabling course of the disorder Studies regarding the impact on functional outcome of premorbid and current general intellectual function intelligence quotient IQ and premorbid functioning in BD patients are sparse The present study addressed the role of premorbid functioning assessed with the Premorbid Adjustment Scale PAS intelligence course of illness and sociodemographics on occupational outcome in BD Bipolar disorder patients were recruited consecutively from psychiatric units outpatient and inpatient in four major hospitals in Oslo Norway N 226 644 bipolar I disorder BDI 301 bipolar II disorder BDII 55 bipolar disorder not otherwise specified BDNOS 386 males The associations between current IQ premorbid IQ assessed using the National Adult Reading Test NART PAS clinical and sociodemographic characteristics and receipt of disability benefit were analysed using descriptive statistics and logistic regression analyses The number of hospitalizations for depressive episodes and illness duration was associated with a higher risk of receipt of disability benefit PAS premorbid and current IQ as well as decline in IQ did not explain the higher risk of receipt of disability benefits Severe clinical course of BD was associated with receipt of disability benefit Occupational outcome was unrelated to PAS premorbid and current IQ as well as decline in IQ This suggests that the persistence of severe clinical symptoms rather than global cognitive functioning determines occupational outcome in BD and emphasizes the protective potential of early and continuous clinical treatment</t>
-  </si>
-  <si>
-    <t>Bipolar disorder is a severe psychiatric syndrome defined by periodic mood shifts Patients with bipolar disorder show cognitive impairments relative to healthy controls The risk of developing schizophrenia and partially also bipolar disorder has previously been shown to increase with lower premorbid intelligence It is not known if premorbid intelligence is associated with level of functioning and illness severity of people having developed bipolar disorder We used multiple linear and ordinal regression to analyze how premorbid intelligence as measured at conscription associate with functional outcome and illness severity in Swedish male bipolar disorder patients n 788 We found that lower premorbid intelligence is associated with lower percentage of time in work after adjusting for age and bipolar subtype and correcting for multiple comparisons We also found a strong negative association with the total number of inpatient episodes and psychiatric comorbidity but not with interepisodic remission treatment with psychotherapy or lithium or the presence of any complicating socioeconomical factors Adjusting for confounding genetic factors using polygenic risk scores for bipolar disorder and schizophrenia had no effect on the associations This study lacks females and controls and may thus have lower generalizability In conclusion premorbid intelligence is associated with both level of functioning and illness severity as well as comorbidity in bipolar disorder patients Further research is needed to develop targeted interventions for this subgroup of bipolar disorder patients</t>
-  </si>
-  <si>
     <t>The aim of this study was to assess if premorbid IQ moderates the association between measures of clinical severity and neurocognitive or psychosocial functioning in euthymic patients with bipolar disorder One hundred and nineteen outpatients and forty healthy controls were included The length of illness number of previous hypomanic and depressive episodes episode density and history of psychosis assessed clinical severity Performances in verbal memory attention and executive functions as well as level of psychosocial functioning were used as outcomes The negative relationship between number of hypomanic episodes and performance in executive functions decreased as a function of higher values of premorbid IQ No other influences of premorbid IQ were found in the association between clinical severity measures and neurocognitive and psychosocial functioning Premorbid IQ might moderate the relationship between the number of hypomanic episodes and executive functioning in bipolar disorder Possible interpretations of this finding are discussed</t>
   </si>
   <si>
-    <t>To evaluate the association between hearing loss and nonverbal intelligence in US children The Third National Health and Nutrition Examination Survey NHANES III is a crosssectional survey 19881994 that used complex multistage sampling design to produce nationally representative demographic and examination data A total of 4823 children ages 6 to 16 years completed audiometric evaluation and cognitive testing during NHANES III Hearing loss was defined as lowfrequency puretone average PTA 25 dB 05 1 2 kHz or highfrequency PTA 25 dB 3 4 6 8 kHz and was designated as unilateral or bilateral Nonverbal intelligence was measured using the Wechsler Intelligence Scale for ChildrenRevised block design subtest Low nonverbal intelligence was defined as a standardized score 4 two standard deviations below the standardized mean of 10 Mean nonverbal intelligence scores differed between children with normal hearing 959 and children with bilateral 687 P 02 but not unilateral 912 P 42 hearing loss NonHispanic black raceethnicity and family income 20000 were associated with 392 and 167 times higher odds of low nonverbal intelligence respectively odds ratio OR 392 P 001 OR 167 P 02 Bilateral hearing loss was independently associated with 577 times increased odds of low nonverbal intelligence compared to normal hearing children OR 577 P 02 Unilateral hearing loss was not associated with higher odds of low nonverbal intelligence OR 073 P 40 Bilateral but not unilateral hearing loss is associated with decreased nonverbal intelligence in US children Longitudinal studies are urgently needed to better understand these associations and their potential impact on future opportunities</t>
-  </si>
-  <si>
-    <t>To evaluate the association between adolescent and youngadult hearing loss and nonverbal intelligence in rural Nepal Crosssectional assessment of hearing loss among a population cohort of adolescents and young adults Sarlahi District southern Nepal Seven hundred sixtyfour individuals aged 14 to 23 years Evaluation of hearing loss defined by World Health Organization criteria of puretone average greater than 25 decibels 05 1 2 4 kHz unilaterally and bilaterally Nonverbal intelligence as measured by the Test of Nonverbal Intelligence 3rd Edition standardized score mean 100 standard deviation 15 Nonverbal intelligence scores differed between participants with normal hearing and those with bilateral p 004 but not unilateral p 074 hearing loss Demographic and socioeconomic factors including male sex higher caste literacy education level occupation reported as student and ownership of a bicycle watch and latrine were strongly associated with higher nonverbal intelligence scores all p 0001 Subjects with bilateral hearing loss scored an average of 316 points lower 95 confidence interval 556 to 075 p 001 than subjects with normal hearing after controlling for socioeconomic factors There was no difference in nonverbal intelligence score based on unilateral hearing loss 097 95 confidence interval 167 to 361 p 047 Nonverbal intelligence is adversely affected by bilateral hearing loss even at mild hearing loss levels Socio economic wellbeing appears compromised in individuals with lower nonverbal intelligence test scores</t>
-  </si>
-  <si>
-    <t>Impaired auditory speech perception abilities in deaf children with hearing aids compromised their verbal intelligence enormously The availability of unilateral cochlear implantation CI auditory speech perception and spoken vocabulary enabled them to reach near ageappropriate levels This holds especially for children in spoken language environments However speech perception in complex listening situations and the acquisition of complex verbal skills remains difficult Bilateral CI was expected to enhance the acquisition of verbal intelligence by improved understanding of speech in noise This study examined the effect of bilateral CI on verbal intelligence of 49 deaf children 3580 years Relations between speech perception in noise auditory shortterm memory and verbal intelligence were analysed with multiple linear regressions In addition the interaction of educational setting mainstream or special on these relations was analysed Children with bilateral CI obtained higher scores on verbal intelligence Significant associations were present between speech perception in noise auditory shortterm memory and verbal intelligence Children with simultaneous bilateral CIs showed better speech perception in noise than children with unilateral CIs which mediated by the auditory shortterm memory capacity enhanced the ability to acquire more complex verbal skills for BICI children in mainstream education</t>
-  </si>
-  <si>
     <t>Longitudinal studies show that lower cognitive performance in adolescence and early adulthood is associated with higher risk of suicide death throughout adulthood However it is unclear whether this cognitive vulnerability originates earlier in childhood since studies conducted in children are scarce and have inconsistent results Vital status of 49853 individuals born between 1959 and 1966 to participants in the Collaborative Perinatal Project cohort was determined by a probabilistic linkage to the National Death Index covering all US deaths occurring from 1979 through 2016 Cox proportional hazard models were used to examine associations of general verbal and nonverbal intelligence at ages 4 and 7 and academic skills at age 7 with suicide death coded according to ICD910 criteria while accounting for sociodemographic and pregnancy factors previously associated with suicide in this sample By the end of 2016 288 cohort members had died by suicide Cognitive performance at 7 years on tests with verbal components was associated with suicide risk average vs high verbal intelligence HR 197 95 CI 105371 low vs high spelling skills HR 202 95 CI 116351 low vs high reading skills HR 201 95 CI 127317 Associations were still evident especially for verbal intelligence and reading skills but hazard ratios were attenuated after adjusting for prenatal and sociodemographic factors at birth verbal intelligence HR 197 95 CI 103378 spelling HR 161 95 CI 090288 reading HR 167 95 CI 102272 Childhood neurocognitive performance is associated with vulnerability to suicide mortality through middleadulthood suggesting that there might be a cognitive diathesis for suicide originating in early childhood Future studies should examine how multiple domains of childhood cognitive performance contribute to vulnerability to suicide risk including by increasing risk for social and environmental factors that are associated not only with suicide but also with many types of psychiatric disorders</t>
   </si>
   <si>
@@ -230,36 +215,15 @@
     <t>The chromosome bands 15q24115q243 contain a complex region with numerous segmental duplications that predispose to regional microduplications and microdeletions both of which have been linked to intellectual disability speech delay and autistic features The region may also harbour common inversion polymorphisms whose functional and phenotypic manifestations are unknown Using single nucleotide polymorphism SNP data we detected four large contiguous haplotypegenotypes at 15q24 with Mendelian inheritance in 2562 trios African origin high population stratification and reduced recombination rates Although the haplotypegenotypes have been most likely generated by decreased or absent recombination among them we could not confirm that they were the product of inversion polymorphisms in the region One of the blocks was composed of three haplotypegenotypes N1a N1b and N2 which significantly correlated with intelligence quotient IQ in 2735 children of European ancestry from three independent population cohorts Homozygosity for N2 was associated with lower verbal IQ 24point loss pvalue 001 while homozygosity for N1b was associated with 32point loss in nonverbal IQ pvalue 00006 The three alleles strongly correlated with expression levels of MAN2C1 and SNUPN in blood and brain Homozygosity for N2 correlated with overexpression of MAN2C1 over many brain areas but the occipital cortex where N1b homozygous highly underexpressed Our populationbased analyses suggest that MAN2C1 may contribute to the verbal difficulties observed in microduplications and to the intellectual disability of microdeletion syndromes whose characteristic dosage increment and removal may affect different brain areas</t>
   </si>
   <si>
-    <t>We evaluated the neurodevelopment and growth of five to sevenyearold children who had participated in a randomised trial of early lowdose hydrocortisone treatment to prevent bronchopulmonary dysplasia The 51 infants in the original study had birthweights of 5011250 g and gestational ages of 2330 weeks required mechanical ventilation during the first 24 hours and received hydrocortisone or a placebo for 10 days The majority 80 of the 90 who survived to five to seven years of age participated in this followup study and their growth neuromotor cognitive and speech development were evaluated Some neurodevelopment impairment was observed in 61 of the hydrocortisone group and 39 of the placebo group ranging from minor neurological dysfunction to severe neurological conditions p 0182 The mean fullscale intelligence quotient IQ was 878 153 in the hydrocortisone group and 957 150 in the placebo group p 0135 and the mean performance IQ was 883 145 and 991 140 p 0034 respectively A fifth 22 of the hydrocortisone group required physiotherapy but none of the placebo group did p 0034 The agestandardised growth was comparable between both groups Early hydrocortisone treatment may have undesired effects on neurodevelopment at preschool age and further safety studies are required</t>
-  </si>
-  <si>
-    <t>To assess the 5year neurocognitive outcomes of children born extremely preterm exposed to prophylactic hydrocortisone to improve survival without bronchopulmonary dysplasia This was a prespecified secondary analysis of the PREMILOC clinical trial trial registration EudraCT no 200700204120 NCT00623740 The primary outcome was fullscale IQ based on the Wechsler Preschool and Primary Scale of Intelligence Among 109 surviving children recruited at the Robert Debre Childrens Hospital Paris outcome data were available for 42 out of 56 infants 75 in the group treated with hydrocortisone and 41 out of 53 77 in the placebo group Mean scores were not significantly different between the two groups on fullscale IQ hydrocortisone 919 SD 139 placebo 863 SD 154 mean difference 57 95 confidence interval CI 10 to 123 p 010 however working memory and retention ability were significantly better in the group treated with hydrocortisone In a multivariate logistic regression including potential confounding variables hydrocortisone treatment was significantly associated with a greater chance to survive at 5 years of age with a fullscale IQ equal to or greater than 90 compared to placebo adjusted odds ratio 426 95 CI 1471236 p 0008 This exploratory analysis provides reassuring data regarding the longterm neurodevelopmental safety of prophylactic hydrocortisone in infants born extremely preterm</t>
-  </si>
-  <si>
     <t>Perinatal exposure to glucocorticoids has been associated with adverse cerebral effects but little is known about their effect on cognitive development and exposure later in childhood This study examined intellectual abilities memory and behavioural problems in children previously treated with glucocorticoids We evaluated 38 children aged from seven to 16 years who had been treated with glucocorticoids for rheumatic disease or nephrotic syndrome together with 42 healthy controls matched for age gender and parental education The median cumulative dose of prednisolone equivalents was 158 mgkg range 21723 and the mean time that had elapsed since treatment was threeandahalf standard deviation 22 years Intellectual abilities were assessed with the Wechsler Intelligence Scale for Children and memory performance and behavioural problems with a pattern recognition memory task and the Child Behaviour Check List There were no significant differences between the groups in pattern recognition memory perceptual organisation index or behavioural problems but patients had a significantly lower verbal comprehension index and this difference was present in both disease groups There were no significant doseresponse relationships regarding verbal intellectual abilities Children and adolescents previously treated with glucocorticoids seemed to have lower intellectual verbal abilities than healthy controls</t>
   </si>
   <si>
-    <t>Micronutrient supplementation is often prescribed during pregnancy The effects of prenatal iron and multimicronutrient supplementation on intellectual development in young schoolaged children are less than clear The aim of this study was to examine the longterm effects of prenatal iron plus folic acid or multiple micronutrient including iron and folic acid supplementation vs folic acid supplementation on the intellectual development of young schoolaged children in rural China Young schoolaged children aged 710 y n 1744 of women who had participated in a trial of prenatal supplementation with various combinations of micronutrients and remained residents in 2 rural counties in China were followed We measured their intellectual development by Wechsler Intelligence Scale for Children Fourth Edition WISCIV The WISCIV generated the FullScale Intelligence Quotient FSIQ Verbal Comprehension Index VCI Working Memory Index WMI Perceptual Reasoning Index PRI and Processing Speed Index PSI Multilevel analyses were used to assess the effect of prenatal micronutrient supplementation on the intellectual development of children The mean differences in FSIQ VCI WMI PRI and PSI respectively were not significant between prenatal folic acid supplementation and either iron plus folic acid 034 P 065 006 P 095 022 P 076 001 P 099 and 126 P 011 or multimicronutrient 039 P 060 064 P 048 011 P 087 043 P 059 and 034 P 065 supplementation after adjusting for confounders There is no evidence to suggest a different effect on intellectual development between prenatal iron plus folic acid multimicronutrient supplementation and prenatal folic acid supplementation in children aged 710 y This trial was registered at wwwisrctncom as ISRCTN08850194</t>
-  </si>
-  <si>
-    <t>The association of micronutrient supplementation during pregnancy with the intellectual development of adolescent offspring is unknown To assess the longterm association of antenatal micronutrient supplementation with adolescent intellectual development This 14year followup study of a randomized clinical trial of micronutrient supplementation in pregnancy was conducted in 2 counties in rural western China in 2118 adolescent offspring aged 10 to 14 years of mothers who were randomized to take a daily capsule of either folic acid folic acid plus iron or multiple micronutrients from August 1 2002 through February 28 2006 Followup was conducted from June 1 2016 through December 31 2016 Data analyses took place from April 1 2017 to June 20 2017 Adolescent fullscale intelligence quotient and aspects of verbal comprehension working memory perceptual reasoning and processing speed indexes were assessed by the Wechsler Intelligence Scale for Children Of 2118 adolescent offspring 1252 591 were boys and 866 409 were girls with a mean SD age of 117 087 years representing 472 of the 4488 single live births that were eligible to participate Compared with folic acid supplementation multiple micronutrient supplementation was associated with a 113point higher fullscale intelligence quotient 95 CI 015210 and a 203point higher verbal comprehension index 95 CI 061345 similar results were found in comparison with folic acid plus iron When mothers initiated supplementation early 12 weeks of gestation and had an adequate dose 180 capsules multiple micronutrient capsules were associated with a 216point higher fullscale intelligence quotient 95 CI 041390 and 429point higher verbal comprehension index 95 CI 133724 compared with folic acid capsules The mean test scores were lower in the substratum of supplementation initiated late 12 weeks of gestation and with an inadequate dose 180 capsules The multiple micronutrient group had higher scores than the other 2 treatment groups and significant differences were observed for fullscale intelligence quotient adjusted mean difference 246 95 CI 098394 when compared with the folic acid plus iron group Compared with folic acid plus iron or...</t>
-  </si>
-  <si>
     <t>Micronutrients are essential for brain development with deficiencies in specific nutrients linked to impaired cognitive function Interventions are shown to be beneficial to childrens mental development particularly in subjects who were micronutrientdeficient at baseline but results on healthy subjects remain inconsistent This systematic review evaluated the effect of micronutrient inventions on different cognitive domains Studies conducted in both developing and developed countries and trials that investigate the effect of both single and multiple micronutrient intervention were reviewed Systematic searches of Medline CINAHL Plus and Academic Search database were undertaken to identify trials published after year 2000 Randomized controlled trials RCTs that evaluate the effect of micronutrients on cognitive performance or academic performance among children aged 418 years were included 19 trials were identified from 18 articles The major cognitive outcomes assessed included fluid intelligence crystallized intelligence shortterm memory longterm memory cognitive processing speed attention and concentration and school performance Eight of ten trials assessing fluid intelligence reported significant positive effects of micronutrient supplementation among micronutrientdeficient children especially those who were irondeficient or iodinedeficient at baseline The effects of micronutrient interventions on other domains were inconsistent Improvement in fluid intelligence among micronutrientdeficient children was consistently reported Further research is needed to provide more definite evidence on the beneficial effects of micronutrient inventions on other cognitive domains and the effects in healthy subjects</t>
   </si>
   <si>
-    <t>Maternal stress during pregnancy has been associated with negative outcomes in children We examined the risk factors for symptoms of depression in 11yearold children including the interaction between birthweight and other variables We collected maternal obstetric and demographic information from birth through to the age of 11 Approximately half of the 609 children were born smallforgestationalage SGA Information collected at 35 and 7 years of age included intelligence testing and parentreported behavioural and emotional development At 11 years of age the children completed the Center for Epidemiological Studies Depression Scale for Children Multivariable logistic regression analysis examined the relationship between selfreported symptoms of moderate to severe depression at the age of 11 and explanatory variables Symptoms of moderate to severe depression were related to increasing maternal stress during pregnancy young maternal age lower intelligence test scores at 7yearsold and being bullied at school in the previous 6 months There was also a significant interaction between maternal stress in pregnancy and symptoms of depression in 11yearold children born SGA Increasing maternal stress during pregnancy was associated with increased risk of symptoms of moderate to severe depression in 11yearold children especially those who were born SGA</t>
-  </si>
-  <si>
-    <t>bMaternal depression and child development A prospective analysis of consequences risk and protective factorsb bAbstractb iObjectivei Maternal stress specifically maternal mental health problems are considered risk factors for child development The literature suggests that prenatal depressive symptoms as well as depressive symptoms are a widespread phenomenon during the further development of the child and have repeatedly been shown to have adverse effects on child mental health outcomes The present study examined the longitudinal relationships between maternal depression prenatal postnatal during childhood and adolescence and child mental health from childhood to adolescence Possible risk and protective factors were also considered iMethodi iNi 112 mothers were assessed for depressive symptoms via a questionnaire at four different timepoints prenatal T1 postnatal T2 during childhood T3 during adolescence T4 Childrens externalizing and internalizing symptoms 509 girls were assessed by their mothers both during childhood iMi 768 iSDi 076 years and during adolescence iMi 1323 iSDi 027 years We evaluated the relationships between maternal depressive symptoms and childrens externalizinginternalizing symptoms using multiple regression models and analyzed possible risk and protective factors using moderation analysis iResultsi ExternalizingInternalizing symptoms were not directly associated with maternal depressive symptoms while associations between such symptoms and maladaptive behavior were found in adolescents The socioeconomic status of families showed a different risk profile for prenatal and postnatal depressive symptoms The IQ of the children proved to be a risk factor for internalizing symptoms iConclusionsi Maternal depressive symptoms at any time during child development in combination with further risk factors have an impact on child mental health The early identification of maternal symptoms followed by interventions to differentiate between prenatal and postnatal depression especially in the context of socioeconomic status are highly relevant for child development</t>
-  </si>
-  <si>
     <t>This study assessed the association between timing and course of maternal depression from pregnancy onwards and childrens cognitive development at ages 5 to 6 Potential interaction effects with child sex and family socioeconomic status were explored One thousand thirtynine motherchild pairs from the French EDEN motherchild birth cohort were followed from 24 to 28 weeks of pregnancy onwards Based on Center for Epidemiological Studies Depression CESD and Edinburgh Postnatal Depression Scale EPDS scores assessed at six timepoints longitudinal maternal depressive symptom trajectories were calculated with a groupbased semiparametric method Childrens cognitive function was assessed at ages 5 to 6 by trained interviewers with the Wechsler Preschool and Primary Scale of Intelligence Third Edition WPPSIIII resulting in three composite scores Verbal IQ VIQ Performance IQ PIQ and FullScale IQ FSIQ Five trajectories of maternal symptoms of depression could be distinguished no symptoms persistent intermediatelevel depressive symptoms persistent high depressive symptoms high symptoms in pregnancy only and high symptoms in the childs preschool period only Multiple linear regression analyses showed that compared to children of mothers who were never depressed children of mothers with persistent high levels of depressive symptoms had reduced VIQ PIQ and FSIQ scores This association was moderated by the childs sex boys appearing especially vulnerable in case of persistent maternal depression Chronicity of maternal depression predicts childrens cognitive development at school entry age particularly in boys As maternal mental health is an early modifiable influence on child development addressing the treatment needs of depressed mothers may help reduce the associated burden on the next generation</t>
   </si>
   <si>
-    <t>Studies from the UK have shown that children with Down syndrome acquire more academic skills in regular education Does this likewise hold true for the Dutch situation even after the effect of selective placement has been taken into account In 2006 an extensive questionnaire was sent to 160 parents of specially and regularly placed children with Down syndrome born 19932000 in primary education in the Netherlands with a response rate of 76 Questions were related to the childs school history academic and nonacademic skills intelligence quotient parental educational level the extent to which parents worked on academics with their child at home and the amount of academic instructional time at school Academic skills were predicted with the other variables as independents For the children in regular schools much more time proved to be spent on academics Academic performance appeared to be predicted reasonably well on the basis of age nonacademic skills parental educational level and the extent to which parents worked at home on academics However more variance could be predicted when the total amount of years that the child spent in regular education was added especially regarding reading and to a lesser extent regarding writing and math In addition we could prove that this finding could not be accounted for by endogenity Regularly placed children with Down syndrome learn more academics However this is not a straight consequence of inclusive placement and age alone but is also determined by factors such as cognitive functioning nonacademic skills parental educational level and the extent to which parents worked at home on academics Nevertheless it could be proven that the more advanced academic skills of the regularly placed children are not only due to selective placement The positive effect of regular school on academics appeared to be most pronounced for reading skills</t>
-  </si>
-  <si>
     <t>In education research and education policy much attention is paid to schools curricula and teachers but little attention is paid to the characteristics of students Differences in general cognitive ability igi are often overlooked as a source of important variance among schools and in outcomes among students within schools Standardized test scores such as the SAT and ACT are reasonably good proxies for igi and are available for most incoming college students Though the idea of igi being important in education is quite old we present contemporary evidence that colleges and universities in the United States vary considerably in the average cognitive ability of their students which correlates strongly with other methods including international methods of ranking colleges We also show that these igi differences are reflected in the extent to which graduates of colleges are represented in various highstatus and highincome occupations Finally we show how including individuallevel measures of cognitive ability can substantially increase the statistical power of experiments designed to measure educational treatment effects We conclude that education policy researchers should give more consideration to the concept of individual differences in cognitive ability as well as other factors</t>
   </si>
   <si>
@@ -332,9 +296,6 @@
     <t>ndcg</t>
   </si>
   <si>
-    <t>BAAI, Jamesgpt:  impact of maternal depression from pregnancy onwards, explores its association with children's cognitive development     Thenlper: systematic review of effects of perinatal depression on IQ of children</t>
-  </si>
-  <si>
     <t>BAAAI: reviews effect of micronutrient interventions on cognitive performance in children, but not directly tied to prenatal micronutrient supplementation      Jamesgpt: evaluates impact of prenatal micronutrient supplementation on children        Thenlper:  evaluates impact of prenatal micronutrient supplementation versus iron/folic acid on children's intelligence</t>
   </si>
   <si>
@@ -345,6 +306,15 @@
   </si>
   <si>
     <t>BAAI, Jamesgpt: focus is on how premorbid IQ moderates the relationship between clinical severity and executive functioning.          Thenlper:  focuses on the relationship between intelligence and risk of developing bipolar disorder, which diverges from query's interest in occupational outcomes</t>
+  </si>
+  <si>
+    <t>Note: Glucocordicoidis are a class of hormons, to which hydricortisone belongs and even is the most important. Dexamethasone is also a glucocoicoidis.        BAAI: patients from 7 to 16 yo, not preschool.       Jamesgpt: Got both infants and hydrocortisone</t>
+  </si>
+  <si>
+    <t>BAAI, Jamesgpt:  impact of maternal depression from pregnancy onwards, explores its association with children's cognitive development. [Matteo] Maternal depression not children's depression.     Thenlper: systematic review of effects of perinatal depression on IQ of children</t>
+  </si>
+  <si>
+    <t>Jamesgpt: Special regard to 10 years old</t>
   </si>
 </sst>
 </file>
@@ -718,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -890,15 +860,72 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -911,64 +938,34 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1025,68 +1022,35 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1801,9 +1765,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5956BC-300C-CB42-87CA-185E2E097C22}">
   <dimension ref="A1:O205"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1825,35 +1789,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="F1" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="73" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="79" t="s">
-        <v>78</v>
-      </c>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="94" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="98" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C2" s="76"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="78"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="97"/>
       <c r="F2" s="25" t="s">
         <v>44</v>
       </c>
@@ -1886,21 +1850,21 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="75"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
+      <c r="N3" s="87"/>
     </row>
     <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
@@ -1909,17 +1873,23 @@
       <c r="C4" s="28"/>
       <c r="D4" s="29"/>
       <c r="E4" s="30"/>
-      <c r="F4" s="25"/>
+      <c r="F4" s="25">
+        <v>2</v>
+      </c>
       <c r="G4" s="25">
         <v>2</v>
       </c>
       <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
+      <c r="I4" s="26">
+        <v>2</v>
+      </c>
       <c r="J4" s="26">
         <v>2</v>
       </c>
       <c r="K4" s="26"/>
-      <c r="L4" s="27"/>
+      <c r="L4" s="27">
+        <v>1</v>
+      </c>
       <c r="M4" s="27">
         <v>1</v>
       </c>
@@ -1928,86 +1898,86 @@
     <row r="5" spans="1:15" ht="255" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="32"/>
       <c r="C5" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="F5" s="86"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="80"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="82"/>
+        <v>73</v>
+      </c>
+      <c r="F5" s="79"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="77"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="75"/>
       <c r="O5" s="45" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="75"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="87"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="75"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="86"/>
+      <c r="N7" s="87"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="74" t="s">
+      <c r="B8" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="75"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="86"/>
+      <c r="N8" s="87"/>
     </row>
     <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" s="32" t="s">
@@ -2015,17 +1985,23 @@
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="30"/>
-      <c r="F9" s="25"/>
+      <c r="F9" s="25">
+        <v>1</v>
+      </c>
       <c r="G9" s="25">
         <v>1</v>
       </c>
       <c r="H9" s="25"/>
-      <c r="I9" s="26"/>
+      <c r="I9" s="26">
+        <v>1</v>
+      </c>
       <c r="J9" s="26">
         <v>1</v>
       </c>
       <c r="K9" s="26"/>
-      <c r="L9" s="27"/>
+      <c r="L9" s="27">
+        <v>3</v>
+      </c>
       <c r="M9" s="27">
         <v>2</v>
       </c>
@@ -2034,46 +2010,46 @@
     <row r="10" spans="1:15" ht="404" x14ac:dyDescent="0.2">
       <c r="B10" s="32"/>
       <c r="C10" s="28" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="F10" s="86"/>
-      <c r="G10" s="87"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="84"/>
-      <c r="K10" s="85"/>
-      <c r="L10" s="80"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="82"/>
+        <v>74</v>
+      </c>
+      <c r="F10" s="79"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="75"/>
       <c r="O10" s="44" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>5</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
-      <c r="M11" s="74"/>
-      <c r="N11" s="75"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="87"/>
     </row>
     <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="s">
@@ -2081,17 +2057,23 @@
       </c>
       <c r="D12" s="29"/>
       <c r="E12" s="30"/>
-      <c r="F12" s="25"/>
+      <c r="F12" s="25">
+        <v>3</v>
+      </c>
       <c r="G12" s="25">
         <v>2</v>
       </c>
       <c r="H12" s="25"/>
-      <c r="I12" s="26"/>
+      <c r="I12" s="26">
+        <v>1</v>
+      </c>
       <c r="J12" s="26">
         <v>1</v>
       </c>
       <c r="K12" s="26"/>
-      <c r="L12" s="27"/>
+      <c r="L12" s="27">
+        <v>1</v>
+      </c>
       <c r="M12" s="27">
         <v>1</v>
       </c>
@@ -2100,46 +2082,46 @@
     <row r="13" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="32"/>
       <c r="C13" s="28" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="86"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="84"/>
-      <c r="K13" s="85"/>
-      <c r="L13" s="80"/>
-      <c r="M13" s="81"/>
-      <c r="N13" s="82"/>
+        <v>75</v>
+      </c>
+      <c r="F13" s="79"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="77"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="74"/>
+      <c r="N13" s="75"/>
       <c r="O13" s="44" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>6</v>
       </c>
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="74"/>
-      <c r="M14" s="74"/>
-      <c r="N14" s="75"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="87"/>
     </row>
     <row r="15" spans="1:15" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="52" t="s">
@@ -2148,60 +2130,69 @@
       <c r="C15" s="64"/>
       <c r="D15" s="54"/>
       <c r="E15" s="55"/>
-      <c r="F15" s="48"/>
+      <c r="F15" s="48">
+        <v>2</v>
+      </c>
       <c r="G15" s="48"/>
       <c r="H15" s="48"/>
-      <c r="I15" s="49"/>
+      <c r="I15" s="49">
+        <v>3</v>
+      </c>
       <c r="J15" s="49"/>
       <c r="K15" s="49"/>
-      <c r="L15" s="50"/>
+      <c r="L15" s="50">
+        <v>2</v>
+      </c>
       <c r="M15" s="50"/>
       <c r="N15" s="50"/>
       <c r="O15" s="46" t="str">
         <f>IF(OR( AND(C16=D16,OR(F15&lt;&gt;G15, I15&lt;&gt;J15,L15&lt;&gt;M15)),  AND(D16=E16,OR(G15&lt;&gt;H15,J15&lt;&gt;K15,M15&lt;&gt;N15)), AND(C16=E16, OR(F15&lt;&gt;H15,I15&lt;&gt;K15,L15&lt;&gt;N15) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="46" customFormat="1" ht="409.5" x14ac:dyDescent="0.2">
+        <v>error: different mark to same abstract</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="46" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B16" s="52"/>
       <c r="C16" s="53" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D16" s="54" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="98"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="94"/>
-      <c r="K16" s="95"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="91"/>
-      <c r="N16" s="92"/>
+        <v>58</v>
+      </c>
+      <c r="F16" s="82"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="91"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="88"/>
+      <c r="M16" s="89"/>
+      <c r="N16" s="90"/>
+      <c r="O16" s="52" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>7</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="74"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="75"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
+      <c r="N17" s="87"/>
     </row>
     <row r="18" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="32" t="s">
@@ -2209,17 +2200,23 @@
       </c>
       <c r="D18" s="29"/>
       <c r="E18" s="30"/>
-      <c r="F18" s="25"/>
+      <c r="F18" s="25">
+        <v>3</v>
+      </c>
       <c r="G18" s="37">
         <v>2</v>
       </c>
       <c r="H18" s="25"/>
-      <c r="I18" s="26"/>
+      <c r="I18" s="26">
+        <v>3</v>
+      </c>
       <c r="J18" s="26">
         <v>3</v>
       </c>
       <c r="K18" s="26"/>
-      <c r="L18" s="27"/>
+      <c r="L18" s="27">
+        <v>3</v>
+      </c>
       <c r="M18" s="27">
         <v>3</v>
       </c>
@@ -2228,46 +2225,46 @@
     <row r="19" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B19" s="32"/>
       <c r="C19" s="28" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="86"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="85"/>
-      <c r="L19" s="80"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="82"/>
+        <v>76</v>
+      </c>
+      <c r="F19" s="79"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="78"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="74"/>
+      <c r="N19" s="75"/>
       <c r="O19" s="44" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>8</v>
       </c>
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="74"/>
-      <c r="N20" s="75"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="86"/>
+      <c r="K20" s="86"/>
+      <c r="L20" s="86"/>
+      <c r="M20" s="86"/>
+      <c r="N20" s="87"/>
     </row>
     <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="32" t="s">
@@ -2275,17 +2272,23 @@
       </c>
       <c r="D21" s="29"/>
       <c r="E21" s="30"/>
-      <c r="F21" s="25"/>
+      <c r="F21" s="25">
+        <v>1</v>
+      </c>
       <c r="G21" s="37">
         <v>3</v>
       </c>
       <c r="H21" s="25"/>
-      <c r="I21" s="26"/>
+      <c r="I21" s="26">
+        <v>1</v>
+      </c>
       <c r="J21" s="38">
         <v>3</v>
       </c>
       <c r="K21" s="26"/>
-      <c r="L21" s="27"/>
+      <c r="L21" s="27">
+        <v>3</v>
+      </c>
       <c r="M21" s="27">
         <v>3</v>
       </c>
@@ -2294,46 +2297,46 @@
     <row r="22" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B22" s="32"/>
       <c r="C22" s="28" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22" s="86"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="88"/>
-      <c r="I22" s="83"/>
-      <c r="J22" s="84"/>
-      <c r="K22" s="85"/>
-      <c r="L22" s="80"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="82"/>
+        <v>77</v>
+      </c>
+      <c r="F22" s="79"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="77"/>
+      <c r="K22" s="78"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="75"/>
       <c r="O22" s="44" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>9</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="74"/>
-      <c r="L23" s="74"/>
-      <c r="M23" s="74"/>
-      <c r="N23" s="75"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="86"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="86"/>
+      <c r="M23" s="86"/>
+      <c r="N23" s="87"/>
     </row>
     <row r="24" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="32" t="s">
@@ -2341,36 +2344,42 @@
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="25"/>
+      <c r="F24" s="25">
+        <v>1</v>
+      </c>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
-      <c r="I24" s="26"/>
+      <c r="I24" s="26">
+        <v>1</v>
+      </c>
       <c r="J24" s="26"/>
       <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
+      <c r="L24" s="27">
+        <v>1</v>
+      </c>
       <c r="M24" s="27"/>
       <c r="N24" s="27"/>
     </row>
     <row r="25" spans="1:15" ht="306" x14ac:dyDescent="0.2">
       <c r="B25" s="32"/>
       <c r="C25" s="28" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="F25" s="86"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="88"/>
-      <c r="I25" s="83"/>
-      <c r="J25" s="84"/>
-      <c r="K25" s="85"/>
-      <c r="L25" s="80"/>
-      <c r="M25" s="81"/>
-      <c r="N25" s="82"/>
+        <v>78</v>
+      </c>
+      <c r="F25" s="79"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="81"/>
+      <c r="I25" s="76"/>
+      <c r="J25" s="77"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="75"/>
     </row>
     <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="32" t="s">
@@ -2378,56 +2387,62 @@
       </c>
       <c r="D26" s="29"/>
       <c r="E26" s="30"/>
-      <c r="F26" s="25"/>
+      <c r="F26" s="25">
+        <v>1</v>
+      </c>
       <c r="G26" s="25"/>
       <c r="H26" s="25"/>
-      <c r="I26" s="26"/>
+      <c r="I26" s="26">
+        <v>1</v>
+      </c>
       <c r="J26" s="26"/>
       <c r="K26" s="26"/>
-      <c r="L26" s="27"/>
+      <c r="L26" s="27">
+        <v>1</v>
+      </c>
       <c r="M26" s="27"/>
       <c r="N26" s="27"/>
     </row>
     <row r="27" spans="1:15" ht="388" x14ac:dyDescent="0.2">
       <c r="B27" s="32"/>
       <c r="C27" s="28" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="E27" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="F27" s="86"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="83"/>
-      <c r="J27" s="84"/>
-      <c r="K27" s="85"/>
-      <c r="L27" s="80"/>
-      <c r="M27" s="81"/>
-      <c r="N27" s="82"/>
+        <v>79</v>
+      </c>
+      <c r="F27" s="79"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="76"/>
+      <c r="J27" s="77"/>
+      <c r="K27" s="78"/>
+      <c r="L27" s="73"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="75"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>10</v>
       </c>
-      <c r="B28" s="74" t="s">
+      <c r="B28" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="74"/>
-      <c r="J28" s="74"/>
-      <c r="K28" s="74"/>
-      <c r="L28" s="74"/>
-      <c r="M28" s="74"/>
-      <c r="N28" s="75"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="86"/>
+      <c r="N28" s="87"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C29"/>
@@ -2444,11 +2459,11 @@
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C30" s="99" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="99"/>
-      <c r="E30" s="99"/>
+      <c r="C30" s="85" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="85"/>
+      <c r="E30" s="85"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -4766,20 +4781,17 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B6:N6"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="B7:N7"/>
     <mergeCell ref="B28:N28"/>
     <mergeCell ref="B23:N23"/>
@@ -4796,17 +4808,20 @@
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="L16:N16"/>
     <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B6:N6"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4814,11 +4829,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03816060-24A7-D946-9AB1-F7E07293AE02}">
-  <dimension ref="A1:O249"/>
+  <dimension ref="A1:O213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F68" sqref="F68:H72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4841,35 +4856,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="131" t="s">
+      <c r="D1" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="132" t="s">
+      <c r="E1" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="134" t="s">
+      <c r="F1" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="135" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="135"/>
-      <c r="K1" s="135"/>
-      <c r="L1" s="133" t="s">
-        <v>78</v>
-      </c>
-      <c r="M1" s="133"/>
-      <c r="N1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="134" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="134"/>
+      <c r="K1" s="134"/>
+      <c r="L1" s="130" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C2" s="130"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="132"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="129"/>
       <c r="F2" s="48" t="s">
         <v>44</v>
       </c>
@@ -4902,1445 +4917,1211 @@
       <c r="A3" s="51">
         <v>1</v>
       </c>
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
-      <c r="N3" s="129"/>
-    </row>
-    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B4" s="52" t="s">
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="131"/>
+      <c r="L3" s="131"/>
+      <c r="M3" s="131"/>
+      <c r="N3" s="132"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="51">
+        <v>2</v>
+      </c>
+      <c r="B4" s="131" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="131"/>
+      <c r="L4" s="131"/>
+      <c r="M4" s="131"/>
+      <c r="N4" s="132"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="51">
+        <v>3</v>
+      </c>
+      <c r="B5" s="131" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="131"/>
+      <c r="K5" s="131"/>
+      <c r="L5" s="131"/>
+      <c r="M5" s="131"/>
+      <c r="N5" s="132"/>
+    </row>
+    <row r="6" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="52" t="s">
         <v>41</v>
-      </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="46" t="str">
-        <f>IF(OR( AND(C5=D5,OR(F4&lt;&gt;G4, I4&lt;&gt;J4,L4&lt;&gt;M4)),  AND(D5=E5,OR(G4&lt;&gt;H4,J4&lt;&gt;K4,M4&lt;&gt;N4)), AND(C5=E5, OR(F4&lt;&gt;H4,I4&lt;&gt;K4,L4&lt;&gt;N4) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="52"/>
-      <c r="C5" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="118"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="110"/>
-      <c r="K5" s="111"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="101"/>
-      <c r="N5" s="102"/>
-    </row>
-    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" s="52" t="s">
-        <v>42</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="54"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="122"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="114"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="104"/>
-      <c r="N6" s="105"/>
-      <c r="O6" s="46" t="str">
-        <f>IF(OR( AND(C7=D7,OR(F6&lt;&gt;G6, I6&lt;&gt;J6,L6&lt;&gt;M6)),  AND(D7=E7,OR(G6&lt;&gt;H6,J6&lt;&gt;K6,M6&lt;&gt;N6)), AND(C7=E7, OR(F6&lt;&gt;H6,I6&lt;&gt;K6,L6&lt;&gt;N6) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="372" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E6" s="56"/>
+      <c r="F6" s="57">
+        <v>1</v>
+      </c>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="60">
+        <v>1</v>
+      </c>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="46" t="e">
+        <f>IF(OR( AND(C7=#REF!,OR(F6&lt;&gt;G6, I6&lt;&gt;J6,L6&lt;&gt;M6)),  AND(#REF!=E7,OR(G6&lt;&gt;H6,J6&lt;&gt;K6,M6&lt;&gt;N6)), AND(C7=E7, OR(F6&lt;&gt;H6,I6&lt;&gt;K6,L6&lt;&gt;N6) )), "error: different mark to same abstract","")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="52"/>
       <c r="C7" s="53" t="s">
         <v>49</v>
       </c>
       <c r="D7" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="121"/>
-      <c r="G7" s="122"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="114"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="104"/>
-      <c r="N7" s="105"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="120"/>
+      <c r="L7" s="109"/>
+      <c r="M7" s="110"/>
+      <c r="N7" s="111"/>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="53"/>
       <c r="D8" s="54"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="121"/>
-      <c r="G8" s="122"/>
-      <c r="H8" s="123"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="113"/>
-      <c r="K8" s="114"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="105"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="104"/>
+      <c r="H8" s="105"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="122"/>
+      <c r="K8" s="123"/>
+      <c r="L8" s="112"/>
+      <c r="M8" s="113"/>
+      <c r="N8" s="114"/>
       <c r="O8" s="46" t="str">
-        <f>IF(OR( AND(C9=D9,OR(F8&lt;&gt;G8, I8&lt;&gt;J8,L8&lt;&gt;M8)),  AND(D9=E9,OR(G8&lt;&gt;H8,J8&lt;&gt;K8,M8&lt;&gt;N8)), AND(C9=E9, OR(F8&lt;&gt;H8,I8&lt;&gt;K8,L8&lt;&gt;N8) )), "error: different mark to same abstract","")</f>
+        <f>IF(OR( AND(C9=D7,OR(F8&lt;&gt;G8, I8&lt;&gt;J8,L8&lt;&gt;M8)),  AND(D7=E9,OR(G8&lt;&gt;H8,J8&lt;&gt;K8,M8&lt;&gt;N8)), AND(C9=E9, OR(F8&lt;&gt;H8,I8&lt;&gt;K8,L8&lt;&gt;N8) )), "error: different mark to same abstract","")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="255" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="404" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="52"/>
       <c r="C9" s="53" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="124"/>
-      <c r="G9" s="125"/>
-      <c r="H9" s="126"/>
-      <c r="I9" s="115"/>
-      <c r="J9" s="116"/>
-      <c r="K9" s="117"/>
-      <c r="L9" s="106"/>
-      <c r="M9" s="107"/>
-      <c r="N9" s="108"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="51">
-        <v>2</v>
-      </c>
-      <c r="B10" s="128" t="s">
+      <c r="F9" s="103"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="122"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="112"/>
+      <c r="M9" s="113"/>
+      <c r="N9" s="114"/>
+    </row>
+    <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="53"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="122"/>
+      <c r="K10" s="123"/>
+      <c r="L10" s="112"/>
+      <c r="M10" s="113"/>
+      <c r="N10" s="114"/>
+      <c r="O10" s="46" t="str">
+        <f>IF(OR( AND(C11=D9,OR(F10&lt;&gt;G10, I10&lt;&gt;J10,L10&lt;&gt;M10)),  AND(D9=E11,OR(G10&lt;&gt;H10,J10&lt;&gt;K10,M10&lt;&gt;N10)), AND(C11=E11, OR(F10&lt;&gt;H10,I10&lt;&gt;K10,L10&lt;&gt;N10) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="372" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="52"/>
+      <c r="C11" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="106"/>
+      <c r="G11" s="107"/>
+      <c r="H11" s="108"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="125"/>
+      <c r="K11" s="126"/>
+      <c r="L11" s="115"/>
+      <c r="M11" s="116"/>
+      <c r="N11" s="117"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="51">
         <v>4</v>
       </c>
-      <c r="C10" s="128"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="128"/>
-      <c r="G10" s="128"/>
-      <c r="H10" s="128"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
-      <c r="K10" s="128"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="128"/>
-      <c r="N10" s="129"/>
-    </row>
-    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B11" s="52" t="s">
+      <c r="B12" s="131" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="131"/>
+      <c r="D12" s="131"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="131"/>
+      <c r="G12" s="131"/>
+      <c r="H12" s="131"/>
+      <c r="I12" s="131"/>
+      <c r="J12" s="131"/>
+      <c r="K12" s="131"/>
+      <c r="L12" s="131"/>
+      <c r="M12" s="131"/>
+      <c r="N12" s="132"/>
+    </row>
+    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="46" t="str">
-        <f>IF(OR( AND(C12=D12,OR(F11&lt;&gt;G11, I11&lt;&gt;J11,L11&lt;&gt;M11)),  AND(D12=E12,OR(G11&lt;&gt;H11,J11&lt;&gt;K11,M11&lt;&gt;N11)), AND(C12=E12, OR(F11&lt;&gt;H11,I11&lt;&gt;K11,L11&lt;&gt;N11) )), "error: different mark to same abstract","")</f>
+      <c r="C13" s="62"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="60">
+        <v>1</v>
+      </c>
+      <c r="M13" s="60"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="46" t="str">
+        <f>IF(OR( AND(C14=D16,OR(F13&lt;&gt;G13, I13&lt;&gt;J13,L13&lt;&gt;M13)),  AND(D16=E16,OR(G13&lt;&gt;H13,J13&lt;&gt;K13,M13&lt;&gt;N13)), AND(C14=E16, OR(F13&lt;&gt;H13,I13&lt;&gt;K13,L13&lt;&gt;N13) )), "error: different mark to same abstract","")</f>
+        <v>error: different mark to same abstract</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="B14" s="52"/>
+      <c r="C14" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="100"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="118"/>
+      <c r="J14" s="119"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="109"/>
+      <c r="M14" s="110"/>
+      <c r="N14" s="111"/>
+    </row>
+    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="B15" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="54"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="103"/>
+      <c r="G15" s="104"/>
+      <c r="H15" s="105"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="122"/>
+      <c r="K15" s="123"/>
+      <c r="L15" s="112"/>
+      <c r="M15" s="113"/>
+      <c r="N15" s="114"/>
+      <c r="O15" s="46" t="str">
+        <f>IF(OR( AND(C16=D14,OR(F15&lt;&gt;G15, I15&lt;&gt;J15,L15&lt;&gt;M15)),  AND(D14=E14,OR(G15&lt;&gt;H15,J15&lt;&gt;K15,M15&lt;&gt;N15)), AND(C16=E14, OR(F15&lt;&gt;H15,I15&lt;&gt;K15,L15&lt;&gt;N15) )), "error: different mark to same abstract","")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="404" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="52"/>
-      <c r="C12" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="118"/>
-      <c r="G12" s="119"/>
-      <c r="H12" s="120"/>
-      <c r="I12" s="109"/>
-      <c r="J12" s="110"/>
-      <c r="K12" s="111"/>
-      <c r="L12" s="100"/>
-      <c r="M12" s="101"/>
-      <c r="N12" s="102"/>
-    </row>
-    <row r="13" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="121"/>
-      <c r="G13" s="122"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="112"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="114"/>
-      <c r="L13" s="103"/>
-      <c r="M13" s="104"/>
-      <c r="N13" s="105"/>
-      <c r="O13" s="46" t="str">
-        <f>IF(OR( AND(C14=D14,OR(F13&lt;&gt;G13, I13&lt;&gt;J13,L13&lt;&gt;M13)),  AND(D14=E14,OR(G13&lt;&gt;H13,J13&lt;&gt;K13,M13&lt;&gt;N13)), AND(C14=E14, OR(F13&lt;&gt;H13,I13&lt;&gt;K13,L13&lt;&gt;N13) )), "error: different mark to same abstract","")</f>
+    <row r="16" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="B16" s="52"/>
+      <c r="C16" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="103"/>
+      <c r="G16" s="104"/>
+      <c r="H16" s="105"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="122"/>
+      <c r="K16" s="123"/>
+      <c r="L16" s="112"/>
+      <c r="M16" s="113"/>
+      <c r="N16" s="114"/>
+    </row>
+    <row r="17" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="B17" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="54"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="121"/>
+      <c r="J17" s="122"/>
+      <c r="K17" s="123"/>
+      <c r="L17" s="112"/>
+      <c r="M17" s="113"/>
+      <c r="N17" s="114"/>
+      <c r="O17" s="46" t="str">
+        <f>IF(OR( AND(C18=D18,OR(F17&lt;&gt;G17, I17&lt;&gt;J17,L17&lt;&gt;M17)),  AND(D18=E18,OR(G17&lt;&gt;H17,J17&lt;&gt;K17,M17&lt;&gt;N17)), AND(C18=E18, OR(F17&lt;&gt;H17,I17&lt;&gt;K17,L17&lt;&gt;N17) )), "error: different mark to same abstract","")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="344" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="52"/>
-      <c r="C14" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="121"/>
-      <c r="G14" s="122"/>
-      <c r="H14" s="123"/>
-      <c r="I14" s="112"/>
-      <c r="J14" s="113"/>
-      <c r="K14" s="114"/>
-      <c r="L14" s="103"/>
-      <c r="M14" s="104"/>
-      <c r="N14" s="105"/>
-    </row>
-    <row r="15" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="121"/>
-      <c r="G15" s="122"/>
-      <c r="H15" s="123"/>
-      <c r="I15" s="112"/>
-      <c r="J15" s="113"/>
-      <c r="K15" s="114"/>
-      <c r="L15" s="103"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
-      <c r="O15" s="46" t="str">
-        <f>IF(OR( AND(C16=D16,OR(F15&lt;&gt;G15, I15&lt;&gt;J15,L15&lt;&gt;M15)),  AND(D16=E16,OR(G15&lt;&gt;H15,J15&lt;&gt;K15,M15&lt;&gt;N15)), AND(C16=E16, OR(F15&lt;&gt;H15,I15&lt;&gt;K15,L15&lt;&gt;N15) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="340" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="52"/>
-      <c r="C16" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="56" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="124"/>
-      <c r="G16" s="125"/>
-      <c r="H16" s="126"/>
-      <c r="I16" s="115"/>
-      <c r="J16" s="116"/>
-      <c r="K16" s="117"/>
-      <c r="L16" s="106"/>
-      <c r="M16" s="107"/>
-      <c r="N16" s="108"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="51">
-        <v>3</v>
-      </c>
-      <c r="B17" s="128" t="s">
+    <row r="18" spans="1:15" ht="404" x14ac:dyDescent="0.2">
+      <c r="B18" s="52"/>
+      <c r="C18" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="106"/>
+      <c r="G18" s="107"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="124"/>
+      <c r="J18" s="125"/>
+      <c r="K18" s="126"/>
+      <c r="L18" s="115"/>
+      <c r="M18" s="116"/>
+      <c r="N18" s="117"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="51">
         <v>5</v>
       </c>
-      <c r="C17" s="128"/>
-      <c r="D17" s="128"/>
-      <c r="E17" s="128"/>
-      <c r="F17" s="128"/>
-      <c r="G17" s="128"/>
-      <c r="H17" s="128"/>
-      <c r="I17" s="128"/>
-      <c r="J17" s="128"/>
-      <c r="K17" s="128"/>
-      <c r="L17" s="128"/>
-      <c r="M17" s="128"/>
-      <c r="N17" s="129"/>
-    </row>
-    <row r="18" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="46" t="e">
-        <f>IF(OR( AND(C19=#REF!,OR(F18&lt;&gt;G18, I18&lt;&gt;J18,L18&lt;&gt;M18)),  AND(#REF!=E19,OR(G18&lt;&gt;H18,J18&lt;&gt;K18,M18&lt;&gt;N18)), AND(C19=E19, OR(F18&lt;&gt;H18,I18&lt;&gt;K18,L18&lt;&gt;N18) )), "error: different mark to same abstract","")</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="52"/>
-      <c r="C19" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="118"/>
-      <c r="G19" s="119"/>
-      <c r="H19" s="120"/>
-      <c r="I19" s="109"/>
-      <c r="J19" s="110"/>
-      <c r="K19" s="111"/>
-      <c r="L19" s="100"/>
-      <c r="M19" s="101"/>
-      <c r="N19" s="102"/>
+      <c r="B19" s="131" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="131"/>
+      <c r="D19" s="131"/>
+      <c r="E19" s="131"/>
+      <c r="F19" s="131"/>
+      <c r="G19" s="131"/>
+      <c r="H19" s="131"/>
+      <c r="I19" s="131"/>
+      <c r="J19" s="131"/>
+      <c r="K19" s="131"/>
+      <c r="L19" s="131"/>
+      <c r="M19" s="131"/>
+      <c r="N19" s="132"/>
     </row>
     <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="53"/>
+        <v>41</v>
+      </c>
       <c r="D20" s="54"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="121"/>
-      <c r="G20" s="122"/>
-      <c r="H20" s="123"/>
-      <c r="I20" s="112"/>
-      <c r="J20" s="113"/>
-      <c r="K20" s="114"/>
-      <c r="L20" s="103"/>
-      <c r="M20" s="104"/>
-      <c r="N20" s="105"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="59">
+        <v>1</v>
+      </c>
+      <c r="J20" s="59"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="60"/>
       <c r="O20" s="46" t="str">
-        <f>IF(OR( AND(C21=D19,OR(F20&lt;&gt;G20, I20&lt;&gt;J20,L20&lt;&gt;M20)),  AND(D19=E21,OR(G20&lt;&gt;H20,J20&lt;&gt;K20,M20&lt;&gt;N20)), AND(C21=E21, OR(F20&lt;&gt;H20,I20&lt;&gt;K20,L20&lt;&gt;N20) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="404" customHeight="1" x14ac:dyDescent="0.2">
+        <f>IF(OR( AND(C21=D21,OR(F20&lt;&gt;G20, I20&lt;&gt;J20,L20&lt;&gt;M20)),  AND(D21=E21,OR(G20&lt;&gt;H20,J20&lt;&gt;K20,M20&lt;&gt;N20)), AND(C21=E21, OR(F20&lt;&gt;H20,I20&lt;&gt;K20,L20&lt;&gt;N20) )), "error: different mark to same abstract","")</f>
+        <v>error: different mark to same abstract</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="289" x14ac:dyDescent="0.2">
       <c r="B21" s="52"/>
       <c r="C21" s="53" t="s">
         <v>55</v>
       </c>
       <c r="D21" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="121"/>
-      <c r="G21" s="122"/>
-      <c r="H21" s="123"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="113"/>
-      <c r="K21" s="114"/>
-      <c r="L21" s="103"/>
-      <c r="M21" s="104"/>
-      <c r="N21" s="105"/>
+      <c r="E21" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="100"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="102"/>
+      <c r="I21" s="118"/>
+      <c r="J21" s="119"/>
+      <c r="K21" s="120"/>
+      <c r="L21" s="109"/>
+      <c r="M21" s="110"/>
+      <c r="N21" s="111"/>
     </row>
     <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="53"/>
+        <v>42</v>
+      </c>
       <c r="D22" s="54"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="121"/>
-      <c r="G22" s="122"/>
-      <c r="H22" s="123"/>
-      <c r="I22" s="112"/>
-      <c r="J22" s="113"/>
-      <c r="K22" s="114"/>
-      <c r="L22" s="103"/>
-      <c r="M22" s="104"/>
-      <c r="N22" s="105"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="121"/>
+      <c r="J22" s="122"/>
+      <c r="K22" s="123"/>
+      <c r="L22" s="112"/>
+      <c r="M22" s="113"/>
+      <c r="N22" s="114"/>
       <c r="O22" s="46" t="str">
-        <f>IF(OR( AND(C23=D21,OR(F22&lt;&gt;G22, I22&lt;&gt;J22,L22&lt;&gt;M22)),  AND(D21=E23,OR(G22&lt;&gt;H22,J22&lt;&gt;K22,M22&lt;&gt;N22)), AND(C23=E23, OR(F22&lt;&gt;H22,I22&lt;&gt;K22,L22&lt;&gt;N22) )), "error: different mark to same abstract","")</f>
+        <f>IF(OR( AND(C23=D23,OR(F22&lt;&gt;G22, I22&lt;&gt;J22,L22&lt;&gt;M22)),  AND(D23=E25,OR(G22&lt;&gt;H22,J22&lt;&gt;K22,M22&lt;&gt;N22)), AND(C23=E25, OR(F22&lt;&gt;H22,I22&lt;&gt;K22,L22&lt;&gt;N22) )), "error: different mark to same abstract","")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="372" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="340" x14ac:dyDescent="0.2">
       <c r="B23" s="52"/>
       <c r="C23" s="53" t="s">
         <v>56</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="124"/>
-      <c r="G23" s="125"/>
-      <c r="H23" s="126"/>
-      <c r="I23" s="115"/>
-      <c r="J23" s="116"/>
-      <c r="K23" s="117"/>
-      <c r="L23" s="106"/>
-      <c r="M23" s="107"/>
-      <c r="N23" s="108"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="51">
-        <v>4</v>
-      </c>
-      <c r="B24" s="128" t="s">
+      <c r="E23" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="103"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="121"/>
+      <c r="J23" s="122"/>
+      <c r="K23" s="123"/>
+      <c r="L23" s="112"/>
+      <c r="M23" s="113"/>
+      <c r="N23" s="114"/>
+    </row>
+    <row r="24" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="54"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="103"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="121"/>
+      <c r="J24" s="122"/>
+      <c r="K24" s="123"/>
+      <c r="L24" s="112"/>
+      <c r="M24" s="113"/>
+      <c r="N24" s="114"/>
+      <c r="O24" s="46" t="str">
+        <f>IF(OR( AND(C25=D25,OR(F24&lt;&gt;G24, I24&lt;&gt;J24,L24&lt;&gt;M24)),  AND(D25=E23,OR(G24&lt;&gt;H24,J24&lt;&gt;K24,M24&lt;&gt;N24)), AND(C25=E23, OR(F24&lt;&gt;H24,I24&lt;&gt;K24,L24&lt;&gt;N24) )), "error: different mark to same abstract","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="52"/>
+      <c r="C25" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="106"/>
+      <c r="G25" s="107"/>
+      <c r="H25" s="108"/>
+      <c r="I25" s="124"/>
+      <c r="J25" s="125"/>
+      <c r="K25" s="126"/>
+      <c r="L25" s="115"/>
+      <c r="M25" s="116"/>
+      <c r="N25" s="117"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="51">
         <v>6</v>
       </c>
-      <c r="C24" s="128"/>
-      <c r="D24" s="128"/>
-      <c r="E24" s="128"/>
-      <c r="F24" s="128"/>
-      <c r="G24" s="128"/>
-      <c r="H24" s="128"/>
-      <c r="I24" s="128"/>
-      <c r="J24" s="128"/>
-      <c r="K24" s="128"/>
-      <c r="L24" s="128"/>
-      <c r="M24" s="128"/>
-      <c r="N24" s="129"/>
-    </row>
-    <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B25" s="52" t="s">
+      <c r="B26" s="131" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="131"/>
+      <c r="D26" s="131"/>
+      <c r="E26" s="131"/>
+      <c r="F26" s="131"/>
+      <c r="G26" s="131"/>
+      <c r="H26" s="131"/>
+      <c r="I26" s="131"/>
+      <c r="J26" s="131"/>
+      <c r="K26" s="131"/>
+      <c r="L26" s="131"/>
+      <c r="M26" s="131"/>
+      <c r="N26" s="132"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="51">
+        <v>7</v>
+      </c>
+      <c r="B27" s="131" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="131"/>
+      <c r="D27" s="131"/>
+      <c r="E27" s="131"/>
+      <c r="F27" s="131"/>
+      <c r="G27" s="131"/>
+      <c r="H27" s="131"/>
+      <c r="I27" s="131"/>
+      <c r="J27" s="131"/>
+      <c r="K27" s="131"/>
+      <c r="L27" s="131"/>
+      <c r="M27" s="131"/>
+      <c r="N27" s="132"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="51">
+        <v>8</v>
+      </c>
+      <c r="B28" s="131" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="131"/>
+      <c r="D28" s="131"/>
+      <c r="E28" s="131"/>
+      <c r="F28" s="131"/>
+      <c r="G28" s="131"/>
+      <c r="H28" s="131"/>
+      <c r="I28" s="131"/>
+      <c r="J28" s="131"/>
+      <c r="K28" s="131"/>
+      <c r="L28" s="131"/>
+      <c r="M28" s="131"/>
+      <c r="N28" s="132"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="51">
+        <v>9</v>
+      </c>
+      <c r="B29" s="131" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="131"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="131"/>
+      <c r="F29" s="131"/>
+      <c r="G29" s="131"/>
+      <c r="H29" s="131"/>
+      <c r="I29" s="131"/>
+      <c r="J29" s="131"/>
+      <c r="K29" s="131"/>
+      <c r="L29" s="131"/>
+      <c r="M29" s="131"/>
+      <c r="N29" s="132"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="51">
+        <v>10</v>
+      </c>
+      <c r="B30" s="131" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="131"/>
+      <c r="D30" s="131"/>
+      <c r="E30" s="131"/>
+      <c r="F30" s="131"/>
+      <c r="G30" s="131"/>
+      <c r="H30" s="131"/>
+      <c r="I30" s="131"/>
+      <c r="J30" s="131"/>
+      <c r="K30" s="131"/>
+      <c r="L30" s="131"/>
+      <c r="M30" s="131"/>
+      <c r="N30" s="132"/>
+    </row>
+    <row r="31" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="B31" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="46" t="str">
-        <f>IF(OR( AND(C26=D28,OR(F25&lt;&gt;G25, I25&lt;&gt;J25,L25&lt;&gt;M25)),  AND(D28=E28,OR(G25&lt;&gt;H25,J25&lt;&gt;K25,M25&lt;&gt;N25)), AND(C26=E28, OR(F25&lt;&gt;H25,I25&lt;&gt;K25,L25&lt;&gt;N25) )), "error: different mark to same abstract","")</f>
+      <c r="D31" s="54"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="59">
+        <v>1</v>
+      </c>
+      <c r="J31" s="59"/>
+      <c r="K31" s="59"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="60"/>
+      <c r="N31" s="60"/>
+    </row>
+    <row r="32" spans="1:15" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="52"/>
+      <c r="C32" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="100"/>
+      <c r="G32" s="101"/>
+      <c r="H32" s="102"/>
+      <c r="I32" s="118"/>
+      <c r="J32" s="119"/>
+      <c r="K32" s="120"/>
+      <c r="L32" s="109"/>
+      <c r="M32" s="110"/>
+      <c r="N32" s="111"/>
+      <c r="O32" s="136" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="54"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="103"/>
+      <c r="G33" s="104"/>
+      <c r="H33" s="105"/>
+      <c r="I33" s="121"/>
+      <c r="J33" s="122"/>
+      <c r="K33" s="123"/>
+      <c r="L33" s="112"/>
+      <c r="M33" s="113"/>
+      <c r="N33" s="114"/>
+      <c r="O33" s="46" t="str">
+        <f>IF(OR( AND(C34=D36,OR(F33&lt;&gt;G33, I33&lt;&gt;J33,L33&lt;&gt;M33)),  AND(D36=E34,OR(G33&lt;&gt;H33,J33&lt;&gt;K33,M33&lt;&gt;N33)), AND(C34=E34, OR(F33&lt;&gt;H33,I33&lt;&gt;K33,L33&lt;&gt;N33) )), "error: different mark to same abstract","")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="B26" s="52"/>
-      <c r="C26" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="118"/>
-      <c r="G26" s="119"/>
-      <c r="H26" s="120"/>
-      <c r="I26" s="109"/>
-      <c r="J26" s="110"/>
-      <c r="K26" s="111"/>
-      <c r="L26" s="100"/>
-      <c r="M26" s="101"/>
-      <c r="N26" s="102"/>
-    </row>
-    <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B27" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="54"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="121"/>
-      <c r="G27" s="122"/>
-      <c r="H27" s="123"/>
-      <c r="I27" s="112"/>
-      <c r="J27" s="113"/>
-      <c r="K27" s="114"/>
-      <c r="L27" s="103"/>
-      <c r="M27" s="104"/>
-      <c r="N27" s="105"/>
-      <c r="O27" s="46" t="str">
-        <f>IF(OR( AND(C28=D26,OR(F27&lt;&gt;G27, I27&lt;&gt;J27,L27&lt;&gt;M27)),  AND(D26=E26,OR(G27&lt;&gt;H27,J27&lt;&gt;K27,M27&lt;&gt;N27)), AND(C28=E26, OR(F27&lt;&gt;H27,I27&lt;&gt;K27,L27&lt;&gt;N27) )), "error: different mark to same abstract","")</f>
+    <row r="34" spans="2:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="52"/>
+      <c r="C34" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="103"/>
+      <c r="G34" s="104"/>
+      <c r="H34" s="105"/>
+      <c r="I34" s="121"/>
+      <c r="J34" s="122"/>
+      <c r="K34" s="123"/>
+      <c r="L34" s="112"/>
+      <c r="M34" s="113"/>
+      <c r="N34" s="114"/>
+    </row>
+    <row r="35" spans="2:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="53"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="103"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="105"/>
+      <c r="I35" s="121"/>
+      <c r="J35" s="122"/>
+      <c r="K35" s="123"/>
+      <c r="L35" s="112"/>
+      <c r="M35" s="113"/>
+      <c r="N35" s="114"/>
+      <c r="O35" s="46" t="str">
+        <f>IF(OR( AND(C36=D34,OR(F35&lt;&gt;G35, I35&lt;&gt;J35,L35&lt;&gt;M35)),  AND(D34=E36,OR(G35&lt;&gt;H35,J35&lt;&gt;K35,M35&lt;&gt;N35)), AND(C36=E36, OR(F35&lt;&gt;H35,I35&lt;&gt;K35,L35&lt;&gt;N35) )), "error: different mark to same abstract","")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="B28" s="52"/>
-      <c r="C28" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="F28" s="121"/>
-      <c r="G28" s="122"/>
-      <c r="H28" s="123"/>
-      <c r="I28" s="112"/>
-      <c r="J28" s="113"/>
-      <c r="K28" s="114"/>
-      <c r="L28" s="103"/>
-      <c r="M28" s="104"/>
-      <c r="N28" s="105"/>
-    </row>
-    <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="54"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="121"/>
-      <c r="G29" s="122"/>
-      <c r="H29" s="123"/>
-      <c r="I29" s="112"/>
-      <c r="J29" s="113"/>
-      <c r="K29" s="114"/>
-      <c r="L29" s="103"/>
-      <c r="M29" s="104"/>
-      <c r="N29" s="105"/>
-      <c r="O29" s="46" t="str">
-        <f>IF(OR( AND(C30=D30,OR(F29&lt;&gt;G29, I29&lt;&gt;J29,L29&lt;&gt;M29)),  AND(D30=E30,OR(G29&lt;&gt;H29,J29&lt;&gt;K29,M29&lt;&gt;N29)), AND(C30=E30, OR(F29&lt;&gt;H29,I29&lt;&gt;K29,L29&lt;&gt;N29) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="404" x14ac:dyDescent="0.2">
-      <c r="B30" s="52"/>
-      <c r="C30" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="54" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30" s="124"/>
-      <c r="G30" s="125"/>
-      <c r="H30" s="126"/>
-      <c r="I30" s="115"/>
-      <c r="J30" s="116"/>
-      <c r="K30" s="117"/>
-      <c r="L30" s="106"/>
-      <c r="M30" s="107"/>
-      <c r="N30" s="108"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="51">
-        <v>5</v>
-      </c>
-      <c r="B31" s="128" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="128"/>
-      <c r="D31" s="128"/>
-      <c r="E31" s="128"/>
-      <c r="F31" s="128"/>
-      <c r="G31" s="128"/>
-      <c r="H31" s="128"/>
-      <c r="I31" s="128"/>
-      <c r="J31" s="128"/>
-      <c r="K31" s="128"/>
-      <c r="L31" s="128"/>
-      <c r="M31" s="128"/>
-      <c r="N31" s="129"/>
-    </row>
-    <row r="32" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B32" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" s="54"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="59"/>
-      <c r="K32" s="59"/>
-      <c r="L32" s="60"/>
-      <c r="M32" s="60"/>
-      <c r="N32" s="60"/>
-      <c r="O32" s="46" t="str">
-        <f>IF(OR( AND(C33=D33,OR(F32&lt;&gt;G32, I32&lt;&gt;J32,L32&lt;&gt;M32)),  AND(D33=E33,OR(G32&lt;&gt;H32,J32&lt;&gt;K32,M32&lt;&gt;N32)), AND(C33=E33, OR(F32&lt;&gt;H32,I32&lt;&gt;K32,L32&lt;&gt;N32) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="289" x14ac:dyDescent="0.2">
-      <c r="B33" s="52"/>
-      <c r="C33" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="F33" s="118"/>
-      <c r="G33" s="119"/>
-      <c r="H33" s="120"/>
-      <c r="I33" s="109"/>
-      <c r="J33" s="110"/>
-      <c r="K33" s="111"/>
-      <c r="L33" s="100"/>
-      <c r="M33" s="101"/>
-      <c r="N33" s="102"/>
-    </row>
-    <row r="34" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B34" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="54"/>
-      <c r="E34" s="55"/>
-      <c r="F34" s="121"/>
-      <c r="G34" s="122"/>
-      <c r="H34" s="123"/>
-      <c r="I34" s="112"/>
-      <c r="J34" s="113"/>
-      <c r="K34" s="114"/>
-      <c r="L34" s="103"/>
-      <c r="M34" s="104"/>
-      <c r="N34" s="105"/>
-      <c r="O34" s="46" t="str">
-        <f>IF(OR( AND(C35=D35,OR(F34&lt;&gt;G34, I34&lt;&gt;J34,L34&lt;&gt;M34)),  AND(D35=E37,OR(G34&lt;&gt;H34,J34&lt;&gt;K34,M34&lt;&gt;N34)), AND(C35=E37, OR(F34&lt;&gt;H34,I34&lt;&gt;K34,L34&lt;&gt;N34) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="340" x14ac:dyDescent="0.2">
-      <c r="B35" s="52"/>
-      <c r="C35" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="E35" s="55" t="s">
-        <v>87</v>
-      </c>
-      <c r="F35" s="121"/>
-      <c r="G35" s="122"/>
-      <c r="H35" s="123"/>
-      <c r="I35" s="112"/>
-      <c r="J35" s="113"/>
-      <c r="K35" s="114"/>
-      <c r="L35" s="103"/>
-      <c r="M35" s="104"/>
-      <c r="N35" s="105"/>
-    </row>
-    <row r="36" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B36" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="54"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="121"/>
-      <c r="G36" s="122"/>
-      <c r="H36" s="123"/>
-      <c r="I36" s="112"/>
-      <c r="J36" s="113"/>
-      <c r="K36" s="114"/>
-      <c r="L36" s="103"/>
-      <c r="M36" s="104"/>
-      <c r="N36" s="105"/>
-      <c r="O36" s="46" t="str">
-        <f>IF(OR( AND(C37=D37,OR(F36&lt;&gt;G36, I36&lt;&gt;J36,L36&lt;&gt;M36)),  AND(D37=E35,OR(G36&lt;&gt;H36,J36&lt;&gt;K36,M36&lt;&gt;N36)), AND(C37=E35, OR(F36&lt;&gt;H36,I36&lt;&gt;K36,L36&lt;&gt;N36) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="52"/>
-      <c r="C37" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" s="54" t="s">
+    <row r="36" spans="2:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="52"/>
+      <c r="C36" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="106"/>
+      <c r="G36" s="107"/>
+      <c r="H36" s="108"/>
+      <c r="I36" s="124"/>
+      <c r="J36" s="125"/>
+      <c r="K36" s="126"/>
+      <c r="L36" s="115"/>
+      <c r="M36" s="116"/>
+      <c r="N36" s="117"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
+      <c r="L37" s="51"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="51"/>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C38" s="135" t="s">
         <v>80</v>
       </c>
-      <c r="E37" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="F37" s="124"/>
-      <c r="G37" s="125"/>
-      <c r="H37" s="126"/>
-      <c r="I37" s="115"/>
-      <c r="J37" s="116"/>
-      <c r="K37" s="117"/>
-      <c r="L37" s="106"/>
-      <c r="M37" s="107"/>
-      <c r="N37" s="108"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="51">
-        <v>6</v>
-      </c>
-      <c r="B38" s="128" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="128"/>
-      <c r="D38" s="128"/>
-      <c r="E38" s="128"/>
-      <c r="F38" s="128"/>
-      <c r="G38" s="128"/>
-      <c r="H38" s="128"/>
-      <c r="I38" s="128"/>
-      <c r="J38" s="128"/>
-      <c r="K38" s="128"/>
-      <c r="L38" s="128"/>
-      <c r="M38" s="128"/>
-      <c r="N38" s="129"/>
-    </row>
-    <row r="39" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B39" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="54"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="50"/>
-      <c r="M39" s="50"/>
-      <c r="N39" s="50"/>
-      <c r="O39" s="46" t="str">
-        <f>IF(OR( AND(C40=D40,OR(F39&lt;&gt;G39, I39&lt;&gt;J39,L39&lt;&gt;M39)),  AND(D40=E40,OR(G39&lt;&gt;H39,J39&lt;&gt;K39,M39&lt;&gt;N39)), AND(C40=E40, OR(F39&lt;&gt;H39,I39&lt;&gt;K39,L39&lt;&gt;N39) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="323" x14ac:dyDescent="0.2">
-      <c r="B40" s="52"/>
-      <c r="C40" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="54" t="s">
-        <v>63</v>
-      </c>
-      <c r="E40" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="F40" s="118"/>
-      <c r="G40" s="119"/>
-      <c r="H40" s="120"/>
-      <c r="I40" s="109"/>
-      <c r="J40" s="110"/>
-      <c r="K40" s="111"/>
-      <c r="L40" s="100"/>
-      <c r="M40" s="101"/>
-      <c r="N40" s="102"/>
-    </row>
-    <row r="41" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B41" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" s="54"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="121"/>
-      <c r="G41" s="122"/>
-      <c r="H41" s="123"/>
-      <c r="I41" s="112"/>
-      <c r="J41" s="113"/>
-      <c r="K41" s="114"/>
-      <c r="L41" s="103"/>
-      <c r="M41" s="104"/>
-      <c r="N41" s="105"/>
-      <c r="O41" s="46" t="str">
-        <f>IF(OR( AND(C42=D42,OR(F41&lt;&gt;G41, I41&lt;&gt;J41,L41&lt;&gt;M41)),  AND(D42=E42,OR(G41&lt;&gt;H41,J41&lt;&gt;K41,M41&lt;&gt;N41)), AND(C42=E42, OR(F41&lt;&gt;H41,I41&lt;&gt;K41,L41&lt;&gt;N41) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:15" ht="340" x14ac:dyDescent="0.2">
-      <c r="B42" s="52"/>
-      <c r="C42" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="54" t="s">
-        <v>64</v>
-      </c>
-      <c r="E42" s="55" t="s">
-        <v>64</v>
-      </c>
-      <c r="F42" s="121"/>
-      <c r="G42" s="122"/>
-      <c r="H42" s="123"/>
-      <c r="I42" s="112"/>
-      <c r="J42" s="113"/>
-      <c r="K42" s="114"/>
-      <c r="L42" s="103"/>
-      <c r="M42" s="104"/>
-      <c r="N42" s="105"/>
-    </row>
-    <row r="43" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B43" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="54"/>
-      <c r="E43" s="55"/>
-      <c r="F43" s="121"/>
-      <c r="G43" s="122"/>
-      <c r="H43" s="123"/>
-      <c r="I43" s="112"/>
-      <c r="J43" s="113"/>
-      <c r="K43" s="114"/>
-      <c r="L43" s="103"/>
-      <c r="M43" s="104"/>
-      <c r="N43" s="105"/>
-      <c r="O43" s="46" t="str">
-        <f>IF(OR( AND(C44=D44,OR(F43&lt;&gt;G43, I43&lt;&gt;J43,L43&lt;&gt;M43)),  AND(D44=E44,OR(G43&lt;&gt;H43,J43&lt;&gt;K43,M43&lt;&gt;N43)), AND(C44=E44, OR(F43&lt;&gt;H43,I43&lt;&gt;K43,L43&lt;&gt;N43) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="B44" s="52"/>
-      <c r="C44" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="D44" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="E44" s="55" t="s">
-        <v>65</v>
-      </c>
-      <c r="F44" s="124"/>
-      <c r="G44" s="125"/>
-      <c r="H44" s="126"/>
-      <c r="I44" s="115"/>
-      <c r="J44" s="116"/>
-      <c r="K44" s="117"/>
-      <c r="L44" s="106"/>
-      <c r="M44" s="107"/>
-      <c r="N44" s="108"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="51">
-        <v>7</v>
-      </c>
-      <c r="B45" s="128" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="128"/>
-      <c r="D45" s="128"/>
-      <c r="E45" s="128"/>
-      <c r="F45" s="128"/>
-      <c r="G45" s="128"/>
-      <c r="H45" s="128"/>
-      <c r="I45" s="128"/>
-      <c r="J45" s="128"/>
-      <c r="K45" s="128"/>
-      <c r="L45" s="128"/>
-      <c r="M45" s="128"/>
-      <c r="N45" s="129"/>
-    </row>
-    <row r="46" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B46" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" s="54"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="59"/>
-      <c r="J46" s="59"/>
-      <c r="K46" s="59"/>
-      <c r="L46" s="60"/>
-      <c r="M46" s="60"/>
-      <c r="N46" s="60"/>
-      <c r="O46" s="46" t="e">
-        <f>IF(OR( AND(C47=D47,OR(F46&lt;&gt;G46, I46&lt;&gt;J46,L46&lt;&gt;#REF!)),  AND(D47=E47,OR(G46&lt;&gt;H46,J46&lt;&gt;K46,#REF!&lt;&gt;N46)), AND(C47=E47, OR(F46&lt;&gt;H46,I46&lt;&gt;K46,L46&lt;&gt;N46) )), "error: different mark to same abstract","")</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="52"/>
-      <c r="C47" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="E47" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="F47" s="118"/>
-      <c r="G47" s="119"/>
-      <c r="H47" s="120"/>
-      <c r="I47" s="109"/>
-      <c r="J47" s="110"/>
-      <c r="K47" s="111"/>
-      <c r="L47" s="100"/>
-      <c r="M47" s="101"/>
-      <c r="N47" s="102"/>
-    </row>
-    <row r="48" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B48" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="D48" s="54"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="121"/>
-      <c r="G48" s="122"/>
-      <c r="H48" s="123"/>
-      <c r="I48" s="112"/>
-      <c r="J48" s="113"/>
-      <c r="K48" s="114"/>
-      <c r="L48" s="103"/>
-      <c r="M48" s="104"/>
-      <c r="N48" s="105"/>
-      <c r="O48" s="46" t="str">
-        <f>IF(OR( AND(C49=D49,OR(F48&lt;&gt;G48, I48&lt;&gt;J48,L48&lt;&gt;M48)),  AND(D49=E49,OR(G48&lt;&gt;H48,J48&lt;&gt;K48,M48&lt;&gt;N48)), AND(C49=E49, OR(F48&lt;&gt;H48,I48&lt;&gt;K48,L48&lt;&gt;N48) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="52"/>
-      <c r="C49" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="E49" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="F49" s="121"/>
-      <c r="G49" s="122"/>
-      <c r="H49" s="123"/>
-      <c r="I49" s="112"/>
-      <c r="J49" s="113"/>
-      <c r="K49" s="114"/>
-      <c r="L49" s="103"/>
-      <c r="M49" s="104"/>
-      <c r="N49" s="105"/>
-    </row>
-    <row r="50" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B50" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="D50" s="54"/>
-      <c r="E50" s="55"/>
-      <c r="F50" s="121"/>
-      <c r="G50" s="122"/>
-      <c r="H50" s="123"/>
-      <c r="I50" s="112"/>
-      <c r="J50" s="113"/>
-      <c r="K50" s="114"/>
-      <c r="L50" s="103"/>
-      <c r="M50" s="104"/>
-      <c r="N50" s="105"/>
-      <c r="O50" s="46" t="str">
-        <f>IF(OR( AND(C51=D51,OR(F50&lt;&gt;G50, I50&lt;&gt;J50,L50&lt;&gt;M50)),  AND(D51=E51,OR(G50&lt;&gt;H50,J50&lt;&gt;K50,M50&lt;&gt;N50)), AND(C51=E51, OR(F50&lt;&gt;H50,I50&lt;&gt;K50,L50&lt;&gt;N50) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="B51" s="52"/>
-      <c r="C51" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="D51" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="E51" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="F51" s="124"/>
-      <c r="G51" s="125"/>
-      <c r="H51" s="126"/>
-      <c r="I51" s="115"/>
-      <c r="J51" s="116"/>
-      <c r="K51" s="117"/>
-      <c r="L51" s="106"/>
-      <c r="M51" s="107"/>
-      <c r="N51" s="108"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A52" s="51">
-        <v>8</v>
-      </c>
-      <c r="B52" s="128" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" s="128"/>
-      <c r="D52" s="128"/>
-      <c r="E52" s="128"/>
-      <c r="F52" s="128"/>
-      <c r="G52" s="128"/>
-      <c r="H52" s="128"/>
-      <c r="I52" s="128"/>
-      <c r="J52" s="128"/>
-      <c r="K52" s="128"/>
-      <c r="L52" s="128"/>
-      <c r="M52" s="128"/>
-      <c r="N52" s="129"/>
-    </row>
-    <row r="53" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B53" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="D53" s="54"/>
-      <c r="E53" s="55"/>
-      <c r="F53" s="57"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="59"/>
-      <c r="J53" s="59"/>
-      <c r="K53" s="59"/>
-      <c r="L53" s="60"/>
-      <c r="M53" s="50"/>
-      <c r="N53" s="60"/>
-      <c r="O53" s="46" t="str">
-        <f>IF(OR( AND(C54=D54,OR(F53&lt;&gt;G53, I53&lt;&gt;J53,L53&lt;&gt;M46)),  AND(D54=E54,OR(G53&lt;&gt;H53,J53&lt;&gt;K53,M46&lt;&gt;N53)), AND(C54=E54, OR(F53&lt;&gt;H53,I53&lt;&gt;K53,L53&lt;&gt;N53) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="340" x14ac:dyDescent="0.2">
-      <c r="B54" s="52"/>
-      <c r="C54" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="D54" s="54" t="s">
-        <v>69</v>
-      </c>
-      <c r="E54" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="F54" s="118"/>
-      <c r="G54" s="119"/>
-      <c r="H54" s="120"/>
-      <c r="I54" s="109"/>
-      <c r="J54" s="110"/>
-      <c r="K54" s="111"/>
-      <c r="L54" s="100"/>
-      <c r="M54" s="101"/>
-      <c r="N54" s="102"/>
-    </row>
-    <row r="55" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B55" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" s="54"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="121"/>
-      <c r="G55" s="122"/>
-      <c r="H55" s="123"/>
-      <c r="I55" s="112"/>
-      <c r="J55" s="113"/>
-      <c r="K55" s="114"/>
-      <c r="L55" s="103"/>
-      <c r="M55" s="104"/>
-      <c r="N55" s="105"/>
-      <c r="O55" s="46" t="str">
-        <f>IF(OR( AND(C56=D56,OR(F55&lt;&gt;G55, I55&lt;&gt;J55,L55&lt;&gt;M55)),  AND(D56=E56,OR(G55&lt;&gt;H55,J55&lt;&gt;K55,M55&lt;&gt;N55)), AND(C56=E56, OR(F55&lt;&gt;H55,I55&lt;&gt;K55,L55&lt;&gt;N55) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="B56" s="52"/>
-      <c r="C56" s="53" t="s">
-        <v>70</v>
-      </c>
-      <c r="D56" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="E56" s="55" t="s">
-        <v>70</v>
-      </c>
-      <c r="F56" s="121"/>
-      <c r="G56" s="122"/>
-      <c r="H56" s="123"/>
-      <c r="I56" s="112"/>
-      <c r="J56" s="113"/>
-      <c r="K56" s="114"/>
-      <c r="L56" s="103"/>
-      <c r="M56" s="104"/>
-      <c r="N56" s="105"/>
-    </row>
-    <row r="57" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B57" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="D57" s="54"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="121"/>
-      <c r="G57" s="122"/>
-      <c r="H57" s="123"/>
-      <c r="I57" s="112"/>
-      <c r="J57" s="113"/>
-      <c r="K57" s="114"/>
-      <c r="L57" s="103"/>
-      <c r="M57" s="104"/>
-      <c r="N57" s="105"/>
-      <c r="O57" s="46" t="str">
-        <f>IF(OR( AND(C58=D58,OR(F57&lt;&gt;G57, I57&lt;&gt;J57,L57&lt;&gt;M57)),  AND(D58=E58,OR(G57&lt;&gt;H57,J57&lt;&gt;K57,M57&lt;&gt;N57)), AND(C58=E58, OR(F57&lt;&gt;H57,I57&lt;&gt;K57,L57&lt;&gt;N57) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="B58" s="52"/>
-      <c r="C58" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="D58" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="E58" s="55" t="s">
-        <v>89</v>
-      </c>
-      <c r="F58" s="124"/>
-      <c r="G58" s="125"/>
-      <c r="H58" s="126"/>
-      <c r="I58" s="115"/>
-      <c r="J58" s="116"/>
-      <c r="K58" s="117"/>
-      <c r="L58" s="106"/>
-      <c r="M58" s="107"/>
-      <c r="N58" s="108"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" s="51">
-        <v>9</v>
-      </c>
-      <c r="B59" s="128" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="128"/>
-      <c r="D59" s="128"/>
-      <c r="E59" s="128"/>
-      <c r="F59" s="128"/>
-      <c r="G59" s="128"/>
-      <c r="H59" s="128"/>
-      <c r="I59" s="128"/>
-      <c r="J59" s="128"/>
-      <c r="K59" s="128"/>
-      <c r="L59" s="128"/>
-      <c r="M59" s="128"/>
-      <c r="N59" s="129"/>
-    </row>
-    <row r="60" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B60" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="D60" s="54"/>
-      <c r="E60" s="55"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58"/>
-      <c r="I60" s="59"/>
-      <c r="J60" s="59"/>
-      <c r="K60" s="59"/>
-      <c r="L60" s="60"/>
-      <c r="M60" s="60"/>
-      <c r="N60" s="60"/>
-      <c r="O60" s="46" t="str">
-        <f>IF(OR( AND(C61=D61,OR(F60&lt;&gt;G60, I60&lt;&gt;J60,L60&lt;&gt;M60)),  AND(D61=E61,OR(G60&lt;&gt;H60,J60&lt;&gt;K60,M60&lt;&gt;N60)), AND(C61=E61, OR(F60&lt;&gt;H60,I60&lt;&gt;K60,L60&lt;&gt;N60) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="52"/>
-      <c r="C61" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="D61" s="54" t="s">
-        <v>72</v>
-      </c>
-      <c r="E61" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="F61" s="118"/>
-      <c r="G61" s="119"/>
-      <c r="H61" s="120"/>
-      <c r="I61" s="109"/>
-      <c r="J61" s="110"/>
-      <c r="K61" s="111"/>
-      <c r="L61" s="100"/>
-      <c r="M61" s="101"/>
-      <c r="N61" s="102"/>
-    </row>
-    <row r="62" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B62" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="D62" s="54"/>
-      <c r="E62" s="55"/>
-      <c r="F62" s="121"/>
-      <c r="G62" s="122"/>
-      <c r="H62" s="123"/>
-      <c r="I62" s="112"/>
-      <c r="J62" s="136"/>
-      <c r="K62" s="114"/>
-      <c r="L62" s="103"/>
-      <c r="M62" s="137"/>
-      <c r="N62" s="105"/>
-      <c r="O62" s="46" t="str">
-        <f>IF(OR( AND(C63=D63,OR(F62&lt;&gt;G62, I62&lt;&gt;J62,L62&lt;&gt;M62)),  AND(D63=E63,OR(G62&lt;&gt;H62,J62&lt;&gt;K62,M62&lt;&gt;N62)), AND(C63=E63, OR(F62&lt;&gt;H62,I62&lt;&gt;K62,L62&lt;&gt;N62) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:15" ht="306" x14ac:dyDescent="0.2">
-      <c r="B63" s="52"/>
-      <c r="C63" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="D63" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="E63" s="55" t="s">
-        <v>90</v>
-      </c>
-      <c r="F63" s="121"/>
-      <c r="G63" s="122"/>
-      <c r="H63" s="123"/>
-      <c r="I63" s="112"/>
-      <c r="J63" s="136"/>
-      <c r="K63" s="114"/>
-      <c r="L63" s="103"/>
-      <c r="M63" s="137"/>
-      <c r="N63" s="105"/>
-      <c r="O63" s="51"/>
-    </row>
-    <row r="64" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B64" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="D64" s="54"/>
-      <c r="E64" s="55"/>
-      <c r="F64" s="121"/>
-      <c r="G64" s="122"/>
-      <c r="H64" s="123"/>
-      <c r="I64" s="112"/>
-      <c r="J64" s="136"/>
-      <c r="K64" s="114"/>
-      <c r="L64" s="103"/>
-      <c r="M64" s="137"/>
-      <c r="N64" s="105"/>
-      <c r="O64" s="46" t="str">
-        <f>IF(OR( AND(C65=D65,OR(F64&lt;&gt;G64, I64&lt;&gt;J64,L64&lt;&gt;M64)),  AND(D65=E65,OR(G64&lt;&gt;H64,J64&lt;&gt;K64,M64&lt;&gt;N64)), AND(C65=E65, OR(F64&lt;&gt;H64,I64&lt;&gt;K64,L64&lt;&gt;N64) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:15" ht="388" x14ac:dyDescent="0.2">
-      <c r="B65" s="52"/>
-      <c r="C65" s="53" t="s">
-        <v>74</v>
-      </c>
-      <c r="D65" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="E65" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="F65" s="124"/>
-      <c r="G65" s="125"/>
-      <c r="H65" s="126"/>
-      <c r="I65" s="115"/>
-      <c r="J65" s="116"/>
-      <c r="K65" s="117"/>
-      <c r="L65" s="106"/>
-      <c r="M65" s="107"/>
-      <c r="N65" s="108"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A66" s="51">
-        <v>10</v>
-      </c>
-      <c r="B66" s="128" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="128"/>
-      <c r="D66" s="128"/>
-      <c r="E66" s="128"/>
-      <c r="F66" s="128"/>
-      <c r="G66" s="128"/>
-      <c r="H66" s="128"/>
-      <c r="I66" s="128"/>
-      <c r="J66" s="128"/>
-      <c r="K66" s="128"/>
-      <c r="L66" s="128"/>
-      <c r="M66" s="128"/>
-      <c r="N66" s="129"/>
-    </row>
-    <row r="67" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="B67" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="D67" s="54"/>
-      <c r="E67" s="55"/>
-      <c r="F67" s="57"/>
-      <c r="G67" s="58"/>
-      <c r="H67" s="58"/>
-      <c r="I67" s="59"/>
-      <c r="J67" s="59"/>
-      <c r="K67" s="59"/>
-      <c r="L67" s="60"/>
-      <c r="M67" s="60"/>
-      <c r="N67" s="60"/>
-      <c r="O67" s="46" t="str">
-        <f>IF(OR( AND(C68=D68,OR(F67&lt;&gt;G67, I67&lt;&gt;J67,L67&lt;&gt;M67)),  AND(D68=E68,OR(G67&lt;&gt;H67,J67&lt;&gt;K67,M67&lt;&gt;N67)), AND(C68=E68, OR(F67&lt;&gt;H67,I67&lt;&gt;K67,L67&lt;&gt;N67) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:15" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="52"/>
-      <c r="C68" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="D68" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="E68" s="55" t="s">
-        <v>75</v>
-      </c>
-      <c r="F68" s="118"/>
-      <c r="G68" s="119"/>
-      <c r="H68" s="120"/>
-      <c r="I68" s="109"/>
-      <c r="J68" s="110"/>
-      <c r="K68" s="111"/>
-      <c r="L68" s="100"/>
-      <c r="M68" s="101"/>
-      <c r="N68" s="102"/>
-    </row>
-    <row r="69" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="D69" s="54"/>
-      <c r="E69" s="55"/>
-      <c r="F69" s="121"/>
-      <c r="G69" s="138"/>
-      <c r="H69" s="123"/>
-      <c r="I69" s="112"/>
-      <c r="J69" s="136"/>
-      <c r="K69" s="114"/>
-      <c r="L69" s="103"/>
-      <c r="M69" s="137"/>
-      <c r="N69" s="105"/>
-      <c r="O69" s="46" t="str">
-        <f>IF(OR( AND(C70=D72,OR(F69&lt;&gt;G69, I69&lt;&gt;J69,L69&lt;&gt;M69)),  AND(D72=E70,OR(G69&lt;&gt;H69,J69&lt;&gt;K69,M69&lt;&gt;N69)), AND(C70=E70, OR(F69&lt;&gt;H69,I69&lt;&gt;K69,L69&lt;&gt;N69) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="52"/>
-      <c r="C70" s="53" t="s">
-        <v>76</v>
-      </c>
-      <c r="D70" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="E70" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="F70" s="121"/>
-      <c r="G70" s="138"/>
-      <c r="H70" s="123"/>
-      <c r="I70" s="112"/>
-      <c r="J70" s="136"/>
-      <c r="K70" s="114"/>
-      <c r="L70" s="103"/>
-      <c r="M70" s="137"/>
-      <c r="N70" s="105"/>
-    </row>
-    <row r="71" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="C71" s="53"/>
-      <c r="D71" s="54"/>
-      <c r="E71" s="55"/>
-      <c r="F71" s="121"/>
-      <c r="G71" s="138"/>
-      <c r="H71" s="123"/>
-      <c r="I71" s="112"/>
-      <c r="J71" s="136"/>
-      <c r="K71" s="114"/>
-      <c r="L71" s="103"/>
-      <c r="M71" s="137"/>
-      <c r="N71" s="105"/>
-      <c r="O71" s="46" t="str">
-        <f>IF(OR( AND(C72=D70,OR(F71&lt;&gt;G71, I71&lt;&gt;J71,L71&lt;&gt;M71)),  AND(D70=E72,OR(G71&lt;&gt;H71,J71&lt;&gt;K71,M71&lt;&gt;N71)), AND(C72=E72, OR(F71&lt;&gt;H71,I71&lt;&gt;K71,L71&lt;&gt;N71) )), "error: different mark to same abstract","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="52"/>
-      <c r="C72" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="D72" s="54" t="s">
-        <v>76</v>
-      </c>
-      <c r="E72" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="F72" s="124"/>
-      <c r="G72" s="125"/>
-      <c r="H72" s="126"/>
-      <c r="I72" s="115"/>
-      <c r="J72" s="116"/>
-      <c r="K72" s="117"/>
-      <c r="L72" s="106"/>
-      <c r="M72" s="107"/>
-      <c r="N72" s="108"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D38" s="135"/>
+      <c r="E38" s="135"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="51"/>
+      <c r="K38" s="51"/>
+      <c r="L38" s="51"/>
+      <c r="M38" s="51"/>
+      <c r="N38" s="51"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C39" s="64" t="e">
+        <f>AVERAGE(AVERAGE(F4:F35),AVERAGE(G4:G38),AVERAGE(H4:H38))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D39" s="64" t="e">
+        <f>AVERAGE(AVERAGE(I4:I35),AVERAGE(J4:J38),AVERAGE(K4:K38))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E39" s="64" t="e">
+        <f>AVERAGE(AVERAGE(L4:L35),AVERAGE(M4:M38),AVERAGE(N4:N38))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="51"/>
+      <c r="M40" s="51"/>
+      <c r="N40" s="51"/>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="51"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="51"/>
+      <c r="L41" s="51"/>
+      <c r="M41" s="51"/>
+      <c r="N41" s="51"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="51"/>
+      <c r="K42" s="51"/>
+      <c r="L42" s="51"/>
+      <c r="M42" s="51"/>
+      <c r="N42" s="51"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="51"/>
+      <c r="L43" s="51"/>
+      <c r="M43" s="51"/>
+      <c r="N43" s="51"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="51"/>
+      <c r="M44" s="51"/>
+      <c r="N44" s="51"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="51"/>
+      <c r="M45" s="51"/>
+      <c r="N45" s="51"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="51"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="51"/>
+      <c r="M46" s="51"/>
+      <c r="N46" s="51"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="51"/>
+      <c r="L47" s="51"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="51"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="51"/>
+      <c r="I48" s="51"/>
+      <c r="J48" s="51"/>
+      <c r="K48" s="51"/>
+      <c r="L48" s="51"/>
+      <c r="M48" s="51"/>
+      <c r="N48" s="51"/>
+    </row>
+    <row r="49" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="51"/>
+      <c r="K49" s="51"/>
+      <c r="L49" s="51"/>
+      <c r="M49" s="51"/>
+      <c r="N49" s="51"/>
+    </row>
+    <row r="50" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="51"/>
+      <c r="I50" s="51"/>
+      <c r="J50" s="51"/>
+      <c r="K50" s="51"/>
+      <c r="L50" s="51"/>
+      <c r="M50" s="51"/>
+      <c r="N50" s="51"/>
+    </row>
+    <row r="51" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="51"/>
+      <c r="K51" s="51"/>
+      <c r="L51" s="51"/>
+      <c r="M51" s="51"/>
+      <c r="N51" s="51"/>
+    </row>
+    <row r="52" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C52" s="46"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="51"/>
+      <c r="J52" s="51"/>
+      <c r="K52" s="51"/>
+      <c r="L52" s="51"/>
+      <c r="M52" s="51"/>
+      <c r="N52" s="51"/>
+    </row>
+    <row r="53" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C53" s="46"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="51"/>
+      <c r="H53" s="51"/>
+      <c r="I53" s="51"/>
+      <c r="J53" s="51"/>
+      <c r="K53" s="51"/>
+      <c r="L53" s="51"/>
+      <c r="M53" s="51"/>
+      <c r="N53" s="51"/>
+    </row>
+    <row r="54" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="51"/>
+      <c r="H54" s="51"/>
+      <c r="I54" s="51"/>
+      <c r="J54" s="51"/>
+      <c r="K54" s="51"/>
+      <c r="L54" s="51"/>
+      <c r="M54" s="51"/>
+      <c r="N54" s="51"/>
+    </row>
+    <row r="55" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C55" s="46"/>
+      <c r="D55" s="46"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="51"/>
+      <c r="I55" s="51"/>
+      <c r="J55" s="51"/>
+      <c r="K55" s="51"/>
+      <c r="L55" s="51"/>
+      <c r="M55" s="51"/>
+      <c r="N55" s="51"/>
+    </row>
+    <row r="56" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C56" s="46"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="51"/>
+      <c r="I56" s="51"/>
+      <c r="J56" s="51"/>
+      <c r="K56" s="51"/>
+      <c r="L56" s="51"/>
+      <c r="M56" s="51"/>
+      <c r="N56" s="51"/>
+    </row>
+    <row r="57" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="51"/>
+      <c r="G57" s="51"/>
+      <c r="H57" s="51"/>
+      <c r="I57" s="51"/>
+      <c r="J57" s="51"/>
+      <c r="K57" s="51"/>
+      <c r="L57" s="51"/>
+      <c r="M57" s="51"/>
+      <c r="N57" s="51"/>
+    </row>
+    <row r="58" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C58" s="46"/>
+      <c r="D58" s="46"/>
+      <c r="E58" s="46"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="51"/>
+      <c r="H58" s="51"/>
+      <c r="I58" s="51"/>
+      <c r="J58" s="51"/>
+      <c r="K58" s="51"/>
+      <c r="L58" s="51"/>
+      <c r="M58" s="51"/>
+      <c r="N58" s="51"/>
+    </row>
+    <row r="59" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C59" s="46"/>
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
+      <c r="H59" s="51"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="51"/>
+      <c r="K59" s="51"/>
+      <c r="L59" s="51"/>
+      <c r="M59" s="51"/>
+      <c r="N59" s="51"/>
+    </row>
+    <row r="60" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C60" s="46"/>
+      <c r="D60" s="46"/>
+      <c r="E60" s="46"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="51"/>
+      <c r="H60" s="51"/>
+      <c r="I60" s="51"/>
+      <c r="J60" s="51"/>
+      <c r="K60" s="51"/>
+      <c r="L60" s="51"/>
+      <c r="M60" s="51"/>
+    </row>
+    <row r="61" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C61" s="46"/>
+      <c r="D61" s="46"/>
+      <c r="E61" s="46"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="51"/>
+      <c r="H61" s="51"/>
+      <c r="I61" s="51"/>
+      <c r="J61" s="51"/>
+      <c r="K61" s="51"/>
+      <c r="L61" s="51"/>
+      <c r="M61" s="51"/>
+    </row>
+    <row r="62" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C62" s="46"/>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="51"/>
+      <c r="G62" s="51"/>
+      <c r="H62" s="51"/>
+      <c r="I62" s="51"/>
+      <c r="J62" s="51"/>
+      <c r="K62" s="51"/>
+      <c r="L62" s="51"/>
+      <c r="M62" s="51"/>
+    </row>
+    <row r="63" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C63" s="46"/>
+      <c r="D63" s="46"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="51"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="51"/>
+      <c r="I63" s="51"/>
+      <c r="J63" s="51"/>
+      <c r="K63" s="51"/>
+      <c r="L63" s="51"/>
+      <c r="M63" s="51"/>
+    </row>
+    <row r="64" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C64" s="46"/>
+      <c r="D64" s="46"/>
+      <c r="E64" s="46"/>
+      <c r="F64" s="51"/>
+      <c r="G64" s="51"/>
+      <c r="H64" s="51"/>
+      <c r="I64" s="51"/>
+      <c r="J64" s="51"/>
+      <c r="K64" s="51"/>
+      <c r="L64" s="51"/>
+      <c r="M64" s="51"/>
+    </row>
+    <row r="65" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C65" s="46"/>
+      <c r="D65" s="46"/>
+      <c r="E65" s="46"/>
+      <c r="F65" s="51"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="51"/>
+      <c r="I65" s="51"/>
+      <c r="J65" s="51"/>
+      <c r="K65" s="51"/>
+      <c r="L65" s="51"/>
+      <c r="M65" s="51"/>
+    </row>
+    <row r="66" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="51"/>
+      <c r="G66" s="51"/>
+      <c r="H66" s="51"/>
+      <c r="I66" s="51"/>
+      <c r="J66" s="51"/>
+      <c r="K66" s="51"/>
+      <c r="L66" s="51"/>
+      <c r="M66" s="51"/>
+    </row>
+    <row r="67" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C67" s="46"/>
+      <c r="D67" s="46"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="51"/>
+      <c r="G67" s="51"/>
+      <c r="H67" s="51"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="51"/>
+      <c r="K67" s="51"/>
+      <c r="L67" s="51"/>
+      <c r="M67" s="51"/>
+    </row>
+    <row r="68" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C68" s="46"/>
+      <c r="D68" s="46"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="51"/>
+      <c r="G68" s="51"/>
+      <c r="H68" s="51"/>
+      <c r="I68" s="51"/>
+      <c r="J68" s="51"/>
+      <c r="K68" s="51"/>
+      <c r="L68" s="51"/>
+      <c r="M68" s="51"/>
+    </row>
+    <row r="69" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C69" s="46"/>
+      <c r="D69" s="46"/>
+      <c r="E69" s="46"/>
+      <c r="F69" s="51"/>
+      <c r="G69" s="51"/>
+      <c r="H69" s="51"/>
+      <c r="I69" s="51"/>
+      <c r="J69" s="51"/>
+      <c r="K69" s="51"/>
+      <c r="L69" s="51"/>
+      <c r="M69" s="51"/>
+    </row>
+    <row r="70" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C70" s="46"/>
+      <c r="D70" s="46"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="51"/>
+      <c r="G70" s="51"/>
+      <c r="H70" s="51"/>
+      <c r="I70" s="51"/>
+      <c r="J70" s="51"/>
+      <c r="K70" s="51"/>
+      <c r="L70" s="51"/>
+      <c r="M70" s="51"/>
+    </row>
+    <row r="71" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C71" s="46"/>
+      <c r="D71" s="46"/>
+      <c r="E71" s="46"/>
+      <c r="F71" s="51"/>
+      <c r="G71" s="51"/>
+      <c r="H71" s="51"/>
+      <c r="I71" s="51"/>
+      <c r="J71" s="51"/>
+      <c r="K71" s="51"/>
+      <c r="L71" s="51"/>
+      <c r="M71" s="51"/>
+    </row>
+    <row r="72" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C72" s="46"/>
+      <c r="D72" s="46"/>
+      <c r="E72" s="46"/>
+      <c r="F72" s="51"/>
+      <c r="G72" s="51"/>
+      <c r="H72" s="51"/>
+      <c r="I72" s="51"/>
+      <c r="J72" s="51"/>
+      <c r="K72" s="51"/>
+      <c r="L72" s="51"/>
+      <c r="M72" s="51"/>
+    </row>
+    <row r="73" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C73" s="46"/>
       <c r="D73" s="46"/>
       <c r="E73" s="46"/>
@@ -6352,14 +6133,11 @@
       <c r="K73" s="51"/>
       <c r="L73" s="51"/>
       <c r="M73" s="51"/>
-      <c r="N73" s="51"/>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C74" s="127" t="s">
-        <v>92</v>
-      </c>
-      <c r="D74" s="127"/>
-      <c r="E74" s="127"/>
+    </row>
+    <row r="74" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C74" s="46"/>
+      <c r="D74" s="46"/>
+      <c r="E74" s="46"/>
       <c r="F74" s="51"/>
       <c r="G74" s="51"/>
       <c r="H74" s="51"/>
@@ -6368,21 +6146,11 @@
       <c r="K74" s="51"/>
       <c r="L74" s="51"/>
       <c r="M74" s="51"/>
-      <c r="N74" s="51"/>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C75" s="64" t="e">
-        <f>AVERAGE(AVERAGE(F4:F71),AVERAGE(G4:G74),AVERAGE(H4:H74))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D75" s="64" t="e">
-        <f>AVERAGE(AVERAGE(I4:I71),AVERAGE(J4:J74),AVERAGE(K4:K74))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E75" s="64" t="e">
-        <f>AVERAGE(AVERAGE(L4:L71),AVERAGE(M4:M74),AVERAGE(N4:N74))</f>
-        <v>#DIV/0!</v>
-      </c>
+    </row>
+    <row r="75" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
       <c r="F75" s="51"/>
       <c r="G75" s="51"/>
       <c r="H75" s="51"/>
@@ -6391,9 +6159,8 @@
       <c r="K75" s="51"/>
       <c r="L75" s="51"/>
       <c r="M75" s="51"/>
-      <c r="N75" s="51"/>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C76" s="46"/>
       <c r="D76" s="46"/>
       <c r="E76" s="46"/>
@@ -6405,9 +6172,8 @@
       <c r="K76" s="51"/>
       <c r="L76" s="51"/>
       <c r="M76" s="51"/>
-      <c r="N76" s="51"/>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C77" s="46"/>
       <c r="D77" s="46"/>
       <c r="E77" s="46"/>
@@ -6419,9 +6185,8 @@
       <c r="K77" s="51"/>
       <c r="L77" s="51"/>
       <c r="M77" s="51"/>
-      <c r="N77" s="51"/>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C78" s="46"/>
       <c r="D78" s="46"/>
       <c r="E78" s="46"/>
@@ -6433,9 +6198,8 @@
       <c r="K78" s="51"/>
       <c r="L78" s="51"/>
       <c r="M78" s="51"/>
-      <c r="N78" s="51"/>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C79" s="46"/>
       <c r="D79" s="46"/>
       <c r="E79" s="46"/>
@@ -6447,9 +6211,8 @@
       <c r="K79" s="51"/>
       <c r="L79" s="51"/>
       <c r="M79" s="51"/>
-      <c r="N79" s="51"/>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C80" s="46"/>
       <c r="D80" s="46"/>
       <c r="E80" s="46"/>
@@ -6461,9 +6224,8 @@
       <c r="K80" s="51"/>
       <c r="L80" s="51"/>
       <c r="M80" s="51"/>
-      <c r="N80" s="51"/>
-    </row>
-    <row r="81" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C81" s="46"/>
       <c r="D81" s="46"/>
       <c r="E81" s="46"/>
@@ -6475,9 +6237,8 @@
       <c r="K81" s="51"/>
       <c r="L81" s="51"/>
       <c r="M81" s="51"/>
-      <c r="N81" s="51"/>
-    </row>
-    <row r="82" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C82" s="46"/>
       <c r="D82" s="46"/>
       <c r="E82" s="46"/>
@@ -6489,9 +6250,8 @@
       <c r="K82" s="51"/>
       <c r="L82" s="51"/>
       <c r="M82" s="51"/>
-      <c r="N82" s="51"/>
-    </row>
-    <row r="83" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C83" s="46"/>
       <c r="D83" s="46"/>
       <c r="E83" s="46"/>
@@ -6503,9 +6263,8 @@
       <c r="K83" s="51"/>
       <c r="L83" s="51"/>
       <c r="M83" s="51"/>
-      <c r="N83" s="51"/>
-    </row>
-    <row r="84" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C84" s="46"/>
       <c r="D84" s="46"/>
       <c r="E84" s="46"/>
@@ -6517,9 +6276,8 @@
       <c r="K84" s="51"/>
       <c r="L84" s="51"/>
       <c r="M84" s="51"/>
-      <c r="N84" s="51"/>
-    </row>
-    <row r="85" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C85" s="46"/>
       <c r="D85" s="46"/>
       <c r="E85" s="46"/>
@@ -6531,9 +6289,8 @@
       <c r="K85" s="51"/>
       <c r="L85" s="51"/>
       <c r="M85" s="51"/>
-      <c r="N85" s="51"/>
-    </row>
-    <row r="86" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C86" s="46"/>
       <c r="D86" s="46"/>
       <c r="E86" s="46"/>
@@ -6545,9 +6302,8 @@
       <c r="K86" s="51"/>
       <c r="L86" s="51"/>
       <c r="M86" s="51"/>
-      <c r="N86" s="51"/>
-    </row>
-    <row r="87" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C87" s="46"/>
       <c r="D87" s="46"/>
       <c r="E87" s="46"/>
@@ -6559,9 +6315,8 @@
       <c r="K87" s="51"/>
       <c r="L87" s="51"/>
       <c r="M87" s="51"/>
-      <c r="N87" s="51"/>
-    </row>
-    <row r="88" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C88" s="46"/>
       <c r="D88" s="46"/>
       <c r="E88" s="46"/>
@@ -6573,9 +6328,8 @@
       <c r="K88" s="51"/>
       <c r="L88" s="51"/>
       <c r="M88" s="51"/>
-      <c r="N88" s="51"/>
-    </row>
-    <row r="89" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C89" s="46"/>
       <c r="D89" s="46"/>
       <c r="E89" s="46"/>
@@ -6587,9 +6341,8 @@
       <c r="K89" s="51"/>
       <c r="L89" s="51"/>
       <c r="M89" s="51"/>
-      <c r="N89" s="51"/>
-    </row>
-    <row r="90" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C90" s="46"/>
       <c r="D90" s="46"/>
       <c r="E90" s="46"/>
@@ -6601,9 +6354,8 @@
       <c r="K90" s="51"/>
       <c r="L90" s="51"/>
       <c r="M90" s="51"/>
-      <c r="N90" s="51"/>
-    </row>
-    <row r="91" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C91" s="46"/>
       <c r="D91" s="46"/>
       <c r="E91" s="46"/>
@@ -6615,9 +6367,8 @@
       <c r="K91" s="51"/>
       <c r="L91" s="51"/>
       <c r="M91" s="51"/>
-      <c r="N91" s="51"/>
-    </row>
-    <row r="92" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C92" s="46"/>
       <c r="D92" s="46"/>
       <c r="E92" s="46"/>
@@ -6629,9 +6380,8 @@
       <c r="K92" s="51"/>
       <c r="L92" s="51"/>
       <c r="M92" s="51"/>
-      <c r="N92" s="51"/>
-    </row>
-    <row r="93" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C93" s="46"/>
       <c r="D93" s="46"/>
       <c r="E93" s="46"/>
@@ -6643,9 +6393,8 @@
       <c r="K93" s="51"/>
       <c r="L93" s="51"/>
       <c r="M93" s="51"/>
-      <c r="N93" s="51"/>
-    </row>
-    <row r="94" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C94" s="46"/>
       <c r="D94" s="46"/>
       <c r="E94" s="46"/>
@@ -6657,9 +6406,8 @@
       <c r="K94" s="51"/>
       <c r="L94" s="51"/>
       <c r="M94" s="51"/>
-      <c r="N94" s="51"/>
-    </row>
-    <row r="95" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C95" s="46"/>
       <c r="D95" s="46"/>
       <c r="E95" s="46"/>
@@ -6671,9 +6419,8 @@
       <c r="K95" s="51"/>
       <c r="L95" s="51"/>
       <c r="M95" s="51"/>
-      <c r="N95" s="51"/>
-    </row>
-    <row r="96" spans="3:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C96" s="46"/>
       <c r="D96" s="46"/>
       <c r="E96" s="46"/>
@@ -8207,482 +7954,22 @@
       <c r="L213" s="51"/>
       <c r="M213" s="51"/>
     </row>
-    <row r="214" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C214" s="46"/>
-      <c r="D214" s="46"/>
-      <c r="E214" s="46"/>
-      <c r="F214" s="51"/>
-      <c r="G214" s="51"/>
-      <c r="H214" s="51"/>
-      <c r="I214" s="51"/>
-      <c r="J214" s="51"/>
-      <c r="K214" s="51"/>
-      <c r="L214" s="51"/>
-      <c r="M214" s="51"/>
-    </row>
-    <row r="215" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C215" s="46"/>
-      <c r="D215" s="46"/>
-      <c r="E215" s="46"/>
-      <c r="F215" s="51"/>
-      <c r="G215" s="51"/>
-      <c r="H215" s="51"/>
-      <c r="I215" s="51"/>
-      <c r="J215" s="51"/>
-      <c r="K215" s="51"/>
-      <c r="L215" s="51"/>
-      <c r="M215" s="51"/>
-    </row>
-    <row r="216" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C216" s="46"/>
-      <c r="D216" s="46"/>
-      <c r="E216" s="46"/>
-      <c r="F216" s="51"/>
-      <c r="G216" s="51"/>
-      <c r="H216" s="51"/>
-      <c r="I216" s="51"/>
-      <c r="J216" s="51"/>
-      <c r="K216" s="51"/>
-      <c r="L216" s="51"/>
-      <c r="M216" s="51"/>
-    </row>
-    <row r="217" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C217" s="46"/>
-      <c r="D217" s="46"/>
-      <c r="E217" s="46"/>
-      <c r="F217" s="51"/>
-      <c r="G217" s="51"/>
-      <c r="H217" s="51"/>
-      <c r="I217" s="51"/>
-      <c r="J217" s="51"/>
-      <c r="K217" s="51"/>
-      <c r="L217" s="51"/>
-      <c r="M217" s="51"/>
-    </row>
-    <row r="218" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C218" s="46"/>
-      <c r="D218" s="46"/>
-      <c r="E218" s="46"/>
-      <c r="F218" s="51"/>
-      <c r="G218" s="51"/>
-      <c r="H218" s="51"/>
-      <c r="I218" s="51"/>
-      <c r="J218" s="51"/>
-      <c r="K218" s="51"/>
-      <c r="L218" s="51"/>
-      <c r="M218" s="51"/>
-    </row>
-    <row r="219" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C219" s="46"/>
-      <c r="D219" s="46"/>
-      <c r="E219" s="46"/>
-      <c r="F219" s="51"/>
-      <c r="G219" s="51"/>
-      <c r="H219" s="51"/>
-      <c r="I219" s="51"/>
-      <c r="J219" s="51"/>
-      <c r="K219" s="51"/>
-      <c r="L219" s="51"/>
-      <c r="M219" s="51"/>
-    </row>
-    <row r="220" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C220" s="46"/>
-      <c r="D220" s="46"/>
-      <c r="E220" s="46"/>
-      <c r="F220" s="51"/>
-      <c r="G220" s="51"/>
-      <c r="H220" s="51"/>
-      <c r="I220" s="51"/>
-      <c r="J220" s="51"/>
-      <c r="K220" s="51"/>
-      <c r="L220" s="51"/>
-      <c r="M220" s="51"/>
-    </row>
-    <row r="221" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C221" s="46"/>
-      <c r="D221" s="46"/>
-      <c r="E221" s="46"/>
-      <c r="F221" s="51"/>
-      <c r="G221" s="51"/>
-      <c r="H221" s="51"/>
-      <c r="I221" s="51"/>
-      <c r="J221" s="51"/>
-      <c r="K221" s="51"/>
-      <c r="L221" s="51"/>
-      <c r="M221" s="51"/>
-    </row>
-    <row r="222" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C222" s="46"/>
-      <c r="D222" s="46"/>
-      <c r="E222" s="46"/>
-      <c r="F222" s="51"/>
-      <c r="G222" s="51"/>
-      <c r="H222" s="51"/>
-      <c r="I222" s="51"/>
-      <c r="J222" s="51"/>
-      <c r="K222" s="51"/>
-      <c r="L222" s="51"/>
-      <c r="M222" s="51"/>
-    </row>
-    <row r="223" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C223" s="46"/>
-      <c r="D223" s="46"/>
-      <c r="E223" s="46"/>
-      <c r="F223" s="51"/>
-      <c r="G223" s="51"/>
-      <c r="H223" s="51"/>
-      <c r="I223" s="51"/>
-      <c r="J223" s="51"/>
-      <c r="K223" s="51"/>
-      <c r="L223" s="51"/>
-      <c r="M223" s="51"/>
-    </row>
-    <row r="224" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C224" s="46"/>
-      <c r="D224" s="46"/>
-      <c r="E224" s="46"/>
-      <c r="F224" s="51"/>
-      <c r="G224" s="51"/>
-      <c r="H224" s="51"/>
-      <c r="I224" s="51"/>
-      <c r="J224" s="51"/>
-      <c r="K224" s="51"/>
-      <c r="L224" s="51"/>
-      <c r="M224" s="51"/>
-    </row>
-    <row r="225" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C225" s="46"/>
-      <c r="D225" s="46"/>
-      <c r="E225" s="46"/>
-      <c r="F225" s="51"/>
-      <c r="G225" s="51"/>
-      <c r="H225" s="51"/>
-      <c r="I225" s="51"/>
-      <c r="J225" s="51"/>
-      <c r="K225" s="51"/>
-      <c r="L225" s="51"/>
-      <c r="M225" s="51"/>
-    </row>
-    <row r="226" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C226" s="46"/>
-      <c r="D226" s="46"/>
-      <c r="E226" s="46"/>
-      <c r="F226" s="51"/>
-      <c r="G226" s="51"/>
-      <c r="H226" s="51"/>
-      <c r="I226" s="51"/>
-      <c r="J226" s="51"/>
-      <c r="K226" s="51"/>
-      <c r="L226" s="51"/>
-      <c r="M226" s="51"/>
-    </row>
-    <row r="227" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C227" s="46"/>
-      <c r="D227" s="46"/>
-      <c r="E227" s="46"/>
-      <c r="F227" s="51"/>
-      <c r="G227" s="51"/>
-      <c r="H227" s="51"/>
-      <c r="I227" s="51"/>
-      <c r="J227" s="51"/>
-      <c r="K227" s="51"/>
-      <c r="L227" s="51"/>
-      <c r="M227" s="51"/>
-    </row>
-    <row r="228" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C228" s="46"/>
-      <c r="D228" s="46"/>
-      <c r="E228" s="46"/>
-      <c r="F228" s="51"/>
-      <c r="G228" s="51"/>
-      <c r="H228" s="51"/>
-      <c r="I228" s="51"/>
-      <c r="J228" s="51"/>
-      <c r="K228" s="51"/>
-      <c r="L228" s="51"/>
-      <c r="M228" s="51"/>
-    </row>
-    <row r="229" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C229" s="46"/>
-      <c r="D229" s="46"/>
-      <c r="E229" s="46"/>
-      <c r="F229" s="51"/>
-      <c r="G229" s="51"/>
-      <c r="H229" s="51"/>
-      <c r="I229" s="51"/>
-      <c r="J229" s="51"/>
-      <c r="K229" s="51"/>
-      <c r="L229" s="51"/>
-      <c r="M229" s="51"/>
-    </row>
-    <row r="230" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C230" s="46"/>
-      <c r="D230" s="46"/>
-      <c r="E230" s="46"/>
-      <c r="F230" s="51"/>
-      <c r="G230" s="51"/>
-      <c r="H230" s="51"/>
-      <c r="I230" s="51"/>
-      <c r="J230" s="51"/>
-      <c r="K230" s="51"/>
-      <c r="L230" s="51"/>
-      <c r="M230" s="51"/>
-    </row>
-    <row r="231" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C231" s="46"/>
-      <c r="D231" s="46"/>
-      <c r="E231" s="46"/>
-      <c r="F231" s="51"/>
-      <c r="G231" s="51"/>
-      <c r="H231" s="51"/>
-      <c r="I231" s="51"/>
-      <c r="J231" s="51"/>
-      <c r="K231" s="51"/>
-      <c r="L231" s="51"/>
-      <c r="M231" s="51"/>
-    </row>
-    <row r="232" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C232" s="46"/>
-      <c r="D232" s="46"/>
-      <c r="E232" s="46"/>
-      <c r="F232" s="51"/>
-      <c r="G232" s="51"/>
-      <c r="H232" s="51"/>
-      <c r="I232" s="51"/>
-      <c r="J232" s="51"/>
-      <c r="K232" s="51"/>
-      <c r="L232" s="51"/>
-      <c r="M232" s="51"/>
-    </row>
-    <row r="233" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C233" s="46"/>
-      <c r="D233" s="46"/>
-      <c r="E233" s="46"/>
-      <c r="F233" s="51"/>
-      <c r="G233" s="51"/>
-      <c r="H233" s="51"/>
-      <c r="I233" s="51"/>
-      <c r="J233" s="51"/>
-      <c r="K233" s="51"/>
-      <c r="L233" s="51"/>
-      <c r="M233" s="51"/>
-    </row>
-    <row r="234" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C234" s="46"/>
-      <c r="D234" s="46"/>
-      <c r="E234" s="46"/>
-      <c r="F234" s="51"/>
-      <c r="G234" s="51"/>
-      <c r="H234" s="51"/>
-      <c r="I234" s="51"/>
-      <c r="J234" s="51"/>
-      <c r="K234" s="51"/>
-      <c r="L234" s="51"/>
-      <c r="M234" s="51"/>
-    </row>
-    <row r="235" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C235" s="46"/>
-      <c r="D235" s="46"/>
-      <c r="E235" s="46"/>
-      <c r="F235" s="51"/>
-      <c r="G235" s="51"/>
-      <c r="H235" s="51"/>
-      <c r="I235" s="51"/>
-      <c r="J235" s="51"/>
-      <c r="K235" s="51"/>
-      <c r="L235" s="51"/>
-      <c r="M235" s="51"/>
-    </row>
-    <row r="236" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C236" s="46"/>
-      <c r="D236" s="46"/>
-      <c r="E236" s="46"/>
-      <c r="F236" s="51"/>
-      <c r="G236" s="51"/>
-      <c r="H236" s="51"/>
-      <c r="I236" s="51"/>
-      <c r="J236" s="51"/>
-      <c r="K236" s="51"/>
-      <c r="L236" s="51"/>
-      <c r="M236" s="51"/>
-    </row>
-    <row r="237" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C237" s="46"/>
-      <c r="D237" s="46"/>
-      <c r="E237" s="46"/>
-      <c r="F237" s="51"/>
-      <c r="G237" s="51"/>
-      <c r="H237" s="51"/>
-      <c r="I237" s="51"/>
-      <c r="J237" s="51"/>
-      <c r="K237" s="51"/>
-      <c r="L237" s="51"/>
-      <c r="M237" s="51"/>
-    </row>
-    <row r="238" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C238" s="46"/>
-      <c r="D238" s="46"/>
-      <c r="E238" s="46"/>
-      <c r="F238" s="51"/>
-      <c r="G238" s="51"/>
-      <c r="H238" s="51"/>
-      <c r="I238" s="51"/>
-      <c r="J238" s="51"/>
-      <c r="K238" s="51"/>
-      <c r="L238" s="51"/>
-      <c r="M238" s="51"/>
-    </row>
-    <row r="239" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C239" s="46"/>
-      <c r="D239" s="46"/>
-      <c r="E239" s="46"/>
-      <c r="F239" s="51"/>
-      <c r="G239" s="51"/>
-      <c r="H239" s="51"/>
-      <c r="I239" s="51"/>
-      <c r="J239" s="51"/>
-      <c r="K239" s="51"/>
-      <c r="L239" s="51"/>
-      <c r="M239" s="51"/>
-    </row>
-    <row r="240" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C240" s="46"/>
-      <c r="D240" s="46"/>
-      <c r="E240" s="46"/>
-      <c r="F240" s="51"/>
-      <c r="G240" s="51"/>
-      <c r="H240" s="51"/>
-      <c r="I240" s="51"/>
-      <c r="J240" s="51"/>
-      <c r="K240" s="51"/>
-      <c r="L240" s="51"/>
-      <c r="M240" s="51"/>
-    </row>
-    <row r="241" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C241" s="46"/>
-      <c r="D241" s="46"/>
-      <c r="E241" s="46"/>
-      <c r="F241" s="51"/>
-      <c r="G241" s="51"/>
-      <c r="H241" s="51"/>
-      <c r="I241" s="51"/>
-      <c r="J241" s="51"/>
-      <c r="K241" s="51"/>
-      <c r="L241" s="51"/>
-      <c r="M241" s="51"/>
-    </row>
-    <row r="242" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C242" s="46"/>
-      <c r="D242" s="46"/>
-      <c r="E242" s="46"/>
-      <c r="F242" s="51"/>
-      <c r="G242" s="51"/>
-      <c r="H242" s="51"/>
-      <c r="I242" s="51"/>
-      <c r="J242" s="51"/>
-      <c r="K242" s="51"/>
-      <c r="L242" s="51"/>
-      <c r="M242" s="51"/>
-    </row>
-    <row r="243" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C243" s="46"/>
-      <c r="D243" s="46"/>
-      <c r="E243" s="46"/>
-      <c r="F243" s="51"/>
-      <c r="G243" s="51"/>
-      <c r="H243" s="51"/>
-      <c r="I243" s="51"/>
-      <c r="J243" s="51"/>
-      <c r="K243" s="51"/>
-      <c r="L243" s="51"/>
-      <c r="M243" s="51"/>
-    </row>
-    <row r="244" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C244" s="46"/>
-      <c r="D244" s="46"/>
-      <c r="E244" s="46"/>
-      <c r="F244" s="51"/>
-      <c r="G244" s="51"/>
-      <c r="H244" s="51"/>
-      <c r="I244" s="51"/>
-      <c r="J244" s="51"/>
-      <c r="K244" s="51"/>
-      <c r="L244" s="51"/>
-      <c r="M244" s="51"/>
-    </row>
-    <row r="245" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C245" s="46"/>
-      <c r="D245" s="46"/>
-      <c r="E245" s="46"/>
-      <c r="F245" s="51"/>
-      <c r="G245" s="51"/>
-      <c r="H245" s="51"/>
-      <c r="I245" s="51"/>
-      <c r="J245" s="51"/>
-      <c r="K245" s="51"/>
-      <c r="L245" s="51"/>
-      <c r="M245" s="51"/>
-    </row>
-    <row r="246" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C246" s="46"/>
-      <c r="D246" s="46"/>
-      <c r="E246" s="46"/>
-      <c r="F246" s="51"/>
-      <c r="G246" s="51"/>
-      <c r="H246" s="51"/>
-      <c r="I246" s="51"/>
-      <c r="J246" s="51"/>
-      <c r="K246" s="51"/>
-      <c r="L246" s="51"/>
-      <c r="M246" s="51"/>
-    </row>
-    <row r="247" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C247" s="46"/>
-      <c r="D247" s="46"/>
-      <c r="E247" s="46"/>
-      <c r="F247" s="51"/>
-      <c r="G247" s="51"/>
-      <c r="H247" s="51"/>
-      <c r="I247" s="51"/>
-      <c r="J247" s="51"/>
-      <c r="K247" s="51"/>
-      <c r="L247" s="51"/>
-      <c r="M247" s="51"/>
-    </row>
-    <row r="248" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C248" s="46"/>
-      <c r="D248" s="46"/>
-      <c r="E248" s="46"/>
-      <c r="F248" s="51"/>
-      <c r="G248" s="51"/>
-      <c r="H248" s="51"/>
-      <c r="I248" s="51"/>
-      <c r="J248" s="51"/>
-      <c r="K248" s="51"/>
-      <c r="L248" s="51"/>
-      <c r="M248" s="51"/>
-    </row>
-    <row r="249" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C249" s="46"/>
-      <c r="D249" s="46"/>
-      <c r="E249" s="46"/>
-      <c r="F249" s="51"/>
-      <c r="G249" s="51"/>
-      <c r="H249" s="51"/>
-      <c r="I249" s="51"/>
-      <c r="J249" s="51"/>
-      <c r="K249" s="51"/>
-      <c r="L249" s="51"/>
-      <c r="M249" s="51"/>
-    </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="F68:H72"/>
-    <mergeCell ref="L5:N9"/>
-    <mergeCell ref="I61:K65"/>
-    <mergeCell ref="L61:N65"/>
-    <mergeCell ref="L68:N72"/>
-    <mergeCell ref="I68:K72"/>
+  <mergeCells count="29">
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="B19:N19"/>
+    <mergeCell ref="B12:N12"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="L7:N11"/>
+    <mergeCell ref="I7:K11"/>
+    <mergeCell ref="F7:H11"/>
+    <mergeCell ref="L14:N18"/>
+    <mergeCell ref="I14:K18"/>
+    <mergeCell ref="F14:H18"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="L21:N25"/>
+    <mergeCell ref="I21:K25"/>
+    <mergeCell ref="F21:H25"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
@@ -8690,40 +7977,14 @@
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B66:N66"/>
-    <mergeCell ref="B59:N59"/>
-    <mergeCell ref="B52:N52"/>
-    <mergeCell ref="B45:N45"/>
-    <mergeCell ref="B38:N38"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="L33:N37"/>
-    <mergeCell ref="I33:K37"/>
-    <mergeCell ref="F33:H37"/>
-    <mergeCell ref="L40:N44"/>
-    <mergeCell ref="I40:K44"/>
-    <mergeCell ref="F40:H44"/>
-    <mergeCell ref="F61:H65"/>
-    <mergeCell ref="I5:K9"/>
-    <mergeCell ref="F5:H9"/>
-    <mergeCell ref="L12:N16"/>
-    <mergeCell ref="I12:K16"/>
-    <mergeCell ref="F12:H16"/>
-    <mergeCell ref="L19:N23"/>
-    <mergeCell ref="I19:K23"/>
-    <mergeCell ref="F19:H23"/>
-    <mergeCell ref="L26:N30"/>
-    <mergeCell ref="I26:K30"/>
-    <mergeCell ref="F26:H30"/>
-    <mergeCell ref="B17:N17"/>
-    <mergeCell ref="B31:N31"/>
-    <mergeCell ref="B24:N24"/>
-    <mergeCell ref="B10:N10"/>
-    <mergeCell ref="L47:N51"/>
-    <mergeCell ref="I47:K51"/>
-    <mergeCell ref="F47:H51"/>
-    <mergeCell ref="L54:N58"/>
-    <mergeCell ref="F54:H58"/>
-    <mergeCell ref="I54:K58"/>
+    <mergeCell ref="F32:H36"/>
+    <mergeCell ref="L32:N36"/>
+    <mergeCell ref="I32:K36"/>
+    <mergeCell ref="B30:N30"/>
+    <mergeCell ref="B29:N29"/>
+    <mergeCell ref="B28:N28"/>
+    <mergeCell ref="B27:N27"/>
+    <mergeCell ref="B26:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8744,16 +8005,16 @@
   <sheetData>
     <row r="3" spans="2:11" ht="34" x14ac:dyDescent="0.2">
       <c r="C3" s="42" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E3" s="43" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F3" s="43" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G3" s="41"/>
       <c r="H3" s="39"/>
@@ -8766,7 +8027,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="40" t="e">
-        <f>'Ordering of retrievals'!C75</f>
+        <f>'Ordering of retrievals'!C39</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D4" s="40"/>
@@ -8781,7 +8042,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="40" t="e">
-        <f>'Ordering of retrievals'!D75</f>
+        <f>'Ordering of retrievals'!D39</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D5" s="40"/>
@@ -8796,7 +8057,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="40" t="e">
-        <f>'Ordering of retrievals'!E75</f>
+        <f>'Ordering of retrievals'!E39</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D6" s="40"/>

</xml_diff>

<commit_message>
[Sandra] finish qualitative eval
</commit_message>
<xml_diff>
--- a/project/evaluation/qualitative_evaluation/qualitative_evaluation_table.xlsx
+++ b/project/evaluation/qualitative_evaluation/qualitative_evaluation_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteom/shared-folder/nlpt_group/project/evaluation/qualitative_evaluation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandrafriebolin/Desktop/WS23-24/transformers/nlpt_group/project/evaluation/qualitative_evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C27056F-2193-9542-AC01-25F6A00113DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B7F810-BD87-8243-96BA-226E12151B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-5940" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{BFF5F178-14AB-6B4F-B81C-3E61E0B93405}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{BFF5F178-14AB-6B4F-B81C-3E61E0B93405}"/>
   </bookViews>
   <sheets>
     <sheet name="Correct retrieval" sheetId="1" r:id="rId1"/>
@@ -305,16 +305,19 @@
     <t>BAAI:  no specifik linking of early parenting behaviours and later school outcomes      Jamesgpt:  focus is on socioeconomic factors and early life assessments without explicitly connecting them to parenting behaviors        thenlper: primarily focuses on impact of parental education levels rather than early parenting behavior</t>
   </si>
   <si>
-    <t>BAAI, Jamesgpt: focus is on how premorbid IQ moderates the relationship between clinical severity and executive functioning.          Thenlper:  focuses on the relationship between intelligence and risk of developing bipolar disorder, which diverges from query's interest in occupational outcomes</t>
-  </si>
-  <si>
-    <t>Note: Glucocordicoidis are a class of hormons, to which hydricortisone belongs and even is the most important. Dexamethasone is also a glucocoicoidis.        BAAI: patients from 7 to 16 yo, not preschool.       Jamesgpt: Got both infants and hydrocortisone</t>
-  </si>
-  <si>
     <t>BAAI, Jamesgpt:  impact of maternal depression from pregnancy onwards, explores its association with children's cognitive development. [Matteo] Maternal depression not children's depression.     Thenlper: systematic review of effects of perinatal depression on IQ of children</t>
   </si>
   <si>
     <t>Jamesgpt: Special regard to 10 years old</t>
+  </si>
+  <si>
+    <t>Note: Glucocordicoidis are a class of hormons, to which hydricortisone belongs and even is the most important. Dexamethasone is also a glucocoicoidis.        
+BAAI/thenpler: patients from 7 to 16 yo, not preschool; related to the query but does not focus on randomized trials
+Jamesgpt: Got both infants and hydrocortisone; presents a meta-analysis of trials</t>
+  </si>
+  <si>
+    <t>BAAI, Jamesgpt: focus is on how premorbid IQ moderates the relationship between clinical severity and executive functioning; [Sandra: focus is on how premorbid IQ moderates the relationship between clinical severity and executive functioning]
+ Thenlper:  focuses on the relationship between intelligence and risk of developing bipolar disorder, which diverges from query's interest in occupational outcomes; [Sandra: focuses on the relationship between intelligence and risk of developing bipolar disorder, which diverges from query's interest in occupational outcomes]</t>
   </si>
 </sst>
 </file>
@@ -851,6 +854,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -860,6 +866,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -887,6 +914,27 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -899,46 +947,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -968,58 +1034,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1034,23 +1049,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1079,9 +1082,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1119,7 +1122,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1225,7 +1228,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1367,7 +1370,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1551,30 +1554,30 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="72"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
     </row>
     <row r="26" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="70" t="s">
+      <c r="C26" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="70"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
     </row>
     <row r="27" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C27" s="15" t="s">
@@ -1603,7 +1606,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="71" t="s">
+      <c r="A28" s="72" t="s">
         <v>14</v>
       </c>
       <c r="B28" s="5">
@@ -1619,7 +1622,7 @@
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="71"/>
+      <c r="A29" s="72"/>
       <c r="B29" s="9">
         <v>2</v>
       </c>
@@ -1633,7 +1636,7 @@
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="71"/>
+      <c r="A30" s="72"/>
       <c r="B30" s="9">
         <v>3</v>
       </c>
@@ -1647,7 +1650,7 @@
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="71"/>
+      <c r="A31" s="72"/>
       <c r="B31" s="9">
         <v>4</v>
       </c>
@@ -1661,7 +1664,7 @@
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="71"/>
+      <c r="A32" s="72"/>
       <c r="B32" s="9">
         <v>5</v>
       </c>
@@ -1675,7 +1678,7 @@
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="71"/>
+      <c r="A33" s="72"/>
       <c r="B33" s="9">
         <v>6</v>
       </c>
@@ -1689,7 +1692,7 @@
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="71"/>
+      <c r="A34" s="72"/>
       <c r="B34" s="9">
         <v>7</v>
       </c>
@@ -1703,7 +1706,7 @@
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="71"/>
+      <c r="A35" s="72"/>
       <c r="B35" s="9">
         <v>8</v>
       </c>
@@ -1717,7 +1720,7 @@
       <c r="J35" s="4"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="71"/>
+      <c r="A36" s="72"/>
       <c r="B36" s="9">
         <v>9</v>
       </c>
@@ -1731,7 +1734,7 @@
       <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="71"/>
+      <c r="A37" s="72"/>
       <c r="B37" s="10">
         <v>10</v>
       </c>
@@ -1765,9 +1768,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5956BC-300C-CB42-87CA-185E2E097C22}">
   <dimension ref="A1:O205"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1789,35 +1792,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="96" t="s">
+      <c r="D1" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="99" t="s">
+      <c r="F1" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="94" t="s">
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="98" t="s">
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C2" s="95"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="97"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79"/>
       <c r="F2" s="25" t="s">
         <v>44</v>
       </c>
@@ -1850,21 +1853,21 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="87"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="76"/>
     </row>
     <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
@@ -1906,78 +1909,78 @@
       <c r="E5" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="79"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="75"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="83"/>
       <c r="O5" s="45" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
-      <c r="L6" s="86"/>
-      <c r="M6" s="86"/>
-      <c r="N6" s="87"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
+      <c r="N6" s="76"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
-      <c r="L7" s="86"/>
-      <c r="M7" s="86"/>
-      <c r="N7" s="87"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="76"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="86" t="s">
+      <c r="B8" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="86"/>
-      <c r="L8" s="86"/>
-      <c r="M8" s="86"/>
-      <c r="N8" s="87"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="76"/>
     </row>
     <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" s="32" t="s">
@@ -2018,15 +2021,15 @@
       <c r="E10" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="79"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="77"/>
-      <c r="K10" s="78"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="75"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="84"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="83"/>
       <c r="O10" s="44" t="s">
         <v>87</v>
       </c>
@@ -2035,21 +2038,21 @@
       <c r="A11" s="1">
         <v>5</v>
       </c>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="N11" s="87"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="75"/>
+      <c r="M11" s="75"/>
+      <c r="N11" s="76"/>
     </row>
     <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="s">
@@ -2090,15 +2093,15 @@
       <c r="E13" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="79"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="77"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="73"/>
-      <c r="M13" s="74"/>
-      <c r="N13" s="75"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="83"/>
       <c r="O13" s="44" t="s">
         <v>86</v>
       </c>
@@ -2107,21 +2110,21 @@
       <c r="A14" s="1">
         <v>6</v>
       </c>
-      <c r="B14" s="86" t="s">
+      <c r="B14" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="L14" s="86"/>
-      <c r="M14" s="86"/>
-      <c r="N14" s="87"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="75"/>
+      <c r="M14" s="75"/>
+      <c r="N14" s="76"/>
     </row>
     <row r="15" spans="1:15" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="52" t="s">
@@ -2133,17 +2136,23 @@
       <c r="F15" s="48">
         <v>2</v>
       </c>
-      <c r="G15" s="48"/>
+      <c r="G15" s="48">
+        <v>2</v>
+      </c>
       <c r="H15" s="48"/>
       <c r="I15" s="49">
         <v>3</v>
       </c>
-      <c r="J15" s="49"/>
+      <c r="J15" s="49">
+        <v>3</v>
+      </c>
       <c r="K15" s="49"/>
       <c r="L15" s="50">
         <v>2</v>
       </c>
-      <c r="M15" s="50"/>
+      <c r="M15" s="50">
+        <v>2</v>
+      </c>
       <c r="N15" s="50"/>
       <c r="O15" s="46" t="str">
         <f>IF(OR( AND(C16=D16,OR(F15&lt;&gt;G15, I15&lt;&gt;J15,L15&lt;&gt;M15)),  AND(D16=E16,OR(G15&lt;&gt;H15,J15&lt;&gt;K15,M15&lt;&gt;N15)), AND(C16=E16, OR(F15&lt;&gt;H15,I15&lt;&gt;K15,L15&lt;&gt;N15) )), "error: different mark to same abstract","")</f>
@@ -2161,38 +2170,38 @@
       <c r="E16" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="82"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="93"/>
-      <c r="L16" s="88"/>
-      <c r="M16" s="89"/>
-      <c r="N16" s="90"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="99"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="95"/>
+      <c r="K16" s="96"/>
+      <c r="L16" s="91"/>
+      <c r="M16" s="92"/>
+      <c r="N16" s="93"/>
       <c r="O16" s="52" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>7</v>
       </c>
-      <c r="B17" s="86" t="s">
+      <c r="B17" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="86"/>
-      <c r="K17" s="86"/>
-      <c r="L17" s="86"/>
-      <c r="M17" s="86"/>
-      <c r="N17" s="87"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="75"/>
+      <c r="L17" s="75"/>
+      <c r="M17" s="75"/>
+      <c r="N17" s="76"/>
     </row>
     <row r="18" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="32" t="s">
@@ -2233,15 +2242,15 @@
       <c r="E19" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="79"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="76"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="74"/>
-      <c r="N19" s="75"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="88"/>
+      <c r="H19" s="89"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="83"/>
       <c r="O19" s="44" t="s">
         <v>85</v>
       </c>
@@ -2250,21 +2259,21 @@
       <c r="A20" s="1">
         <v>8</v>
       </c>
-      <c r="B20" s="86" t="s">
+      <c r="B20" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
-      <c r="H20" s="86"/>
-      <c r="I20" s="86"/>
-      <c r="J20" s="86"/>
-      <c r="K20" s="86"/>
-      <c r="L20" s="86"/>
-      <c r="M20" s="86"/>
-      <c r="N20" s="87"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="75"/>
+      <c r="N20" s="76"/>
     </row>
     <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="32" t="s">
@@ -2305,38 +2314,38 @@
       <c r="E22" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="79"/>
-      <c r="G22" s="80"/>
-      <c r="H22" s="81"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="78"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="75"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="88"/>
+      <c r="H22" s="89"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="86"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="83"/>
       <c r="O22" s="44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>9</v>
       </c>
-      <c r="B23" s="86" t="s">
+      <c r="B23" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="86"/>
-      <c r="J23" s="86"/>
-      <c r="K23" s="86"/>
-      <c r="L23" s="86"/>
-      <c r="M23" s="86"/>
-      <c r="N23" s="87"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
+      <c r="M23" s="75"/>
+      <c r="N23" s="76"/>
     </row>
     <row r="24" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="32" t="s">
@@ -2347,17 +2356,23 @@
       <c r="F24" s="25">
         <v>1</v>
       </c>
-      <c r="G24" s="25"/>
+      <c r="G24" s="25">
+        <v>1</v>
+      </c>
       <c r="H24" s="25"/>
       <c r="I24" s="26">
         <v>1</v>
       </c>
-      <c r="J24" s="26"/>
+      <c r="J24" s="26">
+        <v>1</v>
+      </c>
       <c r="K24" s="26"/>
       <c r="L24" s="27">
         <v>1</v>
       </c>
-      <c r="M24" s="27"/>
+      <c r="M24" s="27">
+        <v>1</v>
+      </c>
       <c r="N24" s="27"/>
     </row>
     <row r="25" spans="1:15" ht="306" x14ac:dyDescent="0.2">
@@ -2371,15 +2386,15 @@
       <c r="E25" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="F25" s="79"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="78"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="74"/>
-      <c r="N25" s="75"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="88"/>
+      <c r="H25" s="89"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="86"/>
+      <c r="L25" s="81"/>
+      <c r="M25" s="82"/>
+      <c r="N25" s="83"/>
     </row>
     <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="32" t="s">
@@ -2390,17 +2405,23 @@
       <c r="F26" s="25">
         <v>1</v>
       </c>
-      <c r="G26" s="25"/>
+      <c r="G26" s="25">
+        <v>1</v>
+      </c>
       <c r="H26" s="25"/>
       <c r="I26" s="26">
         <v>1</v>
       </c>
-      <c r="J26" s="26"/>
+      <c r="J26" s="26">
+        <v>1</v>
+      </c>
       <c r="K26" s="26"/>
       <c r="L26" s="27">
         <v>1</v>
       </c>
-      <c r="M26" s="27"/>
+      <c r="M26" s="27">
+        <v>1</v>
+      </c>
       <c r="N26" s="27"/>
     </row>
     <row r="27" spans="1:15" ht="388" x14ac:dyDescent="0.2">
@@ -2414,35 +2435,35 @@
       <c r="E27" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="79"/>
-      <c r="G27" s="80"/>
-      <c r="H27" s="81"/>
-      <c r="I27" s="76"/>
-      <c r="J27" s="77"/>
-      <c r="K27" s="78"/>
-      <c r="L27" s="73"/>
-      <c r="M27" s="74"/>
-      <c r="N27" s="75"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="88"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="84"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="86"/>
+      <c r="L27" s="81"/>
+      <c r="M27" s="82"/>
+      <c r="N27" s="83"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>10</v>
       </c>
-      <c r="B28" s="86" t="s">
+      <c r="B28" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
-      <c r="H28" s="86"/>
-      <c r="I28" s="86"/>
-      <c r="J28" s="86"/>
-      <c r="K28" s="86"/>
-      <c r="L28" s="86"/>
-      <c r="M28" s="86"/>
-      <c r="N28" s="87"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
+      <c r="J28" s="75"/>
+      <c r="K28" s="75"/>
+      <c r="L28" s="75"/>
+      <c r="M28" s="75"/>
+      <c r="N28" s="76"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C29"/>
@@ -2459,11 +2480,11 @@
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C30" s="85" t="s">
+      <c r="C30" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="85"/>
-      <c r="E30" s="85"/>
+      <c r="D30" s="100"/>
+      <c r="E30" s="100"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -4781,17 +4802,20 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B6:N6"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="F19:H19"/>
     <mergeCell ref="B7:N7"/>
     <mergeCell ref="B28:N28"/>
     <mergeCell ref="B23:N23"/>
@@ -4808,20 +4832,17 @@
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="L16:N16"/>
     <mergeCell ref="I16:K16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B6:N6"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4831,9 +4852,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03816060-24A7-D946-9AB1-F7E07293AE02}">
   <dimension ref="A1:O213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4856,35 +4877,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C1" s="127" t="s">
+      <c r="C1" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="128" t="s">
+      <c r="D1" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="129" t="s">
+      <c r="E1" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="133" t="s">
+      <c r="F1" s="135" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="134" t="s">
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="136" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
-      <c r="L1" s="130" t="s">
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="134" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C2" s="127"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="129"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="133"/>
       <c r="F2" s="48" t="s">
         <v>44</v>
       </c>
@@ -4917,61 +4938,61 @@
       <c r="A3" s="51">
         <v>1</v>
       </c>
-      <c r="B3" s="131" t="s">
+      <c r="B3" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="131"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="131"/>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131"/>
-      <c r="H3" s="131"/>
-      <c r="I3" s="131"/>
-      <c r="J3" s="131"/>
-      <c r="K3" s="131"/>
-      <c r="L3" s="131"/>
-      <c r="M3" s="131"/>
-      <c r="N3" s="132"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="102"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="51">
         <v>2</v>
       </c>
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="131"/>
-      <c r="D4" s="131"/>
-      <c r="E4" s="131"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="131"/>
-      <c r="H4" s="131"/>
-      <c r="I4" s="131"/>
-      <c r="J4" s="131"/>
-      <c r="K4" s="131"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="131"/>
-      <c r="N4" s="132"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+      <c r="N4" s="102"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="51">
         <v>3</v>
       </c>
-      <c r="B5" s="131" t="s">
+      <c r="B5" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
-      <c r="H5" s="131"/>
-      <c r="I5" s="131"/>
-      <c r="J5" s="131"/>
-      <c r="K5" s="131"/>
-      <c r="L5" s="131"/>
-      <c r="M5" s="131"/>
-      <c r="N5" s="132"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="102"/>
     </row>
     <row r="6" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="52" t="s">
@@ -4983,7 +5004,9 @@
       <c r="F6" s="57">
         <v>1</v>
       </c>
-      <c r="G6" s="58"/>
+      <c r="G6" s="58">
+        <v>1</v>
+      </c>
       <c r="H6" s="58"/>
       <c r="I6" s="59"/>
       <c r="J6" s="59"/>
@@ -4991,7 +5014,9 @@
       <c r="L6" s="60">
         <v>1</v>
       </c>
-      <c r="M6" s="60"/>
+      <c r="M6" s="60">
+        <v>1</v>
+      </c>
       <c r="N6" s="60"/>
       <c r="O6" s="46" t="e">
         <f>IF(OR( AND(C7=#REF!,OR(F6&lt;&gt;G6, I6&lt;&gt;J6,L6&lt;&gt;M6)),  AND(#REF!=E7,OR(G6&lt;&gt;H6,J6&lt;&gt;K6,M6&lt;&gt;N6)), AND(C7=E7, OR(F6&lt;&gt;H6,I6&lt;&gt;K6,L6&lt;&gt;N6) )), "error: different mark to same abstract","")</f>
@@ -5009,15 +5034,15 @@
       <c r="E7" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="100"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="102"/>
-      <c r="I7" s="118"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="120"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="110"/>
-      <c r="N7" s="111"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="123"/>
+      <c r="I7" s="112"/>
+      <c r="J7" s="113"/>
+      <c r="K7" s="114"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="104"/>
+      <c r="N7" s="105"/>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="52" t="s">
@@ -5026,15 +5051,15 @@
       <c r="C8" s="53"/>
       <c r="D8" s="54"/>
       <c r="E8" s="56"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="104"/>
-      <c r="H8" s="105"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="122"/>
-      <c r="K8" s="123"/>
-      <c r="L8" s="112"/>
-      <c r="M8" s="113"/>
-      <c r="N8" s="114"/>
+      <c r="F8" s="124"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="115"/>
+      <c r="J8" s="116"/>
+      <c r="K8" s="117"/>
+      <c r="L8" s="106"/>
+      <c r="M8" s="107"/>
+      <c r="N8" s="108"/>
       <c r="O8" s="46" t="str">
         <f>IF(OR( AND(C9=D7,OR(F8&lt;&gt;G8, I8&lt;&gt;J8,L8&lt;&gt;M8)),  AND(D7=E9,OR(G8&lt;&gt;H8,J8&lt;&gt;K8,M8&lt;&gt;N8)), AND(C9=E9, OR(F8&lt;&gt;H8,I8&lt;&gt;K8,L8&lt;&gt;N8) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5051,15 +5076,15 @@
       <c r="E9" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="103"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="105"/>
-      <c r="I9" s="121"/>
-      <c r="J9" s="122"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="113"/>
-      <c r="N9" s="114"/>
+      <c r="F9" s="124"/>
+      <c r="G9" s="125"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="117"/>
+      <c r="L9" s="106"/>
+      <c r="M9" s="107"/>
+      <c r="N9" s="108"/>
     </row>
     <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="52" t="s">
@@ -5068,15 +5093,15 @@
       <c r="C10" s="53"/>
       <c r="D10" s="54"/>
       <c r="E10" s="61"/>
-      <c r="F10" s="103"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="121"/>
-      <c r="J10" s="122"/>
-      <c r="K10" s="123"/>
-      <c r="L10" s="112"/>
-      <c r="M10" s="113"/>
-      <c r="N10" s="114"/>
+      <c r="F10" s="124"/>
+      <c r="G10" s="125"/>
+      <c r="H10" s="126"/>
+      <c r="I10" s="115"/>
+      <c r="J10" s="116"/>
+      <c r="K10" s="117"/>
+      <c r="L10" s="106"/>
+      <c r="M10" s="107"/>
+      <c r="N10" s="108"/>
       <c r="O10" s="46" t="str">
         <f>IF(OR( AND(C11=D9,OR(F10&lt;&gt;G10, I10&lt;&gt;J10,L10&lt;&gt;M10)),  AND(D9=E11,OR(G10&lt;&gt;H10,J10&lt;&gt;K10,M10&lt;&gt;N10)), AND(C11=E11, OR(F10&lt;&gt;H10,I10&lt;&gt;K10,L10&lt;&gt;N10) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5093,35 +5118,35 @@
       <c r="E11" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="106"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="108"/>
-      <c r="I11" s="124"/>
-      <c r="J11" s="125"/>
-      <c r="K11" s="126"/>
-      <c r="L11" s="115"/>
-      <c r="M11" s="116"/>
-      <c r="N11" s="117"/>
+      <c r="F11" s="127"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="129"/>
+      <c r="I11" s="118"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="120"/>
+      <c r="L11" s="109"/>
+      <c r="M11" s="110"/>
+      <c r="N11" s="111"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="51">
         <v>4</v>
       </c>
-      <c r="B12" s="131" t="s">
+      <c r="B12" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="131"/>
-      <c r="D12" s="131"/>
-      <c r="E12" s="131"/>
-      <c r="F12" s="131"/>
-      <c r="G12" s="131"/>
-      <c r="H12" s="131"/>
-      <c r="I12" s="131"/>
-      <c r="J12" s="131"/>
-      <c r="K12" s="131"/>
-      <c r="L12" s="131"/>
-      <c r="M12" s="131"/>
-      <c r="N12" s="132"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="101"/>
+      <c r="E12" s="101"/>
+      <c r="F12" s="101"/>
+      <c r="G12" s="101"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="101"/>
+      <c r="J12" s="101"/>
+      <c r="K12" s="101"/>
+      <c r="L12" s="101"/>
+      <c r="M12" s="101"/>
+      <c r="N12" s="102"/>
     </row>
     <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="52" t="s">
@@ -5139,33 +5164,35 @@
       <c r="L13" s="60">
         <v>1</v>
       </c>
-      <c r="M13" s="60"/>
+      <c r="M13" s="60">
+        <v>1</v>
+      </c>
       <c r="N13" s="60"/>
       <c r="O13" s="46" t="str">
         <f>IF(OR( AND(C14=D16,OR(F13&lt;&gt;G13, I13&lt;&gt;J13,L13&lt;&gt;M13)),  AND(D16=E16,OR(G13&lt;&gt;H13,J13&lt;&gt;K13,M13&lt;&gt;N13)), AND(C14=E16, OR(F13&lt;&gt;H13,I13&lt;&gt;K13,L13&lt;&gt;N13) )), "error: different mark to same abstract","")</f>
         <v>error: different mark to same abstract</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="272" x14ac:dyDescent="0.2">
       <c r="B14" s="52"/>
       <c r="C14" s="63" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="100"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="118"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="120"/>
-      <c r="L14" s="109"/>
-      <c r="M14" s="110"/>
-      <c r="N14" s="111"/>
+        <v>52</v>
+      </c>
+      <c r="F14" s="121"/>
+      <c r="G14" s="122"/>
+      <c r="H14" s="123"/>
+      <c r="I14" s="112"/>
+      <c r="J14" s="113"/>
+      <c r="K14" s="114"/>
+      <c r="L14" s="103"/>
+      <c r="M14" s="104"/>
+      <c r="N14" s="105"/>
     </row>
     <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="52" t="s">
@@ -5173,15 +5200,15 @@
       </c>
       <c r="D15" s="54"/>
       <c r="E15" s="55"/>
-      <c r="F15" s="103"/>
-      <c r="G15" s="104"/>
-      <c r="H15" s="105"/>
-      <c r="I15" s="121"/>
-      <c r="J15" s="122"/>
-      <c r="K15" s="123"/>
-      <c r="L15" s="112"/>
-      <c r="M15" s="113"/>
-      <c r="N15" s="114"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="125"/>
+      <c r="H15" s="126"/>
+      <c r="I15" s="115"/>
+      <c r="J15" s="116"/>
+      <c r="K15" s="117"/>
+      <c r="L15" s="106"/>
+      <c r="M15" s="107"/>
+      <c r="N15" s="108"/>
       <c r="O15" s="46" t="str">
         <f>IF(OR( AND(C16=D14,OR(F15&lt;&gt;G15, I15&lt;&gt;J15,L15&lt;&gt;M15)),  AND(D14=E14,OR(G15&lt;&gt;H15,J15&lt;&gt;K15,M15&lt;&gt;N15)), AND(C16=E14, OR(F15&lt;&gt;H15,I15&lt;&gt;K15,L15&lt;&gt;N15) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5193,20 +5220,20 @@
         <v>53</v>
       </c>
       <c r="D16" s="54" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="103"/>
-      <c r="G16" s="104"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="121"/>
-      <c r="J16" s="122"/>
-      <c r="K16" s="123"/>
-      <c r="L16" s="112"/>
-      <c r="M16" s="113"/>
-      <c r="N16" s="114"/>
+        <v>53</v>
+      </c>
+      <c r="F16" s="124"/>
+      <c r="G16" s="125"/>
+      <c r="H16" s="126"/>
+      <c r="I16" s="115"/>
+      <c r="J16" s="116"/>
+      <c r="K16" s="117"/>
+      <c r="L16" s="106"/>
+      <c r="M16" s="107"/>
+      <c r="N16" s="108"/>
     </row>
     <row r="17" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="52" t="s">
@@ -5214,15 +5241,15 @@
       </c>
       <c r="D17" s="54"/>
       <c r="E17" s="55"/>
-      <c r="F17" s="103"/>
-      <c r="G17" s="104"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="122"/>
-      <c r="K17" s="123"/>
-      <c r="L17" s="112"/>
-      <c r="M17" s="113"/>
-      <c r="N17" s="114"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="125"/>
+      <c r="H17" s="126"/>
+      <c r="I17" s="115"/>
+      <c r="J17" s="116"/>
+      <c r="K17" s="117"/>
+      <c r="L17" s="106"/>
+      <c r="M17" s="107"/>
+      <c r="N17" s="108"/>
       <c r="O17" s="46" t="str">
         <f>IF(OR( AND(C18=D18,OR(F17&lt;&gt;G17, I17&lt;&gt;J17,L17&lt;&gt;M17)),  AND(D18=E18,OR(G17&lt;&gt;H17,J17&lt;&gt;K17,M17&lt;&gt;N17)), AND(C18=E18, OR(F17&lt;&gt;H17,I17&lt;&gt;K17,L17&lt;&gt;N17) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5239,35 +5266,35 @@
       <c r="E18" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="106"/>
-      <c r="G18" s="107"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="124"/>
-      <c r="J18" s="125"/>
-      <c r="K18" s="126"/>
-      <c r="L18" s="115"/>
-      <c r="M18" s="116"/>
-      <c r="N18" s="117"/>
+      <c r="F18" s="127"/>
+      <c r="G18" s="128"/>
+      <c r="H18" s="129"/>
+      <c r="I18" s="118"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="120"/>
+      <c r="L18" s="109"/>
+      <c r="M18" s="110"/>
+      <c r="N18" s="111"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="51">
         <v>5</v>
       </c>
-      <c r="B19" s="131" t="s">
+      <c r="B19" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="131"/>
-      <c r="D19" s="131"/>
-      <c r="E19" s="131"/>
-      <c r="F19" s="131"/>
-      <c r="G19" s="131"/>
-      <c r="H19" s="131"/>
-      <c r="I19" s="131"/>
-      <c r="J19" s="131"/>
-      <c r="K19" s="131"/>
-      <c r="L19" s="131"/>
-      <c r="M19" s="131"/>
-      <c r="N19" s="132"/>
+      <c r="C19" s="101"/>
+      <c r="D19" s="101"/>
+      <c r="E19" s="101"/>
+      <c r="F19" s="101"/>
+      <c r="G19" s="101"/>
+      <c r="H19" s="101"/>
+      <c r="I19" s="101"/>
+      <c r="J19" s="101"/>
+      <c r="K19" s="101"/>
+      <c r="L19" s="101"/>
+      <c r="M19" s="101"/>
+      <c r="N19" s="102"/>
     </row>
     <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="52" t="s">
@@ -5276,7 +5303,9 @@
       <c r="D20" s="54"/>
       <c r="E20" s="55"/>
       <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
+      <c r="G20" s="58">
+        <v>1</v>
+      </c>
       <c r="H20" s="58"/>
       <c r="I20" s="59">
         <v>1</v>
@@ -5302,15 +5331,15 @@
       <c r="E21" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="100"/>
-      <c r="G21" s="101"/>
-      <c r="H21" s="102"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="119"/>
-      <c r="K21" s="120"/>
-      <c r="L21" s="109"/>
-      <c r="M21" s="110"/>
-      <c r="N21" s="111"/>
+      <c r="F21" s="121"/>
+      <c r="G21" s="122"/>
+      <c r="H21" s="123"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="114"/>
+      <c r="L21" s="103"/>
+      <c r="M21" s="104"/>
+      <c r="N21" s="105"/>
     </row>
     <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="52" t="s">
@@ -5318,15 +5347,15 @@
       </c>
       <c r="D22" s="54"/>
       <c r="E22" s="55"/>
-      <c r="F22" s="103"/>
-      <c r="G22" s="104"/>
-      <c r="H22" s="105"/>
-      <c r="I22" s="121"/>
-      <c r="J22" s="122"/>
-      <c r="K22" s="123"/>
-      <c r="L22" s="112"/>
-      <c r="M22" s="113"/>
-      <c r="N22" s="114"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="125"/>
+      <c r="H22" s="126"/>
+      <c r="I22" s="115"/>
+      <c r="J22" s="116"/>
+      <c r="K22" s="117"/>
+      <c r="L22" s="106"/>
+      <c r="M22" s="107"/>
+      <c r="N22" s="108"/>
       <c r="O22" s="46" t="str">
         <f>IF(OR( AND(C23=D23,OR(F22&lt;&gt;G22, I22&lt;&gt;J22,L22&lt;&gt;M22)),  AND(D23=E25,OR(G22&lt;&gt;H22,J22&lt;&gt;K22,M22&lt;&gt;N22)), AND(C23=E25, OR(F22&lt;&gt;H22,I22&lt;&gt;K22,L22&lt;&gt;N22) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5343,15 +5372,15 @@
       <c r="E23" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="103"/>
-      <c r="G23" s="104"/>
-      <c r="H23" s="105"/>
-      <c r="I23" s="121"/>
-      <c r="J23" s="122"/>
-      <c r="K23" s="123"/>
-      <c r="L23" s="112"/>
-      <c r="M23" s="113"/>
-      <c r="N23" s="114"/>
+      <c r="F23" s="124"/>
+      <c r="G23" s="125"/>
+      <c r="H23" s="126"/>
+      <c r="I23" s="115"/>
+      <c r="J23" s="116"/>
+      <c r="K23" s="117"/>
+      <c r="L23" s="106"/>
+      <c r="M23" s="107"/>
+      <c r="N23" s="108"/>
     </row>
     <row r="24" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="52" t="s">
@@ -5359,15 +5388,15 @@
       </c>
       <c r="D24" s="54"/>
       <c r="E24" s="55"/>
-      <c r="F24" s="103"/>
-      <c r="G24" s="104"/>
-      <c r="H24" s="105"/>
-      <c r="I24" s="121"/>
-      <c r="J24" s="122"/>
-      <c r="K24" s="123"/>
-      <c r="L24" s="112"/>
-      <c r="M24" s="113"/>
-      <c r="N24" s="114"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="125"/>
+      <c r="H24" s="126"/>
+      <c r="I24" s="115"/>
+      <c r="J24" s="116"/>
+      <c r="K24" s="117"/>
+      <c r="L24" s="106"/>
+      <c r="M24" s="107"/>
+      <c r="N24" s="108"/>
       <c r="O24" s="46" t="str">
         <f>IF(OR( AND(C25=D25,OR(F24&lt;&gt;G24, I24&lt;&gt;J24,L24&lt;&gt;M24)),  AND(D25=E23,OR(G24&lt;&gt;H24,J24&lt;&gt;K24,M24&lt;&gt;N24)), AND(C25=E23, OR(F24&lt;&gt;H24,I24&lt;&gt;K24,L24&lt;&gt;N24) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5384,115 +5413,115 @@
       <c r="E25" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="106"/>
-      <c r="G25" s="107"/>
-      <c r="H25" s="108"/>
-      <c r="I25" s="124"/>
-      <c r="J25" s="125"/>
-      <c r="K25" s="126"/>
-      <c r="L25" s="115"/>
-      <c r="M25" s="116"/>
-      <c r="N25" s="117"/>
+      <c r="F25" s="127"/>
+      <c r="G25" s="128"/>
+      <c r="H25" s="129"/>
+      <c r="I25" s="118"/>
+      <c r="J25" s="119"/>
+      <c r="K25" s="120"/>
+      <c r="L25" s="109"/>
+      <c r="M25" s="110"/>
+      <c r="N25" s="111"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="51">
         <v>6</v>
       </c>
-      <c r="B26" s="131" t="s">
+      <c r="B26" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="131"/>
-      <c r="D26" s="131"/>
-      <c r="E26" s="131"/>
-      <c r="F26" s="131"/>
-      <c r="G26" s="131"/>
-      <c r="H26" s="131"/>
-      <c r="I26" s="131"/>
-      <c r="J26" s="131"/>
-      <c r="K26" s="131"/>
-      <c r="L26" s="131"/>
-      <c r="M26" s="131"/>
-      <c r="N26" s="132"/>
+      <c r="C26" s="101"/>
+      <c r="D26" s="101"/>
+      <c r="E26" s="101"/>
+      <c r="F26" s="101"/>
+      <c r="G26" s="101"/>
+      <c r="H26" s="101"/>
+      <c r="I26" s="101"/>
+      <c r="J26" s="101"/>
+      <c r="K26" s="101"/>
+      <c r="L26" s="101"/>
+      <c r="M26" s="101"/>
+      <c r="N26" s="102"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="51">
         <v>7</v>
       </c>
-      <c r="B27" s="131" t="s">
+      <c r="B27" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="131"/>
-      <c r="D27" s="131"/>
-      <c r="E27" s="131"/>
-      <c r="F27" s="131"/>
-      <c r="G27" s="131"/>
-      <c r="H27" s="131"/>
-      <c r="I27" s="131"/>
-      <c r="J27" s="131"/>
-      <c r="K27" s="131"/>
-      <c r="L27" s="131"/>
-      <c r="M27" s="131"/>
-      <c r="N27" s="132"/>
+      <c r="C27" s="101"/>
+      <c r="D27" s="101"/>
+      <c r="E27" s="101"/>
+      <c r="F27" s="101"/>
+      <c r="G27" s="101"/>
+      <c r="H27" s="101"/>
+      <c r="I27" s="101"/>
+      <c r="J27" s="101"/>
+      <c r="K27" s="101"/>
+      <c r="L27" s="101"/>
+      <c r="M27" s="101"/>
+      <c r="N27" s="102"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="51">
         <v>8</v>
       </c>
-      <c r="B28" s="131" t="s">
+      <c r="B28" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="131"/>
-      <c r="D28" s="131"/>
-      <c r="E28" s="131"/>
-      <c r="F28" s="131"/>
-      <c r="G28" s="131"/>
-      <c r="H28" s="131"/>
-      <c r="I28" s="131"/>
-      <c r="J28" s="131"/>
-      <c r="K28" s="131"/>
-      <c r="L28" s="131"/>
-      <c r="M28" s="131"/>
-      <c r="N28" s="132"/>
+      <c r="C28" s="101"/>
+      <c r="D28" s="101"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="101"/>
+      <c r="G28" s="101"/>
+      <c r="H28" s="101"/>
+      <c r="I28" s="101"/>
+      <c r="J28" s="101"/>
+      <c r="K28" s="101"/>
+      <c r="L28" s="101"/>
+      <c r="M28" s="101"/>
+      <c r="N28" s="102"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="51">
         <v>9</v>
       </c>
-      <c r="B29" s="131" t="s">
+      <c r="B29" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="131"/>
-      <c r="D29" s="131"/>
-      <c r="E29" s="131"/>
-      <c r="F29" s="131"/>
-      <c r="G29" s="131"/>
-      <c r="H29" s="131"/>
-      <c r="I29" s="131"/>
-      <c r="J29" s="131"/>
-      <c r="K29" s="131"/>
-      <c r="L29" s="131"/>
-      <c r="M29" s="131"/>
-      <c r="N29" s="132"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="101"/>
+      <c r="G29" s="101"/>
+      <c r="H29" s="101"/>
+      <c r="I29" s="101"/>
+      <c r="J29" s="101"/>
+      <c r="K29" s="101"/>
+      <c r="L29" s="101"/>
+      <c r="M29" s="101"/>
+      <c r="N29" s="102"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="51">
         <v>10</v>
       </c>
-      <c r="B30" s="131" t="s">
+      <c r="B30" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="131"/>
-      <c r="D30" s="131"/>
-      <c r="E30" s="131"/>
-      <c r="F30" s="131"/>
-      <c r="G30" s="131"/>
-      <c r="H30" s="131"/>
-      <c r="I30" s="131"/>
-      <c r="J30" s="131"/>
-      <c r="K30" s="131"/>
-      <c r="L30" s="131"/>
-      <c r="M30" s="131"/>
-      <c r="N30" s="132"/>
+      <c r="C30" s="101"/>
+      <c r="D30" s="101"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="101"/>
+      <c r="G30" s="101"/>
+      <c r="H30" s="101"/>
+      <c r="I30" s="101"/>
+      <c r="J30" s="101"/>
+      <c r="K30" s="101"/>
+      <c r="L30" s="101"/>
+      <c r="M30" s="101"/>
+      <c r="N30" s="102"/>
     </row>
     <row r="31" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" s="52" t="s">
@@ -5506,7 +5535,9 @@
       <c r="I31" s="59">
         <v>1</v>
       </c>
-      <c r="J31" s="59"/>
+      <c r="J31" s="59">
+        <v>1</v>
+      </c>
       <c r="K31" s="59"/>
       <c r="L31" s="60"/>
       <c r="M31" s="60"/>
@@ -5523,17 +5554,17 @@
       <c r="E32" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="F32" s="100"/>
-      <c r="G32" s="101"/>
-      <c r="H32" s="102"/>
-      <c r="I32" s="118"/>
-      <c r="J32" s="119"/>
-      <c r="K32" s="120"/>
-      <c r="L32" s="109"/>
-      <c r="M32" s="110"/>
-      <c r="N32" s="111"/>
-      <c r="O32" s="136" t="s">
-        <v>91</v>
+      <c r="F32" s="121"/>
+      <c r="G32" s="122"/>
+      <c r="H32" s="123"/>
+      <c r="I32" s="112"/>
+      <c r="J32" s="113"/>
+      <c r="K32" s="114"/>
+      <c r="L32" s="103"/>
+      <c r="M32" s="104"/>
+      <c r="N32" s="105"/>
+      <c r="O32" s="70" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="2:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -5542,15 +5573,15 @@
       </c>
       <c r="D33" s="54"/>
       <c r="E33" s="55"/>
-      <c r="F33" s="103"/>
-      <c r="G33" s="104"/>
-      <c r="H33" s="105"/>
-      <c r="I33" s="121"/>
-      <c r="J33" s="122"/>
-      <c r="K33" s="123"/>
-      <c r="L33" s="112"/>
-      <c r="M33" s="113"/>
-      <c r="N33" s="114"/>
+      <c r="F33" s="124"/>
+      <c r="G33" s="125"/>
+      <c r="H33" s="126"/>
+      <c r="I33" s="115"/>
+      <c r="J33" s="116"/>
+      <c r="K33" s="117"/>
+      <c r="L33" s="106"/>
+      <c r="M33" s="107"/>
+      <c r="N33" s="108"/>
       <c r="O33" s="46" t="str">
         <f>IF(OR( AND(C34=D36,OR(F33&lt;&gt;G33, I33&lt;&gt;J33,L33&lt;&gt;M33)),  AND(D36=E34,OR(G33&lt;&gt;H33,J33&lt;&gt;K33,M33&lt;&gt;N33)), AND(C34=E34, OR(F33&lt;&gt;H33,I33&lt;&gt;K33,L33&lt;&gt;N33) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5567,15 +5598,15 @@
       <c r="E34" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="103"/>
-      <c r="G34" s="104"/>
-      <c r="H34" s="105"/>
-      <c r="I34" s="121"/>
-      <c r="J34" s="122"/>
-      <c r="K34" s="123"/>
-      <c r="L34" s="112"/>
-      <c r="M34" s="113"/>
-      <c r="N34" s="114"/>
+      <c r="F34" s="124"/>
+      <c r="G34" s="125"/>
+      <c r="H34" s="126"/>
+      <c r="I34" s="115"/>
+      <c r="J34" s="116"/>
+      <c r="K34" s="117"/>
+      <c r="L34" s="106"/>
+      <c r="M34" s="107"/>
+      <c r="N34" s="108"/>
     </row>
     <row r="35" spans="2:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="52" t="s">
@@ -5584,15 +5615,15 @@
       <c r="C35" s="53"/>
       <c r="D35" s="54"/>
       <c r="E35" s="55"/>
-      <c r="F35" s="103"/>
-      <c r="G35" s="104"/>
-      <c r="H35" s="105"/>
-      <c r="I35" s="121"/>
-      <c r="J35" s="122"/>
-      <c r="K35" s="123"/>
-      <c r="L35" s="112"/>
-      <c r="M35" s="113"/>
-      <c r="N35" s="114"/>
+      <c r="F35" s="124"/>
+      <c r="G35" s="125"/>
+      <c r="H35" s="126"/>
+      <c r="I35" s="115"/>
+      <c r="J35" s="116"/>
+      <c r="K35" s="117"/>
+      <c r="L35" s="106"/>
+      <c r="M35" s="107"/>
+      <c r="N35" s="108"/>
       <c r="O35" s="46" t="str">
         <f>IF(OR( AND(C36=D34,OR(F35&lt;&gt;G35, I35&lt;&gt;J35,L35&lt;&gt;M35)),  AND(D34=E36,OR(G35&lt;&gt;H35,J35&lt;&gt;K35,M35&lt;&gt;N35)), AND(C36=E36, OR(F35&lt;&gt;H35,I35&lt;&gt;K35,L35&lt;&gt;N35) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5609,15 +5640,15 @@
       <c r="E36" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="F36" s="106"/>
-      <c r="G36" s="107"/>
-      <c r="H36" s="108"/>
-      <c r="I36" s="124"/>
-      <c r="J36" s="125"/>
-      <c r="K36" s="126"/>
-      <c r="L36" s="115"/>
-      <c r="M36" s="116"/>
-      <c r="N36" s="117"/>
+      <c r="F36" s="127"/>
+      <c r="G36" s="128"/>
+      <c r="H36" s="129"/>
+      <c r="I36" s="118"/>
+      <c r="J36" s="119"/>
+      <c r="K36" s="120"/>
+      <c r="L36" s="109"/>
+      <c r="M36" s="110"/>
+      <c r="N36" s="111"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C37" s="46"/>
@@ -5634,11 +5665,11 @@
       <c r="N37" s="51"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C38" s="135" t="s">
+      <c r="C38" s="130" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="135"/>
-      <c r="E38" s="135"/>
+      <c r="D38" s="130"/>
+      <c r="E38" s="130"/>
       <c r="F38" s="51"/>
       <c r="G38" s="51"/>
       <c r="H38" s="51"/>
@@ -7956,16 +7987,9 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B5:N5"/>
-    <mergeCell ref="B19:N19"/>
-    <mergeCell ref="B12:N12"/>
-    <mergeCell ref="B4:N4"/>
-    <mergeCell ref="L7:N11"/>
-    <mergeCell ref="I7:K11"/>
-    <mergeCell ref="F7:H11"/>
-    <mergeCell ref="L14:N18"/>
-    <mergeCell ref="I14:K18"/>
-    <mergeCell ref="F14:H18"/>
+    <mergeCell ref="B28:N28"/>
+    <mergeCell ref="B27:N27"/>
+    <mergeCell ref="B26:N26"/>
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="L21:N25"/>
     <mergeCell ref="I21:K25"/>
@@ -7982,9 +8006,16 @@
     <mergeCell ref="I32:K36"/>
     <mergeCell ref="B30:N30"/>
     <mergeCell ref="B29:N29"/>
-    <mergeCell ref="B28:N28"/>
-    <mergeCell ref="B27:N27"/>
-    <mergeCell ref="B26:N26"/>
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="B19:N19"/>
+    <mergeCell ref="B12:N12"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="L7:N11"/>
+    <mergeCell ref="I7:K11"/>
+    <mergeCell ref="F7:H11"/>
+    <mergeCell ref="L14:N18"/>
+    <mergeCell ref="I14:K18"/>
+    <mergeCell ref="F14:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[Yusuf] finish qualitative eval
</commit_message>
<xml_diff>
--- a/project/evaluation/qualitative_evaluation/qualitative_evaluation_table.xlsx
+++ b/project/evaluation/qualitative_evaluation/qualitative_evaluation_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandrafriebolin/Desktop/WS23-24/transformers/nlpt_group/project/evaluation/qualitative_evaluation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusuf/master/nlp/Assignment1/repo/nlpt_group/project/evaluation/qualitative_evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B7F810-BD87-8243-96BA-226E12151B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED96FB1-1B84-0A44-966E-4103507307EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{BFF5F178-14AB-6B4F-B81C-3E61E0B93405}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17440" activeTab="2" xr2:uid="{BFF5F178-14AB-6B4F-B81C-3E61E0B93405}"/>
   </bookViews>
   <sheets>
     <sheet name="Correct retrieval" sheetId="1" r:id="rId1"/>
@@ -866,15 +866,72 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -887,72 +944,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1032,9 +1035,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1768,9 +1768,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5956BC-300C-CB42-87CA-185E2E097C22}">
   <dimension ref="A1:O205"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M26" sqref="M26"/>
+    <sheetView topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1792,35 +1792,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="90" t="s">
+      <c r="F1" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="74" t="s">
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="80" t="s">
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C2" s="77"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="79"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="98"/>
       <c r="F2" s="25" t="s">
         <v>44</v>
       </c>
@@ -1853,21 +1853,21 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="76"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="88"/>
     </row>
     <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
@@ -1882,21 +1882,27 @@
       <c r="G4" s="25">
         <v>2</v>
       </c>
-      <c r="H4" s="25"/>
+      <c r="H4" s="25">
+        <v>2</v>
+      </c>
       <c r="I4" s="26">
         <v>2</v>
       </c>
       <c r="J4" s="26">
         <v>2</v>
       </c>
-      <c r="K4" s="26"/>
+      <c r="K4" s="26">
+        <v>2</v>
+      </c>
       <c r="L4" s="27">
         <v>1</v>
       </c>
       <c r="M4" s="27">
         <v>1</v>
       </c>
-      <c r="N4" s="27"/>
+      <c r="N4" s="27">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="255" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="32"/>
@@ -1909,15 +1915,15 @@
       <c r="E5" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="87"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="86"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="83"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="76"/>
       <c r="O5" s="45" t="s">
         <v>91</v>
       </c>
@@ -1926,61 +1932,61 @@
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="76"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="88"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="75"/>
-      <c r="M7" s="75"/>
-      <c r="N7" s="76"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="88"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="76"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="88"/>
     </row>
     <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" s="32" t="s">
@@ -1994,21 +2000,27 @@
       <c r="G9" s="25">
         <v>1</v>
       </c>
-      <c r="H9" s="25"/>
+      <c r="H9" s="25">
+        <v>1</v>
+      </c>
       <c r="I9" s="26">
         <v>1</v>
       </c>
       <c r="J9" s="26">
         <v>1</v>
       </c>
-      <c r="K9" s="26"/>
+      <c r="K9" s="26">
+        <v>2</v>
+      </c>
       <c r="L9" s="27">
         <v>3</v>
       </c>
       <c r="M9" s="27">
         <v>2</v>
       </c>
-      <c r="N9" s="27"/>
+      <c r="N9" s="27">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="404" x14ac:dyDescent="0.2">
       <c r="B10" s="32"/>
@@ -2021,15 +2033,15 @@
       <c r="E10" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="87"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="85"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="82"/>
-      <c r="N10" s="83"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="76"/>
       <c r="O10" s="44" t="s">
         <v>87</v>
       </c>
@@ -2038,21 +2050,21 @@
       <c r="A11" s="1">
         <v>5</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="76"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="88"/>
     </row>
     <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="s">
@@ -2066,21 +2078,27 @@
       <c r="G12" s="25">
         <v>2</v>
       </c>
-      <c r="H12" s="25"/>
+      <c r="H12" s="25">
+        <v>2</v>
+      </c>
       <c r="I12" s="26">
         <v>1</v>
       </c>
       <c r="J12" s="26">
         <v>1</v>
       </c>
-      <c r="K12" s="26"/>
+      <c r="K12" s="26">
+        <v>1</v>
+      </c>
       <c r="L12" s="27">
         <v>1</v>
       </c>
       <c r="M12" s="27">
         <v>1</v>
       </c>
-      <c r="N12" s="27"/>
+      <c r="N12" s="27">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="32"/>
@@ -2093,15 +2111,15 @@
       <c r="E13" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="87"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="85"/>
-      <c r="K13" s="86"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="83"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="74"/>
+      <c r="M13" s="75"/>
+      <c r="N13" s="76"/>
       <c r="O13" s="44" t="s">
         <v>86</v>
       </c>
@@ -2110,21 +2128,21 @@
       <c r="A14" s="1">
         <v>6</v>
       </c>
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="75"/>
-      <c r="M14" s="75"/>
-      <c r="N14" s="76"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="87"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="87"/>
+      <c r="L14" s="87"/>
+      <c r="M14" s="87"/>
+      <c r="N14" s="88"/>
     </row>
     <row r="15" spans="1:15" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="52" t="s">
@@ -2139,21 +2157,27 @@
       <c r="G15" s="48">
         <v>2</v>
       </c>
-      <c r="H15" s="48"/>
+      <c r="H15" s="48">
+        <v>2</v>
+      </c>
       <c r="I15" s="49">
         <v>3</v>
       </c>
       <c r="J15" s="49">
         <v>3</v>
       </c>
-      <c r="K15" s="49"/>
+      <c r="K15" s="49">
+        <v>2</v>
+      </c>
       <c r="L15" s="50">
         <v>2</v>
       </c>
       <c r="M15" s="50">
         <v>2</v>
       </c>
-      <c r="N15" s="50"/>
+      <c r="N15" s="50">
+        <v>2</v>
+      </c>
       <c r="O15" s="46" t="str">
         <f>IF(OR( AND(C16=D16,OR(F15&lt;&gt;G15, I15&lt;&gt;J15,L15&lt;&gt;M15)),  AND(D16=E16,OR(G15&lt;&gt;H15,J15&lt;&gt;K15,M15&lt;&gt;N15)), AND(C16=E16, OR(F15&lt;&gt;H15,I15&lt;&gt;K15,L15&lt;&gt;N15) )), "error: different mark to same abstract","")</f>
         <v>error: different mark to same abstract</v>
@@ -2170,15 +2194,15 @@
       <c r="E16" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="97"/>
-      <c r="G16" s="98"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="94"/>
-      <c r="J16" s="95"/>
-      <c r="K16" s="96"/>
-      <c r="L16" s="91"/>
-      <c r="M16" s="92"/>
-      <c r="N16" s="93"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="89"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="91"/>
       <c r="O16" s="52" t="s">
         <v>90</v>
       </c>
@@ -2187,21 +2211,21 @@
       <c r="A17" s="1">
         <v>7</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="75"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="76"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="87"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="88"/>
     </row>
     <row r="18" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="32" t="s">
@@ -2215,21 +2239,27 @@
       <c r="G18" s="37">
         <v>2</v>
       </c>
-      <c r="H18" s="25"/>
+      <c r="H18" s="25">
+        <v>3</v>
+      </c>
       <c r="I18" s="26">
         <v>3</v>
       </c>
       <c r="J18" s="26">
         <v>3</v>
       </c>
-      <c r="K18" s="26"/>
+      <c r="K18" s="26">
+        <v>3</v>
+      </c>
       <c r="L18" s="27">
         <v>3</v>
       </c>
       <c r="M18" s="27">
         <v>3</v>
       </c>
-      <c r="N18" s="27"/>
+      <c r="N18" s="27">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B19" s="32"/>
@@ -2242,15 +2272,15 @@
       <c r="E19" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="87"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="89"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="86"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="82"/>
-      <c r="N19" s="83"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="74"/>
+      <c r="M19" s="75"/>
+      <c r="N19" s="76"/>
       <c r="O19" s="44" t="s">
         <v>85</v>
       </c>
@@ -2259,21 +2289,21 @@
       <c r="A20" s="1">
         <v>8</v>
       </c>
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="75"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="75"/>
-      <c r="K20" s="75"/>
-      <c r="L20" s="75"/>
-      <c r="M20" s="75"/>
-      <c r="N20" s="76"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="87"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="87"/>
+      <c r="M20" s="87"/>
+      <c r="N20" s="88"/>
     </row>
     <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="32" t="s">
@@ -2287,21 +2317,27 @@
       <c r="G21" s="37">
         <v>3</v>
       </c>
-      <c r="H21" s="25"/>
+      <c r="H21" s="25">
+        <v>1</v>
+      </c>
       <c r="I21" s="26">
         <v>1</v>
       </c>
       <c r="J21" s="38">
         <v>3</v>
       </c>
-      <c r="K21" s="26"/>
+      <c r="K21" s="26">
+        <v>1</v>
+      </c>
       <c r="L21" s="27">
         <v>3</v>
       </c>
       <c r="M21" s="27">
         <v>3</v>
       </c>
-      <c r="N21" s="27"/>
+      <c r="N21" s="27">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B22" s="32"/>
@@ -2314,15 +2350,15 @@
       <c r="E22" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="87"/>
-      <c r="G22" s="88"/>
-      <c r="H22" s="89"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="85"/>
-      <c r="K22" s="86"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="82"/>
-      <c r="N22" s="83"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="74"/>
+      <c r="M22" s="75"/>
+      <c r="N22" s="76"/>
       <c r="O22" s="44" t="s">
         <v>88</v>
       </c>
@@ -2331,21 +2367,21 @@
       <c r="A23" s="1">
         <v>9</v>
       </c>
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="75"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="75"/>
-      <c r="L23" s="75"/>
-      <c r="M23" s="75"/>
-      <c r="N23" s="76"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="87"/>
+      <c r="J23" s="87"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="87"/>
+      <c r="M23" s="87"/>
+      <c r="N23" s="88"/>
     </row>
     <row r="24" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="32" t="s">
@@ -2359,21 +2395,27 @@
       <c r="G24" s="25">
         <v>1</v>
       </c>
-      <c r="H24" s="25"/>
+      <c r="H24" s="25">
+        <v>1</v>
+      </c>
       <c r="I24" s="26">
         <v>1</v>
       </c>
       <c r="J24" s="26">
         <v>1</v>
       </c>
-      <c r="K24" s="26"/>
+      <c r="K24" s="26">
+        <v>1</v>
+      </c>
       <c r="L24" s="27">
         <v>1</v>
       </c>
       <c r="M24" s="27">
         <v>1</v>
       </c>
-      <c r="N24" s="27"/>
+      <c r="N24" s="27">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:15" ht="306" x14ac:dyDescent="0.2">
       <c r="B25" s="32"/>
@@ -2386,15 +2428,15 @@
       <c r="E25" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="F25" s="87"/>
-      <c r="G25" s="88"/>
-      <c r="H25" s="89"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="85"/>
-      <c r="K25" s="86"/>
-      <c r="L25" s="81"/>
-      <c r="M25" s="82"/>
-      <c r="N25" s="83"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="81"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="77"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="74"/>
+      <c r="M25" s="75"/>
+      <c r="N25" s="76"/>
     </row>
     <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="32" t="s">
@@ -2408,21 +2450,27 @@
       <c r="G26" s="25">
         <v>1</v>
       </c>
-      <c r="H26" s="25"/>
+      <c r="H26" s="25">
+        <v>1</v>
+      </c>
       <c r="I26" s="26">
         <v>1</v>
       </c>
       <c r="J26" s="26">
         <v>1</v>
       </c>
-      <c r="K26" s="26"/>
+      <c r="K26" s="26">
+        <v>1</v>
+      </c>
       <c r="L26" s="27">
         <v>1</v>
       </c>
       <c r="M26" s="27">
         <v>1</v>
       </c>
-      <c r="N26" s="27"/>
+      <c r="N26" s="27">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:15" ht="388" x14ac:dyDescent="0.2">
       <c r="B27" s="32"/>
@@ -2435,35 +2483,35 @@
       <c r="E27" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="87"/>
-      <c r="G27" s="88"/>
-      <c r="H27" s="89"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="86"/>
-      <c r="L27" s="81"/>
-      <c r="M27" s="82"/>
-      <c r="N27" s="83"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="77"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="74"/>
+      <c r="M27" s="75"/>
+      <c r="N27" s="76"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>10</v>
       </c>
-      <c r="B28" s="75" t="s">
+      <c r="B28" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="75"/>
-      <c r="K28" s="75"/>
-      <c r="L28" s="75"/>
-      <c r="M28" s="75"/>
-      <c r="N28" s="76"/>
+      <c r="C28" s="87"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="87"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="87"/>
+      <c r="M28" s="87"/>
+      <c r="N28" s="88"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C29"/>
@@ -2480,11 +2528,11 @@
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C30" s="100" t="s">
+      <c r="C30" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="100"/>
-      <c r="E30" s="100"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="86"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -2496,17 +2544,17 @@
       <c r="N30" s="1"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C31" s="21" t="e">
+      <c r="C31" s="21">
         <f>AVERAGE(AVERAGE(F4:F28),AVERAGE(G4:G30),AVERAGE(H4:H30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D31" s="21" t="e">
+        <v>1.7083333333333333</v>
+      </c>
+      <c r="D31" s="21">
         <f>AVERAGE(AVERAGE(I4:I28),AVERAGE(J4:J30),AVERAGE(K4:K30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E31" s="21" t="e">
+        <v>1.7083333333333333</v>
+      </c>
+      <c r="E31" s="21">
         <f>AVERAGE(AVERAGE(L4:L28),AVERAGE(M4:M30),AVERAGE(N4:N30))</f>
-        <v>#DIV/0!</v>
+        <v>1.7916666666666667</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -4802,20 +4850,17 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B6:N6"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="B7:N7"/>
     <mergeCell ref="B28:N28"/>
     <mergeCell ref="B23:N23"/>
@@ -4832,17 +4877,20 @@
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="L16:N16"/>
     <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B6:N6"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4852,9 +4900,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03816060-24A7-D946-9AB1-F7E07293AE02}">
   <dimension ref="A1:O213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5007,7 +5055,9 @@
       <c r="G6" s="58">
         <v>1</v>
       </c>
-      <c r="H6" s="58"/>
+      <c r="H6" s="58">
+        <v>1</v>
+      </c>
       <c r="I6" s="59"/>
       <c r="J6" s="59"/>
       <c r="K6" s="59"/>
@@ -5017,7 +5067,9 @@
       <c r="M6" s="60">
         <v>1</v>
       </c>
-      <c r="N6" s="60"/>
+      <c r="N6" s="60">
+        <v>1</v>
+      </c>
       <c r="O6" s="46" t="e">
         <f>IF(OR( AND(C7=#REF!,OR(F6&lt;&gt;G6, I6&lt;&gt;J6,L6&lt;&gt;M6)),  AND(#REF!=E7,OR(G6&lt;&gt;H6,J6&lt;&gt;K6,M6&lt;&gt;N6)), AND(C7=E7, OR(F6&lt;&gt;H6,I6&lt;&gt;K6,L6&lt;&gt;N6) )), "error: different mark to same abstract","")</f>
         <v>#REF!</v>
@@ -5034,15 +5086,15 @@
       <c r="E7" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="121"/>
-      <c r="G7" s="122"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="114"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="104"/>
-      <c r="N7" s="105"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="114"/>
+      <c r="K7" s="115"/>
+      <c r="L7" s="104"/>
+      <c r="M7" s="105"/>
+      <c r="N7" s="106"/>
     </row>
     <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="52" t="s">
@@ -5051,15 +5103,15 @@
       <c r="C8" s="53"/>
       <c r="D8" s="54"/>
       <c r="E8" s="56"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="125"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="115"/>
-      <c r="J8" s="116"/>
-      <c r="K8" s="117"/>
-      <c r="L8" s="106"/>
-      <c r="M8" s="107"/>
-      <c r="N8" s="108"/>
+      <c r="F8" s="125"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="127"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="117"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="107"/>
+      <c r="M8" s="108"/>
+      <c r="N8" s="109"/>
       <c r="O8" s="46" t="str">
         <f>IF(OR( AND(C9=D7,OR(F8&lt;&gt;G8, I8&lt;&gt;J8,L8&lt;&gt;M8)),  AND(D7=E9,OR(G8&lt;&gt;H8,J8&lt;&gt;K8,M8&lt;&gt;N8)), AND(C9=E9, OR(F8&lt;&gt;H8,I8&lt;&gt;K8,L8&lt;&gt;N8) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5076,15 +5128,15 @@
       <c r="E9" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="124"/>
-      <c r="G9" s="125"/>
-      <c r="H9" s="126"/>
-      <c r="I9" s="115"/>
-      <c r="J9" s="116"/>
-      <c r="K9" s="117"/>
-      <c r="L9" s="106"/>
-      <c r="M9" s="107"/>
-      <c r="N9" s="108"/>
+      <c r="F9" s="125"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="127"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="117"/>
+      <c r="K9" s="118"/>
+      <c r="L9" s="107"/>
+      <c r="M9" s="108"/>
+      <c r="N9" s="109"/>
     </row>
     <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="52" t="s">
@@ -5093,15 +5145,15 @@
       <c r="C10" s="53"/>
       <c r="D10" s="54"/>
       <c r="E10" s="61"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="125"/>
-      <c r="H10" s="126"/>
-      <c r="I10" s="115"/>
-      <c r="J10" s="116"/>
-      <c r="K10" s="117"/>
-      <c r="L10" s="106"/>
-      <c r="M10" s="107"/>
-      <c r="N10" s="108"/>
+      <c r="F10" s="125"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="127"/>
+      <c r="I10" s="116"/>
+      <c r="J10" s="117"/>
+      <c r="K10" s="118"/>
+      <c r="L10" s="107"/>
+      <c r="M10" s="108"/>
+      <c r="N10" s="109"/>
       <c r="O10" s="46" t="str">
         <f>IF(OR( AND(C11=D9,OR(F10&lt;&gt;G10, I10&lt;&gt;J10,L10&lt;&gt;M10)),  AND(D9=E11,OR(G10&lt;&gt;H10,J10&lt;&gt;K10,M10&lt;&gt;N10)), AND(C11=E11, OR(F10&lt;&gt;H10,I10&lt;&gt;K10,L10&lt;&gt;N10) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5118,15 +5170,15 @@
       <c r="E11" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="127"/>
-      <c r="G11" s="128"/>
-      <c r="H11" s="129"/>
-      <c r="I11" s="118"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="120"/>
-      <c r="L11" s="109"/>
-      <c r="M11" s="110"/>
-      <c r="N11" s="111"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="129"/>
+      <c r="H11" s="130"/>
+      <c r="I11" s="119"/>
+      <c r="J11" s="120"/>
+      <c r="K11" s="121"/>
+      <c r="L11" s="110"/>
+      <c r="M11" s="111"/>
+      <c r="N11" s="112"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="51">
@@ -5167,10 +5219,12 @@
       <c r="M13" s="60">
         <v>1</v>
       </c>
-      <c r="N13" s="60"/>
+      <c r="N13" s="60">
+        <v>1</v>
+      </c>
       <c r="O13" s="46" t="str">
         <f>IF(OR( AND(C14=D16,OR(F13&lt;&gt;G13, I13&lt;&gt;J13,L13&lt;&gt;M13)),  AND(D16=E16,OR(G13&lt;&gt;H13,J13&lt;&gt;K13,M13&lt;&gt;N13)), AND(C14=E16, OR(F13&lt;&gt;H13,I13&lt;&gt;K13,L13&lt;&gt;N13) )), "error: different mark to same abstract","")</f>
-        <v>error: different mark to same abstract</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:15" ht="272" x14ac:dyDescent="0.2">
@@ -5184,15 +5238,15 @@
       <c r="E14" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="121"/>
-      <c r="G14" s="122"/>
-      <c r="H14" s="123"/>
-      <c r="I14" s="112"/>
-      <c r="J14" s="113"/>
-      <c r="K14" s="114"/>
-      <c r="L14" s="103"/>
-      <c r="M14" s="104"/>
-      <c r="N14" s="105"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="113"/>
+      <c r="J14" s="114"/>
+      <c r="K14" s="115"/>
+      <c r="L14" s="104"/>
+      <c r="M14" s="105"/>
+      <c r="N14" s="106"/>
     </row>
     <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="52" t="s">
@@ -5200,15 +5254,15 @@
       </c>
       <c r="D15" s="54"/>
       <c r="E15" s="55"/>
-      <c r="F15" s="124"/>
-      <c r="G15" s="125"/>
-      <c r="H15" s="126"/>
-      <c r="I15" s="115"/>
-      <c r="J15" s="116"/>
-      <c r="K15" s="117"/>
-      <c r="L15" s="106"/>
-      <c r="M15" s="107"/>
-      <c r="N15" s="108"/>
+      <c r="F15" s="125"/>
+      <c r="G15" s="126"/>
+      <c r="H15" s="127"/>
+      <c r="I15" s="116"/>
+      <c r="J15" s="117"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="107"/>
+      <c r="M15" s="108"/>
+      <c r="N15" s="109"/>
       <c r="O15" s="46" t="str">
         <f>IF(OR( AND(C16=D14,OR(F15&lt;&gt;G15, I15&lt;&gt;J15,L15&lt;&gt;M15)),  AND(D14=E14,OR(G15&lt;&gt;H15,J15&lt;&gt;K15,M15&lt;&gt;N15)), AND(C16=E14, OR(F15&lt;&gt;H15,I15&lt;&gt;K15,L15&lt;&gt;N15) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5225,15 +5279,15 @@
       <c r="E16" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="124"/>
-      <c r="G16" s="125"/>
-      <c r="H16" s="126"/>
-      <c r="I16" s="115"/>
-      <c r="J16" s="116"/>
-      <c r="K16" s="117"/>
-      <c r="L16" s="106"/>
-      <c r="M16" s="107"/>
-      <c r="N16" s="108"/>
+      <c r="F16" s="125"/>
+      <c r="G16" s="126"/>
+      <c r="H16" s="127"/>
+      <c r="I16" s="116"/>
+      <c r="J16" s="117"/>
+      <c r="K16" s="118"/>
+      <c r="L16" s="107"/>
+      <c r="M16" s="108"/>
+      <c r="N16" s="109"/>
     </row>
     <row r="17" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="52" t="s">
@@ -5241,15 +5295,15 @@
       </c>
       <c r="D17" s="54"/>
       <c r="E17" s="55"/>
-      <c r="F17" s="124"/>
-      <c r="G17" s="125"/>
-      <c r="H17" s="126"/>
-      <c r="I17" s="115"/>
-      <c r="J17" s="116"/>
-      <c r="K17" s="117"/>
-      <c r="L17" s="106"/>
-      <c r="M17" s="107"/>
-      <c r="N17" s="108"/>
+      <c r="F17" s="125"/>
+      <c r="G17" s="126"/>
+      <c r="H17" s="127"/>
+      <c r="I17" s="116"/>
+      <c r="J17" s="117"/>
+      <c r="K17" s="118"/>
+      <c r="L17" s="107"/>
+      <c r="M17" s="108"/>
+      <c r="N17" s="109"/>
       <c r="O17" s="46" t="str">
         <f>IF(OR( AND(C18=D18,OR(F17&lt;&gt;G17, I17&lt;&gt;J17,L17&lt;&gt;M17)),  AND(D18=E18,OR(G17&lt;&gt;H17,J17&lt;&gt;K17,M17&lt;&gt;N17)), AND(C18=E18, OR(F17&lt;&gt;H17,I17&lt;&gt;K17,L17&lt;&gt;N17) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5266,15 +5320,15 @@
       <c r="E18" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="127"/>
-      <c r="G18" s="128"/>
-      <c r="H18" s="129"/>
-      <c r="I18" s="118"/>
-      <c r="J18" s="119"/>
-      <c r="K18" s="120"/>
-      <c r="L18" s="109"/>
-      <c r="M18" s="110"/>
-      <c r="N18" s="111"/>
+      <c r="F18" s="128"/>
+      <c r="G18" s="129"/>
+      <c r="H18" s="130"/>
+      <c r="I18" s="119"/>
+      <c r="J18" s="120"/>
+      <c r="K18" s="121"/>
+      <c r="L18" s="110"/>
+      <c r="M18" s="111"/>
+      <c r="N18" s="112"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="51">
@@ -5311,7 +5365,9 @@
         <v>1</v>
       </c>
       <c r="J20" s="59"/>
-      <c r="K20" s="59"/>
+      <c r="K20" s="59">
+        <v>1</v>
+      </c>
       <c r="L20" s="60"/>
       <c r="M20" s="60"/>
       <c r="N20" s="60"/>
@@ -5331,15 +5387,15 @@
       <c r="E21" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="121"/>
-      <c r="G21" s="122"/>
-      <c r="H21" s="123"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="113"/>
-      <c r="K21" s="114"/>
-      <c r="L21" s="103"/>
-      <c r="M21" s="104"/>
-      <c r="N21" s="105"/>
+      <c r="F21" s="122"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="124"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="114"/>
+      <c r="K21" s="115"/>
+      <c r="L21" s="104"/>
+      <c r="M21" s="105"/>
+      <c r="N21" s="106"/>
     </row>
     <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="52" t="s">
@@ -5347,15 +5403,15 @@
       </c>
       <c r="D22" s="54"/>
       <c r="E22" s="55"/>
-      <c r="F22" s="124"/>
-      <c r="G22" s="125"/>
-      <c r="H22" s="126"/>
-      <c r="I22" s="115"/>
-      <c r="J22" s="116"/>
-      <c r="K22" s="117"/>
-      <c r="L22" s="106"/>
-      <c r="M22" s="107"/>
-      <c r="N22" s="108"/>
+      <c r="F22" s="125"/>
+      <c r="G22" s="126"/>
+      <c r="H22" s="127"/>
+      <c r="I22" s="116"/>
+      <c r="J22" s="117"/>
+      <c r="K22" s="118"/>
+      <c r="L22" s="107"/>
+      <c r="M22" s="108"/>
+      <c r="N22" s="109"/>
       <c r="O22" s="46" t="str">
         <f>IF(OR( AND(C23=D23,OR(F22&lt;&gt;G22, I22&lt;&gt;J22,L22&lt;&gt;M22)),  AND(D23=E25,OR(G22&lt;&gt;H22,J22&lt;&gt;K22,M22&lt;&gt;N22)), AND(C23=E25, OR(F22&lt;&gt;H22,I22&lt;&gt;K22,L22&lt;&gt;N22) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5372,15 +5428,15 @@
       <c r="E23" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="124"/>
-      <c r="G23" s="125"/>
-      <c r="H23" s="126"/>
-      <c r="I23" s="115"/>
-      <c r="J23" s="116"/>
-      <c r="K23" s="117"/>
-      <c r="L23" s="106"/>
-      <c r="M23" s="107"/>
-      <c r="N23" s="108"/>
+      <c r="F23" s="125"/>
+      <c r="G23" s="126"/>
+      <c r="H23" s="127"/>
+      <c r="I23" s="116"/>
+      <c r="J23" s="117"/>
+      <c r="K23" s="118"/>
+      <c r="L23" s="107"/>
+      <c r="M23" s="108"/>
+      <c r="N23" s="109"/>
     </row>
     <row r="24" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="52" t="s">
@@ -5388,15 +5444,15 @@
       </c>
       <c r="D24" s="54"/>
       <c r="E24" s="55"/>
-      <c r="F24" s="124"/>
-      <c r="G24" s="125"/>
-      <c r="H24" s="126"/>
-      <c r="I24" s="115"/>
-      <c r="J24" s="116"/>
-      <c r="K24" s="117"/>
-      <c r="L24" s="106"/>
-      <c r="M24" s="107"/>
-      <c r="N24" s="108"/>
+      <c r="F24" s="125"/>
+      <c r="G24" s="126"/>
+      <c r="H24" s="127"/>
+      <c r="I24" s="116"/>
+      <c r="J24" s="117"/>
+      <c r="K24" s="118"/>
+      <c r="L24" s="107"/>
+      <c r="M24" s="108"/>
+      <c r="N24" s="109"/>
       <c r="O24" s="46" t="str">
         <f>IF(OR( AND(C25=D25,OR(F24&lt;&gt;G24, I24&lt;&gt;J24,L24&lt;&gt;M24)),  AND(D25=E23,OR(G24&lt;&gt;H24,J24&lt;&gt;K24,M24&lt;&gt;N24)), AND(C25=E23, OR(F24&lt;&gt;H24,I24&lt;&gt;K24,L24&lt;&gt;N24) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5413,15 +5469,15 @@
       <c r="E25" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="127"/>
-      <c r="G25" s="128"/>
-      <c r="H25" s="129"/>
-      <c r="I25" s="118"/>
-      <c r="J25" s="119"/>
-      <c r="K25" s="120"/>
-      <c r="L25" s="109"/>
-      <c r="M25" s="110"/>
-      <c r="N25" s="111"/>
+      <c r="F25" s="128"/>
+      <c r="G25" s="129"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="119"/>
+      <c r="J25" s="120"/>
+      <c r="K25" s="121"/>
+      <c r="L25" s="110"/>
+      <c r="M25" s="111"/>
+      <c r="N25" s="112"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="51">
@@ -5538,7 +5594,9 @@
       <c r="J31" s="59">
         <v>1</v>
       </c>
-      <c r="K31" s="59"/>
+      <c r="K31" s="59">
+        <v>1</v>
+      </c>
       <c r="L31" s="60"/>
       <c r="M31" s="60"/>
       <c r="N31" s="60"/>
@@ -5554,15 +5612,15 @@
       <c r="E32" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="F32" s="121"/>
-      <c r="G32" s="122"/>
-      <c r="H32" s="123"/>
-      <c r="I32" s="112"/>
-      <c r="J32" s="113"/>
-      <c r="K32" s="114"/>
-      <c r="L32" s="103"/>
-      <c r="M32" s="104"/>
-      <c r="N32" s="105"/>
+      <c r="F32" s="122"/>
+      <c r="G32" s="123"/>
+      <c r="H32" s="124"/>
+      <c r="I32" s="113"/>
+      <c r="J32" s="114"/>
+      <c r="K32" s="115"/>
+      <c r="L32" s="104"/>
+      <c r="M32" s="105"/>
+      <c r="N32" s="106"/>
       <c r="O32" s="70" t="s">
         <v>89</v>
       </c>
@@ -5573,15 +5631,15 @@
       </c>
       <c r="D33" s="54"/>
       <c r="E33" s="55"/>
-      <c r="F33" s="124"/>
-      <c r="G33" s="125"/>
-      <c r="H33" s="126"/>
-      <c r="I33" s="115"/>
-      <c r="J33" s="116"/>
-      <c r="K33" s="117"/>
-      <c r="L33" s="106"/>
-      <c r="M33" s="107"/>
-      <c r="N33" s="108"/>
+      <c r="F33" s="125"/>
+      <c r="G33" s="126"/>
+      <c r="H33" s="127"/>
+      <c r="I33" s="116"/>
+      <c r="J33" s="117"/>
+      <c r="K33" s="118"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="108"/>
+      <c r="N33" s="109"/>
       <c r="O33" s="46" t="str">
         <f>IF(OR( AND(C34=D36,OR(F33&lt;&gt;G33, I33&lt;&gt;J33,L33&lt;&gt;M33)),  AND(D36=E34,OR(G33&lt;&gt;H33,J33&lt;&gt;K33,M33&lt;&gt;N33)), AND(C34=E34, OR(F33&lt;&gt;H33,I33&lt;&gt;K33,L33&lt;&gt;N33) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5598,15 +5656,15 @@
       <c r="E34" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="124"/>
-      <c r="G34" s="125"/>
-      <c r="H34" s="126"/>
-      <c r="I34" s="115"/>
-      <c r="J34" s="116"/>
-      <c r="K34" s="117"/>
-      <c r="L34" s="106"/>
-      <c r="M34" s="107"/>
-      <c r="N34" s="108"/>
+      <c r="F34" s="125"/>
+      <c r="G34" s="126"/>
+      <c r="H34" s="127"/>
+      <c r="I34" s="116"/>
+      <c r="J34" s="117"/>
+      <c r="K34" s="118"/>
+      <c r="L34" s="107"/>
+      <c r="M34" s="108"/>
+      <c r="N34" s="109"/>
     </row>
     <row r="35" spans="2:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="52" t="s">
@@ -5615,15 +5673,15 @@
       <c r="C35" s="53"/>
       <c r="D35" s="54"/>
       <c r="E35" s="55"/>
-      <c r="F35" s="124"/>
-      <c r="G35" s="125"/>
-      <c r="H35" s="126"/>
-      <c r="I35" s="115"/>
-      <c r="J35" s="116"/>
-      <c r="K35" s="117"/>
-      <c r="L35" s="106"/>
-      <c r="M35" s="107"/>
-      <c r="N35" s="108"/>
+      <c r="F35" s="125"/>
+      <c r="G35" s="126"/>
+      <c r="H35" s="127"/>
+      <c r="I35" s="116"/>
+      <c r="J35" s="117"/>
+      <c r="K35" s="118"/>
+      <c r="L35" s="107"/>
+      <c r="M35" s="108"/>
+      <c r="N35" s="109"/>
       <c r="O35" s="46" t="str">
         <f>IF(OR( AND(C36=D34,OR(F35&lt;&gt;G35, I35&lt;&gt;J35,L35&lt;&gt;M35)),  AND(D34=E36,OR(G35&lt;&gt;H35,J35&lt;&gt;K35,M35&lt;&gt;N35)), AND(C36=E36, OR(F35&lt;&gt;H35,I35&lt;&gt;K35,L35&lt;&gt;N35) )), "error: different mark to same abstract","")</f>
         <v/>
@@ -5640,15 +5698,15 @@
       <c r="E36" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="F36" s="127"/>
-      <c r="G36" s="128"/>
-      <c r="H36" s="129"/>
-      <c r="I36" s="118"/>
-      <c r="J36" s="119"/>
-      <c r="K36" s="120"/>
-      <c r="L36" s="109"/>
-      <c r="M36" s="110"/>
-      <c r="N36" s="111"/>
+      <c r="F36" s="128"/>
+      <c r="G36" s="129"/>
+      <c r="H36" s="130"/>
+      <c r="I36" s="119"/>
+      <c r="J36" s="120"/>
+      <c r="K36" s="121"/>
+      <c r="L36" s="110"/>
+      <c r="M36" s="111"/>
+      <c r="N36" s="112"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C37" s="46"/>
@@ -5665,11 +5723,11 @@
       <c r="N37" s="51"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C38" s="130" t="s">
+      <c r="C38" s="103" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="130"/>
-      <c r="E38" s="130"/>
+      <c r="D38" s="103"/>
+      <c r="E38" s="103"/>
       <c r="F38" s="51"/>
       <c r="G38" s="51"/>
       <c r="H38" s="51"/>
@@ -5681,17 +5739,17 @@
       <c r="N38" s="51"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C39" s="64" t="e">
+      <c r="C39" s="64">
         <f>AVERAGE(AVERAGE(F4:F35),AVERAGE(G4:G38),AVERAGE(H4:H38))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D39" s="64" t="e">
+        <v>1</v>
+      </c>
+      <c r="D39" s="64">
         <f>AVERAGE(AVERAGE(I4:I35),AVERAGE(J4:J38),AVERAGE(K4:K38))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E39" s="64" t="e">
+        <v>1</v>
+      </c>
+      <c r="E39" s="64">
         <f>AVERAGE(AVERAGE(L4:L35),AVERAGE(M4:M38),AVERAGE(N4:N38))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="F39" s="51"/>
       <c r="G39" s="51"/>
@@ -7987,25 +8045,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B28:N28"/>
-    <mergeCell ref="B27:N27"/>
-    <mergeCell ref="B26:N26"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="L21:N25"/>
-    <mergeCell ref="I21:K25"/>
-    <mergeCell ref="F21:H25"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="F32:H36"/>
-    <mergeCell ref="L32:N36"/>
-    <mergeCell ref="I32:K36"/>
-    <mergeCell ref="B30:N30"/>
-    <mergeCell ref="B29:N29"/>
     <mergeCell ref="B5:N5"/>
     <mergeCell ref="B19:N19"/>
     <mergeCell ref="B12:N12"/>
@@ -8016,6 +8055,25 @@
     <mergeCell ref="L14:N18"/>
     <mergeCell ref="I14:K18"/>
     <mergeCell ref="F14:H18"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B28:N28"/>
+    <mergeCell ref="B27:N27"/>
+    <mergeCell ref="B26:N26"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="L21:N25"/>
+    <mergeCell ref="I21:K25"/>
+    <mergeCell ref="F21:H25"/>
+    <mergeCell ref="F32:H36"/>
+    <mergeCell ref="L32:N36"/>
+    <mergeCell ref="I32:K36"/>
+    <mergeCell ref="B30:N30"/>
+    <mergeCell ref="B29:N29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8057,9 +8115,9 @@
       <c r="B4" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="40" t="e">
+      <c r="C4" s="40">
         <f>'Ordering of retrievals'!C39</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="D4" s="40"/>
       <c r="E4" s="40"/>
@@ -8072,9 +8130,9 @@
       <c r="B5" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="40" t="e">
+      <c r="C5" s="40">
         <f>'Ordering of retrievals'!D39</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="D5" s="40"/>
       <c r="E5" s="40"/>
@@ -8087,9 +8145,9 @@
       <c r="B6" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="40" t="e">
+      <c r="C6" s="40">
         <f>'Ordering of retrievals'!E39</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="D6" s="40"/>
       <c r="E6" s="40"/>

</xml_diff>